<commit_message>
vault backup: 2025-11-24 15:25:20
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555AE559-B563-4062-9AED-4767A18FDFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC70F7-0D58-4964-8636-7E54D66E6518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21732" yWindow="0" windowWidth="29148" windowHeight="16656" activeTab="1" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
+    <workbookView xWindow="25344" yWindow="0" windowWidth="29148" windowHeight="16656" activeTab="1" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheda V3" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="1089">
   <si>
     <t>Nome</t>
   </si>
@@ -4283,9 +4283,6 @@
     <t>Non sei mai stato veramente convinto della maledizione di Caino, delle Tradizioni, o della religione vampirica in generale.</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Hai un'aura naturale che attira l'attenzione. Sei un leader nato, magnetico, e le persone tendono a seguirti o farsi influenzare</t>
   </si>
   <si>
@@ -4328,7 +4325,50 @@
     <t>Appartamento</t>
   </si>
   <si>
-    <t>Marina Centro</t>
+    <t>La schiatta de’ Montefeltro</t>
+  </si>
+  <si>
+    <t>+1 Dado a schivare, +1 Iniziativa</t>
+  </si>
+  <si>
+    <t>Attiri attenzione. Carisma + Espressione Artistica, Dif. 7</t>
+  </si>
+  <si>
+    <t>Coraggio del bersaglio Dif. 8 o spendere 1 PV</t>
+  </si>
+  <si>
+    <t>Intimidisci: paura, panico. Carisma + Intimidire, Dif. 6/7</t>
+  </si>
+  <si>
+    <t>I Brujah cedono facilmente alla Frenesia: hanno +2 alla difficoltà per controllare rabbia, umiliazioni, provocazioni o frustrazioni. Anche piccoli insulti o ostacoli possono farli scattare, soprattutto se affamati o feriti. Tendono a reagire d’istinto e con violenza quando vengono sfidati o limitati.</t>
+  </si>
+  <si>
+    <t>locali LGBTQ+, backstage, viali turistici.</t>
+  </si>
+  <si>
+    <t>1,78 Mt</t>
+  </si>
+  <si>
+    <t>72 Kg</t>
+  </si>
+  <si>
+    <t>Castani</t>
+  </si>
+  <si>
+    <t>bianca</t>
+  </si>
+  <si>
+    <t>Marrone nocciola</t>
+  </si>
+  <si>
+    <t>Stile: Glamour, teatrale, provocatorio; fuori dal palco è casual ma sempre curato
+Vibe: sguardo morbido ma deciso, sorriso magnetico, movenze sicure da performer veterano</t>
+  </si>
+  <si>
+    <t>Borgo San Giulian</t>
+  </si>
+  <si>
+    <t>Fiat 500L nera, interni glitterati fai-da-te. La definisce “il mio camerino mobile”.</t>
   </si>
 </sst>
 </file>
@@ -5132,7 +5172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5711,6 +5751,21 @@
     <xf numFmtId="0" fontId="61" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="60" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="60" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="60" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5732,38 +5787,29 @@
     <xf numFmtId="164" fontId="60" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="60" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="60" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -20758,45 +20804,45 @@
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A141" s="219" t="s">
+      <c r="A141" s="212" t="s">
         <v>127</v>
       </c>
-      <c r="B141" s="219"/>
-      <c r="C141" s="219"/>
-      <c r="D141" s="219"/>
-      <c r="E141" s="219"/>
-      <c r="F141" s="219"/>
-      <c r="G141" s="219"/>
-      <c r="H141" s="219"/>
-      <c r="I141" s="219"/>
-      <c r="J141" s="219"/>
-      <c r="K141" s="219"/>
+      <c r="B141" s="212"/>
+      <c r="C141" s="212"/>
+      <c r="D141" s="212"/>
+      <c r="E141" s="212"/>
+      <c r="F141" s="212"/>
+      <c r="G141" s="212"/>
+      <c r="H141" s="212"/>
+      <c r="I141" s="212"/>
+      <c r="J141" s="212"/>
+      <c r="K141" s="212"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="219"/>
-      <c r="B142" s="219"/>
-      <c r="C142" s="219"/>
-      <c r="D142" s="219"/>
-      <c r="E142" s="219"/>
-      <c r="F142" s="219"/>
-      <c r="G142" s="219"/>
-      <c r="H142" s="219"/>
-      <c r="I142" s="219"/>
-      <c r="J142" s="219"/>
-      <c r="K142" s="219"/>
+      <c r="A142" s="212"/>
+      <c r="B142" s="212"/>
+      <c r="C142" s="212"/>
+      <c r="D142" s="212"/>
+      <c r="E142" s="212"/>
+      <c r="F142" s="212"/>
+      <c r="G142" s="212"/>
+      <c r="H142" s="212"/>
+      <c r="I142" s="212"/>
+      <c r="J142" s="212"/>
+      <c r="K142" s="212"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A143" s="219"/>
-      <c r="B143" s="219"/>
-      <c r="C143" s="219"/>
-      <c r="D143" s="219"/>
-      <c r="E143" s="219"/>
-      <c r="F143" s="219"/>
-      <c r="G143" s="219"/>
-      <c r="H143" s="219"/>
-      <c r="I143" s="219"/>
-      <c r="J143" s="219"/>
-      <c r="K143" s="219"/>
+      <c r="A143" s="212"/>
+      <c r="B143" s="212"/>
+      <c r="C143" s="212"/>
+      <c r="D143" s="212"/>
+      <c r="E143" s="212"/>
+      <c r="F143" s="212"/>
+      <c r="G143" s="212"/>
+      <c r="H143" s="212"/>
+      <c r="I143" s="212"/>
+      <c r="J143" s="212"/>
+      <c r="K143" s="212"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="90" t="s">
@@ -20804,45 +20850,45 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A146" s="219" t="s">
+      <c r="A146" s="212" t="s">
         <v>124</v>
       </c>
-      <c r="B146" s="219"/>
-      <c r="C146" s="219"/>
-      <c r="D146" s="219"/>
-      <c r="E146" s="219"/>
-      <c r="F146" s="219"/>
-      <c r="G146" s="219"/>
-      <c r="H146" s="219"/>
-      <c r="I146" s="219"/>
-      <c r="J146" s="219"/>
-      <c r="K146" s="219"/>
+      <c r="B146" s="212"/>
+      <c r="C146" s="212"/>
+      <c r="D146" s="212"/>
+      <c r="E146" s="212"/>
+      <c r="F146" s="212"/>
+      <c r="G146" s="212"/>
+      <c r="H146" s="212"/>
+      <c r="I146" s="212"/>
+      <c r="J146" s="212"/>
+      <c r="K146" s="212"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" s="219"/>
-      <c r="B147" s="219"/>
-      <c r="C147" s="219"/>
-      <c r="D147" s="219"/>
-      <c r="E147" s="219"/>
-      <c r="F147" s="219"/>
-      <c r="G147" s="219"/>
-      <c r="H147" s="219"/>
-      <c r="I147" s="219"/>
-      <c r="J147" s="219"/>
-      <c r="K147" s="219"/>
+      <c r="A147" s="212"/>
+      <c r="B147" s="212"/>
+      <c r="C147" s="212"/>
+      <c r="D147" s="212"/>
+      <c r="E147" s="212"/>
+      <c r="F147" s="212"/>
+      <c r="G147" s="212"/>
+      <c r="H147" s="212"/>
+      <c r="I147" s="212"/>
+      <c r="J147" s="212"/>
+      <c r="K147" s="212"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A148" s="219"/>
-      <c r="B148" s="219"/>
-      <c r="C148" s="219"/>
-      <c r="D148" s="219"/>
-      <c r="E148" s="219"/>
-      <c r="F148" s="219"/>
-      <c r="G148" s="219"/>
-      <c r="H148" s="219"/>
-      <c r="I148" s="219"/>
-      <c r="J148" s="219"/>
-      <c r="K148" s="219"/>
+      <c r="A148" s="212"/>
+      <c r="B148" s="212"/>
+      <c r="C148" s="212"/>
+      <c r="D148" s="212"/>
+      <c r="E148" s="212"/>
+      <c r="F148" s="212"/>
+      <c r="G148" s="212"/>
+      <c r="H148" s="212"/>
+      <c r="I148" s="212"/>
+      <c r="J148" s="212"/>
+      <c r="K148" s="212"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F149" s="72" t="s">
@@ -23124,45 +23170,45 @@
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="219" t="s">
+      <c r="A142" s="212" t="s">
         <v>426</v>
       </c>
-      <c r="B142" s="219"/>
-      <c r="C142" s="219"/>
-      <c r="D142" s="219"/>
-      <c r="E142" s="219"/>
-      <c r="F142" s="219"/>
-      <c r="G142" s="219"/>
-      <c r="H142" s="219"/>
-      <c r="I142" s="219"/>
-      <c r="J142" s="219"/>
-      <c r="K142" s="219"/>
+      <c r="B142" s="212"/>
+      <c r="C142" s="212"/>
+      <c r="D142" s="212"/>
+      <c r="E142" s="212"/>
+      <c r="F142" s="212"/>
+      <c r="G142" s="212"/>
+      <c r="H142" s="212"/>
+      <c r="I142" s="212"/>
+      <c r="J142" s="212"/>
+      <c r="K142" s="212"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A143" s="219"/>
-      <c r="B143" s="219"/>
-      <c r="C143" s="219"/>
-      <c r="D143" s="219"/>
-      <c r="E143" s="219"/>
-      <c r="F143" s="219"/>
-      <c r="G143" s="219"/>
-      <c r="H143" s="219"/>
-      <c r="I143" s="219"/>
-      <c r="J143" s="219"/>
-      <c r="K143" s="219"/>
+      <c r="A143" s="212"/>
+      <c r="B143" s="212"/>
+      <c r="C143" s="212"/>
+      <c r="D143" s="212"/>
+      <c r="E143" s="212"/>
+      <c r="F143" s="212"/>
+      <c r="G143" s="212"/>
+      <c r="H143" s="212"/>
+      <c r="I143" s="212"/>
+      <c r="J143" s="212"/>
+      <c r="K143" s="212"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A144" s="219"/>
-      <c r="B144" s="219"/>
-      <c r="C144" s="219"/>
-      <c r="D144" s="219"/>
-      <c r="E144" s="219"/>
-      <c r="F144" s="219"/>
-      <c r="G144" s="219"/>
-      <c r="H144" s="219"/>
-      <c r="I144" s="219"/>
-      <c r="J144" s="219"/>
-      <c r="K144" s="219"/>
+      <c r="A144" s="212"/>
+      <c r="B144" s="212"/>
+      <c r="C144" s="212"/>
+      <c r="D144" s="212"/>
+      <c r="E144" s="212"/>
+      <c r="F144" s="212"/>
+      <c r="G144" s="212"/>
+      <c r="H144" s="212"/>
+      <c r="I144" s="212"/>
+      <c r="J144" s="212"/>
+      <c r="K144" s="212"/>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="90" t="s">
@@ -23170,45 +23216,45 @@
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A147" s="219" t="s">
+      <c r="A147" s="212" t="s">
         <v>427</v>
       </c>
-      <c r="B147" s="219"/>
-      <c r="C147" s="219"/>
-      <c r="D147" s="219"/>
-      <c r="E147" s="219"/>
-      <c r="F147" s="219"/>
-      <c r="G147" s="219"/>
-      <c r="H147" s="219"/>
-      <c r="I147" s="219"/>
-      <c r="J147" s="219"/>
-      <c r="K147" s="219"/>
+      <c r="B147" s="212"/>
+      <c r="C147" s="212"/>
+      <c r="D147" s="212"/>
+      <c r="E147" s="212"/>
+      <c r="F147" s="212"/>
+      <c r="G147" s="212"/>
+      <c r="H147" s="212"/>
+      <c r="I147" s="212"/>
+      <c r="J147" s="212"/>
+      <c r="K147" s="212"/>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A148" s="219"/>
-      <c r="B148" s="219"/>
-      <c r="C148" s="219"/>
-      <c r="D148" s="219"/>
-      <c r="E148" s="219"/>
-      <c r="F148" s="219"/>
-      <c r="G148" s="219"/>
-      <c r="H148" s="219"/>
-      <c r="I148" s="219"/>
-      <c r="J148" s="219"/>
-      <c r="K148" s="219"/>
+      <c r="A148" s="212"/>
+      <c r="B148" s="212"/>
+      <c r="C148" s="212"/>
+      <c r="D148" s="212"/>
+      <c r="E148" s="212"/>
+      <c r="F148" s="212"/>
+      <c r="G148" s="212"/>
+      <c r="H148" s="212"/>
+      <c r="I148" s="212"/>
+      <c r="J148" s="212"/>
+      <c r="K148" s="212"/>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A149" s="219"/>
-      <c r="B149" s="219"/>
-      <c r="C149" s="219"/>
-      <c r="D149" s="219"/>
-      <c r="E149" s="219"/>
-      <c r="F149" s="219"/>
-      <c r="G149" s="219"/>
-      <c r="H149" s="219"/>
-      <c r="I149" s="219"/>
-      <c r="J149" s="219"/>
-      <c r="K149" s="219"/>
+      <c r="A149" s="212"/>
+      <c r="B149" s="212"/>
+      <c r="C149" s="212"/>
+      <c r="D149" s="212"/>
+      <c r="E149" s="212"/>
+      <c r="F149" s="212"/>
+      <c r="G149" s="212"/>
+      <c r="H149" s="212"/>
+      <c r="I149" s="212"/>
+      <c r="J149" s="212"/>
+      <c r="K149" s="212"/>
     </row>
     <row r="150" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F150" s="71" t="s">
@@ -23639,18 +23685,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="221" t="s">
+      <c r="A1" s="223" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="221"/>
-      <c r="H1" s="221"/>
-      <c r="I1" s="221"/>
-      <c r="J1" s="221"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="223"/>
       <c r="K1" s="34"/>
       <c r="L1" s="34"/>
       <c r="M1" s="34"/>
@@ -24067,121 +24113,121 @@
       <c r="A23" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="C23" s="220" t="s">
+      <c r="C23" s="222" t="s">
         <v>230</v>
       </c>
-      <c r="D23" s="220"/>
-      <c r="E23" s="220"/>
-      <c r="F23" s="220"/>
-      <c r="G23" s="220"/>
-      <c r="H23" s="220"/>
-      <c r="I23" s="220"/>
-      <c r="J23" s="220"/>
+      <c r="D23" s="222"/>
+      <c r="E23" s="222"/>
+      <c r="F23" s="222"/>
+      <c r="G23" s="222"/>
+      <c r="H23" s="222"/>
+      <c r="I23" s="222"/>
+      <c r="J23" s="222"/>
     </row>
     <row r="24" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="220" t="s">
+      <c r="C24" s="222" t="s">
         <v>223</v>
       </c>
-      <c r="D24" s="220"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
-      <c r="H24" s="220"/>
-      <c r="I24" s="220"/>
-      <c r="J24" s="220"/>
+      <c r="D24" s="222"/>
+      <c r="E24" s="222"/>
+      <c r="F24" s="222"/>
+      <c r="G24" s="222"/>
+      <c r="H24" s="222"/>
+      <c r="I24" s="222"/>
+      <c r="J24" s="222"/>
     </row>
     <row r="25" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C25" s="220" t="s">
+      <c r="C25" s="222" t="s">
         <v>224</v>
       </c>
-      <c r="D25" s="220"/>
-      <c r="E25" s="220"/>
-      <c r="F25" s="220"/>
-      <c r="G25" s="220"/>
-      <c r="H25" s="220"/>
-      <c r="I25" s="220"/>
-      <c r="J25" s="220"/>
+      <c r="D25" s="222"/>
+      <c r="E25" s="222"/>
+      <c r="F25" s="222"/>
+      <c r="G25" s="222"/>
+      <c r="H25" s="222"/>
+      <c r="I25" s="222"/>
+      <c r="J25" s="222"/>
     </row>
     <row r="26" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C26" s="220" t="s">
+      <c r="C26" s="222" t="s">
         <v>225</v>
       </c>
-      <c r="D26" s="220"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="220"/>
-      <c r="H26" s="220"/>
-      <c r="I26" s="220"/>
-      <c r="J26" s="220"/>
+      <c r="D26" s="222"/>
+      <c r="E26" s="222"/>
+      <c r="F26" s="222"/>
+      <c r="G26" s="222"/>
+      <c r="H26" s="222"/>
+      <c r="I26" s="222"/>
+      <c r="J26" s="222"/>
     </row>
     <row r="27" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="C27" s="220" t="s">
+      <c r="C27" s="222" t="s">
         <v>226</v>
       </c>
-      <c r="D27" s="220"/>
-      <c r="E27" s="220"/>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="220"/>
-      <c r="J27" s="220"/>
+      <c r="D27" s="222"/>
+      <c r="E27" s="222"/>
+      <c r="F27" s="222"/>
+      <c r="G27" s="222"/>
+      <c r="H27" s="222"/>
+      <c r="I27" s="222"/>
+      <c r="J27" s="222"/>
     </row>
     <row r="28" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="C28" s="220" t="s">
+      <c r="C28" s="222" t="s">
         <v>227</v>
       </c>
-      <c r="D28" s="220"/>
-      <c r="E28" s="220"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="220"/>
-      <c r="H28" s="220"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="220"/>
+      <c r="D28" s="222"/>
+      <c r="E28" s="222"/>
+      <c r="F28" s="222"/>
+      <c r="G28" s="222"/>
+      <c r="H28" s="222"/>
+      <c r="I28" s="222"/>
+      <c r="J28" s="222"/>
     </row>
     <row r="29" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="C29" s="220" t="s">
+      <c r="C29" s="222" t="s">
         <v>234</v>
       </c>
-      <c r="D29" s="220"/>
-      <c r="E29" s="220"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
+      <c r="D29" s="222"/>
+      <c r="E29" s="222"/>
+      <c r="F29" s="222"/>
+      <c r="G29" s="222"/>
+      <c r="H29" s="222"/>
+      <c r="I29" s="222"/>
+      <c r="J29" s="222"/>
     </row>
     <row r="30" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="C30" s="220" t="s">
+      <c r="C30" s="222" t="s">
         <v>233</v>
       </c>
-      <c r="D30" s="220"/>
-      <c r="E30" s="220"/>
-      <c r="F30" s="220"/>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
-      <c r="I30" s="220"/>
-      <c r="J30" s="220"/>
+      <c r="D30" s="222"/>
+      <c r="E30" s="222"/>
+      <c r="F30" s="222"/>
+      <c r="G30" s="222"/>
+      <c r="H30" s="222"/>
+      <c r="I30" s="222"/>
+      <c r="J30" s="222"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31"/>
@@ -25979,8 +26025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB020AF3-E2AF-4B08-9CF1-A8BB16CCBDFC}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -26003,7 +26049,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="H1" s="151" t="s">
         <v>173</v>
@@ -26013,7 +26059,7 @@
       </c>
       <c r="J1" s="100"/>
       <c r="K1" s="61"/>
-      <c r="L1" s="222" t="s">
+      <c r="L1" s="210" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -26040,7 +26086,7 @@
         <v>343</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>125</v>
+        <v>1074</v>
       </c>
       <c r="H4" s="55" t="s">
         <v>1048</v>
@@ -26053,7 +26099,7 @@
       <c r="B5" s="152" t="s">
         <v>502</v>
       </c>
-      <c r="E5" s="223" t="s">
+      <c r="E5" s="211" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="139" t="s">
@@ -26494,7 +26540,9 @@
       <c r="B30" s="54">
         <v>1</v>
       </c>
-      <c r="C30" s="80"/>
+      <c r="C30" s="80" t="s">
+        <v>1075</v>
+      </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
@@ -26539,7 +26587,9 @@
       <c r="B32" s="54">
         <v>1</v>
       </c>
-      <c r="C32" s="80"/>
+      <c r="C32" s="80" t="s">
+        <v>1076</v>
+      </c>
       <c r="H32" s="63" t="s">
         <v>70</v>
       </c>
@@ -26555,7 +26605,9 @@
       <c r="B33" s="54">
         <v>2</v>
       </c>
-      <c r="C33" s="80"/>
+      <c r="C33" s="80" t="s">
+        <v>1078</v>
+      </c>
       <c r="H33" s="63" t="s">
         <v>66</v>
       </c>
@@ -26569,12 +26621,14 @@
       <c r="L33" s="54"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="61"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
+      <c r="A34" s="224"/>
+      <c r="B34" s="224"/>
+      <c r="C34" s="225" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D34" s="224"/>
+      <c r="E34" s="224"/>
+      <c r="F34" s="224"/>
       <c r="H34" s="63" t="s">
         <v>20</v>
       </c>
@@ -26863,7 +26917,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="80" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -26874,7 +26928,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="80" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -26885,7 +26939,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="80" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E54" s="155"/>
     </row>
@@ -26897,7 +26951,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="80" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E55" s="155"/>
     </row>
@@ -26909,7 +26963,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="80" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E56" s="155"/>
     </row>
@@ -26921,62 +26975,34 @@
         <v>2</v>
       </c>
       <c r="D57" s="80" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E57" s="155"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E58" s="155"/>
-      <c r="F58" s="224"/>
-      <c r="G58" s="224"/>
-      <c r="H58" s="224"/>
-      <c r="I58" s="224"/>
-      <c r="J58" s="224"/>
-      <c r="K58" s="225"/>
-      <c r="L58" s="224"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="155"/>
       <c r="C59" s="54"/>
       <c r="D59" s="80"/>
       <c r="E59" s="155"/>
-      <c r="F59" s="224"/>
-      <c r="G59" s="224"/>
-      <c r="H59" s="224"/>
-      <c r="I59" s="224"/>
-      <c r="J59" s="224"/>
-      <c r="K59" s="225"/>
-      <c r="L59" s="224"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="155"/>
       <c r="C60" s="54"/>
       <c r="D60" s="80"/>
       <c r="E60" s="155"/>
-      <c r="F60" s="224"/>
-      <c r="G60" s="224"/>
-      <c r="H60" s="224"/>
-      <c r="I60" s="224"/>
-      <c r="J60" s="224"/>
-      <c r="K60" s="225"/>
-      <c r="L60" s="224"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="155"/>
       <c r="C61" s="54"/>
       <c r="D61" s="80"/>
       <c r="E61" s="155"/>
-      <c r="F61" s="224"/>
-      <c r="G61" s="224"/>
-      <c r="H61" s="224"/>
-      <c r="I61" s="224"/>
-      <c r="J61" s="224"/>
-      <c r="K61" s="225"/>
-      <c r="L61" s="224"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="55" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C62" s="75" t="s">
         <v>203</v>
@@ -26989,138 +27015,68 @@
       <c r="A63" s="155" t="s">
         <v>1056</v>
       </c>
-      <c r="C63" s="225">
+      <c r="C63" s="54">
         <v>5</v>
       </c>
-      <c r="D63" s="226" t="s">
-        <v>1061</v>
+      <c r="D63" s="80" t="s">
+        <v>1060</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D64" s="226" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E64" s="224"/>
-      <c r="F64" s="224"/>
-      <c r="G64" s="224"/>
-      <c r="H64" s="224"/>
-      <c r="I64" s="224"/>
-      <c r="J64" s="224"/>
-      <c r="K64" s="225"/>
-      <c r="L64" s="224"/>
+      <c r="D64" s="80" t="s">
+        <v>1063</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="155" t="s">
         <v>1054</v>
       </c>
-      <c r="C65" s="225">
+      <c r="C65" s="54">
         <v>1</v>
       </c>
-      <c r="D65" s="226" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E65" s="224"/>
-      <c r="F65" s="224"/>
-      <c r="G65" s="224"/>
-      <c r="H65" s="224"/>
-      <c r="I65" s="224"/>
-      <c r="J65" s="224"/>
-      <c r="K65" s="225"/>
-      <c r="L65" s="224"/>
+      <c r="D65" s="80" t="s">
+        <v>1061</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="155" t="s">
         <v>1057</v>
       </c>
-      <c r="C66" s="225">
+      <c r="C66" s="54">
         <v>-3</v>
       </c>
-      <c r="D66" s="226" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E66" s="224"/>
-      <c r="F66" s="224"/>
-      <c r="G66" s="224"/>
-      <c r="H66" s="224"/>
-      <c r="I66" s="224"/>
-      <c r="J66" s="224"/>
-      <c r="K66" s="225"/>
-      <c r="L66" s="224"/>
+      <c r="D66" s="80" t="s">
+        <v>1064</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="155" t="s">
         <v>1055</v>
       </c>
-      <c r="C67" s="225">
+      <c r="C67" s="54">
         <v>-2</v>
       </c>
-      <c r="D67" s="226" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E67" s="224"/>
-      <c r="F67" s="224"/>
-      <c r="G67" s="224"/>
-      <c r="H67" s="224"/>
-      <c r="I67" s="224"/>
-      <c r="J67" s="224"/>
-      <c r="K67" s="225"/>
-      <c r="L67" s="224"/>
+      <c r="D67" s="80" t="s">
+        <v>1065</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="155" t="s">
         <v>1058</v>
       </c>
-      <c r="C68" s="225">
+      <c r="C68" s="54">
         <v>-1</v>
       </c>
-      <c r="D68" s="226" t="s">
+      <c r="D68" s="80" t="s">
         <v>1059</v>
       </c>
-      <c r="E68" s="224"/>
-      <c r="F68" s="224"/>
-      <c r="G68" s="224"/>
-      <c r="H68" s="224"/>
-      <c r="I68" s="224"/>
-      <c r="J68" s="224"/>
-      <c r="K68" s="225"/>
-      <c r="L68" s="224"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E69" s="224"/>
-      <c r="F69" s="224"/>
-      <c r="G69" s="224"/>
-      <c r="H69" s="224"/>
-      <c r="I69" s="224"/>
-      <c r="J69" s="224"/>
-      <c r="K69" s="225"/>
-      <c r="L69" s="224"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E70" s="224"/>
-      <c r="F70" s="224"/>
-      <c r="G70" s="224"/>
-      <c r="H70" s="224"/>
-      <c r="I70" s="224"/>
-      <c r="J70" s="224"/>
-      <c r="K70" s="225"/>
-      <c r="L70" s="224"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E71" s="224"/>
-      <c r="F71" s="224"/>
-      <c r="G71" s="224"/>
-      <c r="H71" s="224"/>
-      <c r="I71" s="224"/>
-      <c r="J71" s="224"/>
-      <c r="K71" s="225"/>
-      <c r="L71" s="224"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="57" t="s">
         <v>105</v>
       </c>
       <c r="C73" s="100" t="s">
-        <v>421</v>
+        <v>1080</v>
       </c>
       <c r="D73" s="61"/>
       <c r="E73" s="61"/>
@@ -27136,7 +27092,9 @@
       <c r="A74" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="63"/>
+      <c r="C74" s="63" t="s">
+        <v>1088</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="57" t="s">
@@ -27181,11 +27139,11 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="82" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B79" s="82"/>
       <c r="C79" s="82" t="s">
-        <v>1075</v>
+        <v>1087</v>
       </c>
       <c r="D79" s="66"/>
       <c r="E79" s="66"/>
@@ -27239,11 +27197,14 @@
       <c r="A84" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="C84" s="57">
-        <v>41</v>
+      <c r="C84" s="228">
+        <v>29</v>
       </c>
       <c r="E84" s="80" t="s">
         <v>118</v>
+      </c>
+      <c r="G84" s="228" t="s">
+        <v>1084</v>
       </c>
       <c r="I84" s="57" t="s">
         <v>0</v>
@@ -27257,14 +27218,16 @@
         <v>112</v>
       </c>
       <c r="B85" s="66"/>
-      <c r="C85" s="66">
-        <v>41</v>
+      <c r="C85" s="227">
+        <v>29</v>
       </c>
       <c r="E85" s="82" t="s">
         <v>119</v>
       </c>
       <c r="F85" s="66"/>
-      <c r="G85" s="66"/>
+      <c r="G85" s="227" t="s">
+        <v>392</v>
+      </c>
       <c r="I85" s="66"/>
       <c r="J85" s="66"/>
       <c r="K85" s="66"/>
@@ -27274,8 +27237,14 @@
       <c r="A86" s="80" t="s">
         <v>114</v>
       </c>
+      <c r="C86" s="228">
+        <v>1998</v>
+      </c>
       <c r="E86" s="80" t="s">
         <v>120</v>
+      </c>
+      <c r="G86" s="228" t="s">
+        <v>1081</v>
       </c>
       <c r="I86" s="85"/>
       <c r="J86" s="85"/>
@@ -27287,12 +27256,16 @@
         <v>115</v>
       </c>
       <c r="B87" s="66"/>
-      <c r="C87" s="66"/>
+      <c r="C87" s="229">
+        <v>45943</v>
+      </c>
       <c r="E87" s="82" t="s">
         <v>121</v>
       </c>
       <c r="F87" s="66"/>
-      <c r="G87" s="66"/>
+      <c r="G87" s="227" t="s">
+        <v>1082</v>
+      </c>
       <c r="I87" s="66"/>
       <c r="J87" s="66"/>
       <c r="K87" s="66"/>
@@ -27302,8 +27275,14 @@
       <c r="A88" s="80" t="s">
         <v>116</v>
       </c>
+      <c r="C88" s="228" t="s">
+        <v>1083</v>
+      </c>
       <c r="E88" s="80" t="s">
         <v>122</v>
+      </c>
+      <c r="G88" s="228" t="s">
+        <v>394</v>
       </c>
       <c r="K88" s="57"/>
       <c r="L88" s="54"/>
@@ -27313,10 +27292,12 @@
         <v>117</v>
       </c>
       <c r="B89" s="66"/>
-      <c r="C89" s="66"/>
+      <c r="C89" s="227" t="s">
+        <v>1085</v>
+      </c>
       <c r="E89" s="82"/>
       <c r="F89" s="66"/>
-      <c r="G89" s="66"/>
+      <c r="G89" s="227"/>
       <c r="I89" s="66"/>
       <c r="J89" s="66"/>
       <c r="K89" s="66"/>
@@ -27334,62 +27315,62 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="227" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B93" s="227"/>
-      <c r="C93" s="227"/>
-      <c r="D93" s="227"/>
-      <c r="E93" s="227"/>
-      <c r="F93" s="227"/>
-      <c r="G93" s="227"/>
-      <c r="H93" s="227"/>
-      <c r="I93" s="227"/>
-      <c r="J93" s="227"/>
-      <c r="K93" s="227"/>
-      <c r="L93" s="227"/>
+      <c r="A93" s="226" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B93" s="226"/>
+      <c r="C93" s="226"/>
+      <c r="D93" s="226"/>
+      <c r="E93" s="226"/>
+      <c r="F93" s="226"/>
+      <c r="G93" s="226"/>
+      <c r="H93" s="226"/>
+      <c r="I93" s="226"/>
+      <c r="J93" s="226"/>
+      <c r="K93" s="226"/>
+      <c r="L93" s="226"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="227"/>
-      <c r="B94" s="227"/>
-      <c r="C94" s="227"/>
-      <c r="D94" s="227"/>
-      <c r="E94" s="227"/>
-      <c r="F94" s="227"/>
-      <c r="G94" s="227"/>
-      <c r="H94" s="227"/>
-      <c r="I94" s="227"/>
-      <c r="J94" s="227"/>
-      <c r="K94" s="227"/>
-      <c r="L94" s="227"/>
+      <c r="A94" s="226"/>
+      <c r="B94" s="226"/>
+      <c r="C94" s="226"/>
+      <c r="D94" s="226"/>
+      <c r="E94" s="226"/>
+      <c r="F94" s="226"/>
+      <c r="G94" s="226"/>
+      <c r="H94" s="226"/>
+      <c r="I94" s="226"/>
+      <c r="J94" s="226"/>
+      <c r="K94" s="226"/>
+      <c r="L94" s="226"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="227"/>
-      <c r="B95" s="227"/>
-      <c r="C95" s="227"/>
-      <c r="D95" s="227"/>
-      <c r="E95" s="227"/>
-      <c r="F95" s="227"/>
-      <c r="G95" s="227"/>
-      <c r="H95" s="227"/>
-      <c r="I95" s="227"/>
-      <c r="J95" s="227"/>
-      <c r="K95" s="227"/>
-      <c r="L95" s="227"/>
+      <c r="A95" s="226"/>
+      <c r="B95" s="226"/>
+      <c r="C95" s="226"/>
+      <c r="D95" s="226"/>
+      <c r="E95" s="226"/>
+      <c r="F95" s="226"/>
+      <c r="G95" s="226"/>
+      <c r="H95" s="226"/>
+      <c r="I95" s="226"/>
+      <c r="J95" s="226"/>
+      <c r="K95" s="226"/>
+      <c r="L95" s="226"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="227"/>
-      <c r="B96" s="227"/>
-      <c r="C96" s="227"/>
-      <c r="D96" s="227"/>
-      <c r="E96" s="227"/>
-      <c r="F96" s="227"/>
-      <c r="G96" s="227"/>
-      <c r="H96" s="227"/>
-      <c r="I96" s="227"/>
-      <c r="J96" s="227"/>
-      <c r="K96" s="227"/>
-      <c r="L96" s="227"/>
+      <c r="A96" s="226"/>
+      <c r="B96" s="226"/>
+      <c r="C96" s="226"/>
+      <c r="D96" s="226"/>
+      <c r="E96" s="226"/>
+      <c r="F96" s="226"/>
+      <c r="G96" s="226"/>
+      <c r="H96" s="226"/>
+      <c r="I96" s="226"/>
+      <c r="J96" s="226"/>
+      <c r="K96" s="226"/>
+      <c r="L96" s="226"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="90" t="s">
@@ -27397,48 +27378,48 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="227" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B98" s="227"/>
-      <c r="C98" s="227"/>
-      <c r="D98" s="227"/>
-      <c r="E98" s="227"/>
-      <c r="F98" s="227"/>
-      <c r="G98" s="227"/>
-      <c r="H98" s="227"/>
-      <c r="I98" s="227"/>
-      <c r="J98" s="227"/>
-      <c r="K98" s="227"/>
-      <c r="L98" s="227"/>
+      <c r="A98" s="226" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B98" s="226"/>
+      <c r="C98" s="226"/>
+      <c r="D98" s="226"/>
+      <c r="E98" s="226"/>
+      <c r="F98" s="226"/>
+      <c r="G98" s="226"/>
+      <c r="H98" s="226"/>
+      <c r="I98" s="226"/>
+      <c r="J98" s="226"/>
+      <c r="K98" s="226"/>
+      <c r="L98" s="226"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="227"/>
-      <c r="B99" s="227"/>
-      <c r="C99" s="227"/>
-      <c r="D99" s="227"/>
-      <c r="E99" s="227"/>
-      <c r="F99" s="227"/>
-      <c r="G99" s="227"/>
-      <c r="H99" s="227"/>
-      <c r="I99" s="227"/>
-      <c r="J99" s="227"/>
-      <c r="K99" s="227"/>
-      <c r="L99" s="227"/>
+      <c r="A99" s="226"/>
+      <c r="B99" s="226"/>
+      <c r="C99" s="226"/>
+      <c r="D99" s="226"/>
+      <c r="E99" s="226"/>
+      <c r="F99" s="226"/>
+      <c r="G99" s="226"/>
+      <c r="H99" s="226"/>
+      <c r="I99" s="226"/>
+      <c r="J99" s="226"/>
+      <c r="K99" s="226"/>
+      <c r="L99" s="226"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="227"/>
-      <c r="B100" s="227"/>
-      <c r="C100" s="227"/>
-      <c r="D100" s="227"/>
-      <c r="E100" s="227"/>
-      <c r="F100" s="227"/>
-      <c r="G100" s="227"/>
-      <c r="H100" s="227"/>
-      <c r="I100" s="227"/>
-      <c r="J100" s="227"/>
-      <c r="K100" s="227"/>
-      <c r="L100" s="227"/>
+      <c r="A100" s="226"/>
+      <c r="B100" s="226"/>
+      <c r="C100" s="226"/>
+      <c r="D100" s="226"/>
+      <c r="E100" s="226"/>
+      <c r="F100" s="226"/>
+      <c r="G100" s="226"/>
+      <c r="H100" s="226"/>
+      <c r="I100" s="226"/>
+      <c r="J100" s="226"/>
+      <c r="K100" s="226"/>
+      <c r="L100" s="226"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
@@ -30032,45 +30013,45 @@
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A141" s="219" t="s">
+      <c r="A141" s="212" t="s">
         <v>127</v>
       </c>
-      <c r="B141" s="219"/>
-      <c r="C141" s="219"/>
-      <c r="D141" s="219"/>
-      <c r="E141" s="219"/>
-      <c r="F141" s="219"/>
-      <c r="G141" s="219"/>
-      <c r="H141" s="219"/>
-      <c r="I141" s="219"/>
-      <c r="J141" s="219"/>
-      <c r="K141" s="219"/>
+      <c r="B141" s="212"/>
+      <c r="C141" s="212"/>
+      <c r="D141" s="212"/>
+      <c r="E141" s="212"/>
+      <c r="F141" s="212"/>
+      <c r="G141" s="212"/>
+      <c r="H141" s="212"/>
+      <c r="I141" s="212"/>
+      <c r="J141" s="212"/>
+      <c r="K141" s="212"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="219"/>
-      <c r="B142" s="219"/>
-      <c r="C142" s="219"/>
-      <c r="D142" s="219"/>
-      <c r="E142" s="219"/>
-      <c r="F142" s="219"/>
-      <c r="G142" s="219"/>
-      <c r="H142" s="219"/>
-      <c r="I142" s="219"/>
-      <c r="J142" s="219"/>
-      <c r="K142" s="219"/>
+      <c r="A142" s="212"/>
+      <c r="B142" s="212"/>
+      <c r="C142" s="212"/>
+      <c r="D142" s="212"/>
+      <c r="E142" s="212"/>
+      <c r="F142" s="212"/>
+      <c r="G142" s="212"/>
+      <c r="H142" s="212"/>
+      <c r="I142" s="212"/>
+      <c r="J142" s="212"/>
+      <c r="K142" s="212"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A143" s="219"/>
-      <c r="B143" s="219"/>
-      <c r="C143" s="219"/>
-      <c r="D143" s="219"/>
-      <c r="E143" s="219"/>
-      <c r="F143" s="219"/>
-      <c r="G143" s="219"/>
-      <c r="H143" s="219"/>
-      <c r="I143" s="219"/>
-      <c r="J143" s="219"/>
-      <c r="K143" s="219"/>
+      <c r="A143" s="212"/>
+      <c r="B143" s="212"/>
+      <c r="C143" s="212"/>
+      <c r="D143" s="212"/>
+      <c r="E143" s="212"/>
+      <c r="F143" s="212"/>
+      <c r="G143" s="212"/>
+      <c r="H143" s="212"/>
+      <c r="I143" s="212"/>
+      <c r="J143" s="212"/>
+      <c r="K143" s="212"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="90" t="s">
@@ -30078,45 +30059,45 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A146" s="219" t="s">
+      <c r="A146" s="212" t="s">
         <v>124</v>
       </c>
-      <c r="B146" s="219"/>
-      <c r="C146" s="219"/>
-      <c r="D146" s="219"/>
-      <c r="E146" s="219"/>
-      <c r="F146" s="219"/>
-      <c r="G146" s="219"/>
-      <c r="H146" s="219"/>
-      <c r="I146" s="219"/>
-      <c r="J146" s="219"/>
-      <c r="K146" s="219"/>
+      <c r="B146" s="212"/>
+      <c r="C146" s="212"/>
+      <c r="D146" s="212"/>
+      <c r="E146" s="212"/>
+      <c r="F146" s="212"/>
+      <c r="G146" s="212"/>
+      <c r="H146" s="212"/>
+      <c r="I146" s="212"/>
+      <c r="J146" s="212"/>
+      <c r="K146" s="212"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" s="219"/>
-      <c r="B147" s="219"/>
-      <c r="C147" s="219"/>
-      <c r="D147" s="219"/>
-      <c r="E147" s="219"/>
-      <c r="F147" s="219"/>
-      <c r="G147" s="219"/>
-      <c r="H147" s="219"/>
-      <c r="I147" s="219"/>
-      <c r="J147" s="219"/>
-      <c r="K147" s="219"/>
+      <c r="A147" s="212"/>
+      <c r="B147" s="212"/>
+      <c r="C147" s="212"/>
+      <c r="D147" s="212"/>
+      <c r="E147" s="212"/>
+      <c r="F147" s="212"/>
+      <c r="G147" s="212"/>
+      <c r="H147" s="212"/>
+      <c r="I147" s="212"/>
+      <c r="J147" s="212"/>
+      <c r="K147" s="212"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A148" s="219"/>
-      <c r="B148" s="219"/>
-      <c r="C148" s="219"/>
-      <c r="D148" s="219"/>
-      <c r="E148" s="219"/>
-      <c r="F148" s="219"/>
-      <c r="G148" s="219"/>
-      <c r="H148" s="219"/>
-      <c r="I148" s="219"/>
-      <c r="J148" s="219"/>
-      <c r="K148" s="219"/>
+      <c r="A148" s="212"/>
+      <c r="B148" s="212"/>
+      <c r="C148" s="212"/>
+      <c r="D148" s="212"/>
+      <c r="E148" s="212"/>
+      <c r="F148" s="212"/>
+      <c r="G148" s="212"/>
+      <c r="H148" s="212"/>
+      <c r="I148" s="212"/>
+      <c r="J148" s="212"/>
+      <c r="K148" s="212"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F149" s="72" t="s">
@@ -30439,42 +30420,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="219" t="s">
         <v>1028</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="214"/>
-      <c r="I1" s="214"/>
-      <c r="J1" s="215">
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="219"/>
+      <c r="H1" s="219"/>
+      <c r="I1" s="219"/>
+      <c r="J1" s="220">
         <f>C7</f>
         <v>0.8125</v>
       </c>
-      <c r="K1" s="216"/>
-      <c r="L1" s="217">
+      <c r="K1" s="221"/>
+      <c r="L1" s="213">
         <f>C8</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M1" s="216"/>
-      <c r="N1" s="217">
+      <c r="M1" s="221"/>
+      <c r="N1" s="213">
         <f>C9</f>
         <v>0.85416666666666674</v>
       </c>
-      <c r="O1" s="216"/>
-      <c r="P1" s="217">
+      <c r="O1" s="221"/>
+      <c r="P1" s="213">
         <f>C10</f>
         <v>0.87500000000000011</v>
       </c>
-      <c r="Q1" s="216"/>
-      <c r="R1" s="217">
+      <c r="Q1" s="221"/>
+      <c r="R1" s="213">
         <f>C11</f>
         <v>0.89583333333333348</v>
       </c>
-      <c r="S1" s="218"/>
+      <c r="S1" s="214"/>
     </row>
     <row r="2" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="J2" s="197"/>
@@ -30554,31 +30535,31 @@
       <c r="F6" s="7" t="s">
         <v>1027</v>
       </c>
-      <c r="J6" s="210">
+      <c r="J6" s="215">
         <f>C12</f>
         <v>0.91666666666666685</v>
       </c>
-      <c r="K6" s="211"/>
-      <c r="L6" s="212">
+      <c r="K6" s="216"/>
+      <c r="L6" s="217">
         <f>C13</f>
         <v>0.93750000000000022</v>
       </c>
-      <c r="M6" s="211"/>
-      <c r="N6" s="212">
+      <c r="M6" s="216"/>
+      <c r="N6" s="217">
         <f>C14</f>
         <v>0.95833333333333359</v>
       </c>
-      <c r="O6" s="211"/>
-      <c r="P6" s="212">
+      <c r="O6" s="216"/>
+      <c r="P6" s="217">
         <f>C15</f>
         <v>0.97916666666666696</v>
       </c>
-      <c r="Q6" s="211"/>
-      <c r="R6" s="212">
+      <c r="Q6" s="216"/>
+      <c r="R6" s="217">
         <f>C16</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S6" s="213"/>
+      <c r="S6" s="218"/>
     </row>
     <row r="7" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
@@ -30716,31 +30697,31 @@
       <c r="F11" s="7" t="s">
         <v>1022</v>
       </c>
-      <c r="J11" s="210">
+      <c r="J11" s="215">
         <f>C17</f>
         <v>1.0208333333333335</v>
       </c>
-      <c r="K11" s="211"/>
-      <c r="L11" s="212">
+      <c r="K11" s="216"/>
+      <c r="L11" s="217">
         <f>C18</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="M11" s="211"/>
-      <c r="N11" s="212">
+      <c r="M11" s="216"/>
+      <c r="N11" s="217">
         <f>C19</f>
         <v>1.0625</v>
       </c>
-      <c r="O11" s="211"/>
-      <c r="P11" s="212">
+      <c r="O11" s="216"/>
+      <c r="P11" s="217">
         <f>C20</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="Q11" s="211"/>
-      <c r="R11" s="212">
+      <c r="Q11" s="216"/>
+      <c r="R11" s="217">
         <f>C21</f>
         <v>1.1041666666666665</v>
       </c>
-      <c r="S11" s="213"/>
+      <c r="S11" s="218"/>
     </row>
     <row r="12" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B12" s="194">
@@ -30870,31 +30851,31 @@
       <c r="E16" s="6" t="s">
         <v>1012</v>
       </c>
-      <c r="J16" s="210">
+      <c r="J16" s="215">
         <f>C22</f>
         <v>1.1249999999999998</v>
       </c>
-      <c r="K16" s="211"/>
-      <c r="L16" s="212">
+      <c r="K16" s="216"/>
+      <c r="L16" s="217">
         <f>C23</f>
         <v>1.145833333333333</v>
       </c>
-      <c r="M16" s="211"/>
-      <c r="N16" s="212">
+      <c r="M16" s="216"/>
+      <c r="N16" s="217">
         <f>C24</f>
         <v>1.1666666666666663</v>
       </c>
-      <c r="O16" s="211"/>
-      <c r="P16" s="212">
+      <c r="O16" s="216"/>
+      <c r="P16" s="217">
         <f>C25</f>
         <v>1.1874999999999996</v>
       </c>
-      <c r="Q16" s="211"/>
-      <c r="R16" s="212">
+      <c r="Q16" s="216"/>
+      <c r="R16" s="217">
         <f>C26</f>
         <v>1.2083333333333328</v>
       </c>
-      <c r="S16" s="213"/>
+      <c r="S16" s="218"/>
     </row>
     <row r="17" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B17" s="194">
@@ -31030,31 +31011,31 @@
       <c r="F21" s="7" t="s">
         <v>1024</v>
       </c>
-      <c r="J21" s="210">
+      <c r="J21" s="215">
         <f>C27</f>
         <v>1.2291666666666661</v>
       </c>
-      <c r="K21" s="211"/>
-      <c r="L21" s="212">
+      <c r="K21" s="216"/>
+      <c r="L21" s="217">
         <f>C28</f>
         <v>1.2499999999999993</v>
       </c>
-      <c r="M21" s="211"/>
-      <c r="N21" s="212">
+      <c r="M21" s="216"/>
+      <c r="N21" s="217">
         <f>C29</f>
         <v>1.2708333333333326</v>
       </c>
-      <c r="O21" s="211"/>
-      <c r="P21" s="212">
+      <c r="O21" s="216"/>
+      <c r="P21" s="217">
         <f>C30</f>
         <v>1.2916666666666659</v>
       </c>
-      <c r="Q21" s="211"/>
-      <c r="R21" s="212">
+      <c r="Q21" s="216"/>
+      <c r="R21" s="217">
         <f>C31</f>
         <v>1.3124999999999991</v>
       </c>
-      <c r="S21" s="213"/>
+      <c r="S21" s="218"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B22" s="194">
@@ -31289,18 +31270,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
@@ -31310,11 +31284,18 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31386,7 +31367,7 @@
       <c r="C3" s="47"/>
       <c r="D3" s="44">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E3" s="44">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
@@ -31394,35 +31375,35 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" s="44"/>
     </row>
@@ -31485,7 +31466,7 @@
       </c>
       <c r="M5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -31495,11 +31476,11 @@
       <c r="C6" s="47"/>
       <c r="D6" s="46">
         <f t="shared" ref="D6:D13" ca="1" si="2">IF(D$3&gt;=$B6,1,0)+IF(D$3=1,-1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="46">
         <f t="shared" ref="E6:M13" ca="1" si="3">IF(E$3&gt;=$B6,1,0)+D6+IF(E$3=1,-1,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31531,7 +31512,7 @@
       </c>
       <c r="M6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -31541,15 +31522,15 @@
       <c r="C7" s="47"/>
       <c r="D7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31577,7 +31558,7 @@
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -31587,15 +31568,15 @@
       <c r="C8" s="47"/>
       <c r="D8" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31623,7 +31604,7 @@
       </c>
       <c r="M8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -31633,15 +31614,15 @@
       <c r="C9" s="47"/>
       <c r="D9" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31649,27 +31630,27 @@
       </c>
       <c r="H9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -31679,43 +31660,43 @@
       <c r="C10" s="47"/>
       <c r="D10" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -31741,11 +31722,11 @@
       </c>
       <c r="H11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31753,15 +31734,15 @@
       </c>
       <c r="K11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -31791,7 +31772,7 @@
       </c>
       <c r="I12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31799,15 +31780,15 @@
       </c>
       <c r="K12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -31837,7 +31818,7 @@
       </c>
       <c r="I13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31853,7 +31834,7 @@
       </c>
       <c r="M13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -31876,7 +31857,7 @@
       </c>
       <c r="G16" s="49" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -31905,7 +31886,7 @@
       <c r="F19" s="46"/>
       <c r="G19" s="50" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(E19+3,D19+3,1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -31918,7 +31899,7 @@
       <c r="F20" s="46"/>
       <c r="G20" s="50" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -31931,7 +31912,7 @@
       <c r="F21" s="46"/>
       <c r="G21" s="50" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(ADDRESS(E21+3,D21+3,1))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -31944,7 +31925,7 @@
       <c r="F22" s="46"/>
       <c r="G22" s="50" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT(ADDRESS(E22+3,D22+3,1))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -31957,7 +31938,7 @@
       <c r="F23" s="46"/>
       <c r="G23" s="50" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-11-24 16:09:35
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC70F7-0D58-4964-8636-7E54D66E6518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F26A1A-223C-47FF-929E-894A9C742AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25344" yWindow="0" windowWidth="29148" windowHeight="16656" activeTab="1" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="1108">
   <si>
     <t>Nome</t>
   </si>
@@ -4355,9 +4355,6 @@
     <t>Castani</t>
   </si>
   <si>
-    <t>bianca</t>
-  </si>
-  <si>
     <t>Marrone nocciola</t>
   </si>
   <si>
@@ -4369,6 +4366,66 @@
   </si>
   <si>
     <t>Fiat 500L nera, interni glitterati fai-da-te. La definisce “il mio camerino mobile”.</t>
+  </si>
+  <si>
+    <t>Stipendio intermittente ma stabile da performer + consulenze per giovani artisti</t>
+  </si>
+  <si>
+    <t>secondo piano di una casa color pastello, con travi a vista e finestre che danno sui murales.</t>
+  </si>
+  <si>
+    <t>Contatti / Amici</t>
+  </si>
+  <si>
+    <t>Contatto</t>
+  </si>
+  <si>
+    <t>Mirko “Due Mic”</t>
+  </si>
+  <si>
+    <t>Conosce tutti i locali LGBTQ+ da Rimini a Riccione.Tipo di aiuto: informazioni, accesso in backstage, favori logistici.</t>
+  </si>
+  <si>
+    <t>Avv. Sonia Belloni</t>
+  </si>
+  <si>
+    <t>Fan della scena drag e tua amica da anni. Tipo di aiuto: consulenza legale, protezione da impresari aggressivi.</t>
+  </si>
+  <si>
+    <t>Dario Fontana</t>
+  </si>
+  <si>
+    <t>Ex Fiamma</t>
+  </si>
+  <si>
+    <t>ex amante artista, emotivamente instabile, ritorna creando caos. Tende a seguirti e filmarti.</t>
+  </si>
+  <si>
+    <t>Gruppo Esordienti</t>
+  </si>
+  <si>
+    <t>3–4 ragazze e ragazzi giovani della scena drag che ti vedono come mentore (“Mama”).</t>
+  </si>
+  <si>
+    <t>Legami di Sangue/Vicoli/Amici</t>
+  </si>
+  <si>
+    <t>Luna (Allieva/Protetta)</t>
+  </si>
+  <si>
+    <t>Sangue</t>
+  </si>
+  <si>
+    <t>Giovane performer emergente, talentuosa ma insicura. Ti vede come mentore, confidente e ancora di salvezza</t>
+  </si>
+  <si>
+    <t>Debolezza di Clan</t>
+  </si>
+  <si>
+    <t>Amica</t>
+  </si>
+  <si>
+    <t>Caucasico</t>
   </si>
 </sst>
 </file>
@@ -5172,7 +5229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5810,6 +5867,18 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -26025,8 +26094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB020AF3-E2AF-4B08-9CF1-A8BB16CCBDFC}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -26983,16 +27052,32 @@
       <c r="E58" s="155"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="155"/>
-      <c r="C59" s="54"/>
-      <c r="D59" s="80"/>
-      <c r="E59" s="155"/>
+      <c r="A59" s="233"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="233"/>
+      <c r="F59" s="66"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="69"/>
+      <c r="L59" s="66"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="155"/>
-      <c r="C60" s="54"/>
-      <c r="D60" s="80"/>
-      <c r="E60" s="155"/>
+      <c r="A60" s="233"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="69"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="233"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="66"/>
+      <c r="I60" s="66"/>
+      <c r="J60" s="66"/>
+      <c r="K60" s="69"/>
+      <c r="L60" s="66"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="155"/>
@@ -27071,103 +27156,153 @@
         <v>1059</v>
       </c>
     </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="66"/>
+      <c r="B70" s="66"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="66"/>
+      <c r="J70" s="66"/>
+      <c r="K70" s="69"/>
+      <c r="L70" s="66"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="66"/>
+      <c r="B71" s="66"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="66"/>
+      <c r="E71" s="66"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="66"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="69"/>
+      <c r="L71" s="66"/>
+    </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="C73" s="100" t="s">
+      <c r="C73" s="230" t="s">
         <v>1080</v>
       </c>
-      <c r="D73" s="61"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="61"/>
-      <c r="G73" s="61"/>
-      <c r="H73" s="61"/>
-      <c r="I73" s="61"/>
-      <c r="J73" s="61"/>
-      <c r="K73" s="78"/>
-      <c r="L73" s="61"/>
+      <c r="D73" s="224"/>
+      <c r="E73" s="224"/>
+      <c r="F73" s="224"/>
+      <c r="G73" s="224"/>
+      <c r="H73" s="224"/>
+      <c r="I73" s="224"/>
+      <c r="J73" s="224"/>
+      <c r="K73" s="232"/>
+      <c r="L73" s="224"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="63" t="s">
-        <v>1088</v>
-      </c>
+      <c r="C74" s="230" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D74" s="224"/>
+      <c r="E74" s="224"/>
+      <c r="F74" s="224"/>
+      <c r="G74" s="224"/>
+      <c r="H74" s="224"/>
+      <c r="I74" s="224"/>
+      <c r="J74" s="224"/>
+      <c r="K74" s="232"/>
+      <c r="L74" s="224"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="99"/>
-      <c r="D75" s="66"/>
-      <c r="E75" s="66"/>
-      <c r="F75" s="66"/>
-      <c r="G75" s="66"/>
-      <c r="H75" s="66"/>
-      <c r="I75" s="66"/>
-      <c r="J75" s="66"/>
-      <c r="K75" s="69"/>
-      <c r="L75" s="66"/>
+      <c r="C75" s="230" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D75" s="224"/>
+      <c r="E75" s="224"/>
+      <c r="F75" s="224"/>
+      <c r="G75" s="224"/>
+      <c r="H75" s="224"/>
+      <c r="I75" s="224"/>
+      <c r="J75" s="224"/>
+      <c r="K75" s="232"/>
+      <c r="L75" s="224"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="C76" s="99"/>
-      <c r="D76" s="66"/>
-      <c r="E76" s="66"/>
-      <c r="F76" s="66"/>
-      <c r="G76" s="66"/>
-      <c r="H76" s="66"/>
-      <c r="I76" s="66"/>
-      <c r="J76" s="66"/>
-      <c r="K76" s="69"/>
-      <c r="L76" s="66"/>
+      <c r="C76" s="100"/>
+      <c r="D76" s="61"/>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61"/>
+      <c r="G76" s="61"/>
+      <c r="H76" s="61"/>
+      <c r="I76" s="61"/>
+      <c r="J76" s="61"/>
+      <c r="K76" s="78"/>
+      <c r="L76" s="61"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="57" t="s">
+      <c r="A78" s="224" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="57" t="s">
+      <c r="B78" s="224"/>
+      <c r="C78" s="224" t="s">
         <v>109</v>
       </c>
-      <c r="E78" s="57" t="s">
+      <c r="D78" s="224"/>
+      <c r="E78" s="224" t="s">
         <v>61</v>
       </c>
+      <c r="F78" s="224"/>
+      <c r="G78" s="224"/>
+      <c r="H78" s="224"/>
+      <c r="I78" s="224"/>
+      <c r="J78" s="224"/>
+      <c r="K78" s="232"/>
+      <c r="L78" s="224"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="82" t="s">
+      <c r="A79" s="225" t="s">
         <v>1073</v>
       </c>
-      <c r="B79" s="82"/>
-      <c r="C79" s="82" t="s">
-        <v>1087</v>
-      </c>
-      <c r="D79" s="66"/>
-      <c r="E79" s="66"/>
-      <c r="F79" s="66"/>
-      <c r="G79" s="66"/>
-      <c r="H79" s="66"/>
-      <c r="I79" s="66"/>
-      <c r="J79" s="66"/>
-      <c r="K79" s="69"/>
-      <c r="L79" s="66"/>
+      <c r="B79" s="225"/>
+      <c r="C79" s="225" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D79" s="224"/>
+      <c r="E79" s="224" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F79" s="224"/>
+      <c r="G79" s="224"/>
+      <c r="H79" s="224"/>
+      <c r="I79" s="224"/>
+      <c r="J79" s="224"/>
+      <c r="K79" s="232"/>
+      <c r="L79" s="224"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A80" s="82"/>
-      <c r="B80" s="82"/>
-      <c r="C80" s="82"/>
-      <c r="D80" s="66"/>
-      <c r="E80" s="66"/>
-      <c r="F80" s="66"/>
-      <c r="G80" s="66"/>
-      <c r="H80" s="66"/>
-      <c r="I80" s="66"/>
-      <c r="J80" s="66"/>
-      <c r="K80" s="69"/>
-      <c r="L80" s="66"/>
+      <c r="A80" s="81"/>
+      <c r="B80" s="81"/>
+      <c r="C80" s="81"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
+      <c r="H80" s="61"/>
+      <c r="I80" s="61"/>
+      <c r="J80" s="61"/>
+      <c r="K80" s="78"/>
+      <c r="L80" s="61"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="82"/>
@@ -27194,17 +27329,17 @@
       <c r="L83" s="54"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" s="80" t="s">
+      <c r="A84" s="225" t="s">
         <v>113</v>
       </c>
       <c r="C84" s="228">
         <v>29</v>
       </c>
-      <c r="E84" s="80" t="s">
+      <c r="E84" s="225" t="s">
         <v>118</v>
       </c>
       <c r="G84" s="228" t="s">
-        <v>1084</v>
+        <v>1107</v>
       </c>
       <c r="I84" s="57" t="s">
         <v>0</v>
@@ -27214,14 +27349,14 @@
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="82" t="s">
+      <c r="A85" s="225" t="s">
         <v>112</v>
       </c>
       <c r="B85" s="66"/>
       <c r="C85" s="227">
         <v>29</v>
       </c>
-      <c r="E85" s="82" t="s">
+      <c r="E85" s="225" t="s">
         <v>119</v>
       </c>
       <c r="F85" s="66"/>
@@ -27234,13 +27369,13 @@
       <c r="L85" s="69"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" s="80" t="s">
+      <c r="A86" s="225" t="s">
         <v>114</v>
       </c>
       <c r="C86" s="228">
         <v>1998</v>
       </c>
-      <c r="E86" s="80" t="s">
+      <c r="E86" s="225" t="s">
         <v>120</v>
       </c>
       <c r="G86" s="228" t="s">
@@ -27252,14 +27387,14 @@
       <c r="L86" s="131"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A87" s="82" t="s">
+      <c r="A87" s="225" t="s">
         <v>115</v>
       </c>
       <c r="B87" s="66"/>
       <c r="C87" s="229">
         <v>45943</v>
       </c>
-      <c r="E87" s="82" t="s">
+      <c r="E87" s="225" t="s">
         <v>121</v>
       </c>
       <c r="F87" s="66"/>
@@ -27272,13 +27407,13 @@
       <c r="L87" s="69"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A88" s="80" t="s">
+      <c r="A88" s="225" t="s">
         <v>116</v>
       </c>
       <c r="C88" s="228" t="s">
         <v>1083</v>
       </c>
-      <c r="E88" s="80" t="s">
+      <c r="E88" s="225" t="s">
         <v>122</v>
       </c>
       <c r="G88" s="228" t="s">
@@ -27288,14 +27423,14 @@
       <c r="L88" s="54"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A89" s="82" t="s">
+      <c r="A89" s="225" t="s">
         <v>117</v>
       </c>
       <c r="B89" s="66"/>
       <c r="C89" s="227" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E89" s="82"/>
+        <v>1084</v>
+      </c>
+      <c r="E89" s="225"/>
       <c r="F89" s="66"/>
       <c r="G89" s="227"/>
       <c r="I89" s="66"/>
@@ -27311,7 +27446,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="90" t="s">
-        <v>68</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
@@ -27379,7 +27514,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="226" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B98" s="226"/>
       <c r="C98" s="226"/>
@@ -27423,243 +27558,326 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="57" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D103" s="57" t="s">
+      <c r="C102" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="E103" s="57" t="s">
+      <c r="D102" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="E102" s="57" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="82" t="s">
+        <v>407</v>
+      </c>
+      <c r="B104" s="66"/>
+      <c r="C104" s="169">
+        <v>1</v>
+      </c>
+      <c r="D104" s="134" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E104" s="82" t="s">
+        <v>483</v>
+      </c>
+      <c r="F104" s="66"/>
+      <c r="G104" s="66"/>
+      <c r="H104" s="66"/>
+      <c r="I104" s="66"/>
+      <c r="J104" s="66"/>
+      <c r="K104" s="69"/>
+      <c r="L104" s="66"/>
+    </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A105" s="99" t="s">
-        <v>407</v>
-      </c>
-      <c r="B105" s="66"/>
-      <c r="C105" s="66"/>
-      <c r="D105" s="169">
-        <v>1</v>
-      </c>
-      <c r="E105" s="99" t="s">
-        <v>483</v>
-      </c>
-      <c r="F105" s="66"/>
-      <c r="G105" s="66"/>
-      <c r="H105" s="66"/>
-      <c r="I105" s="66"/>
-      <c r="J105" s="66"/>
-      <c r="K105" s="69"/>
-      <c r="L105" s="66"/>
+      <c r="A105" s="80" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C105" s="169" t="s">
+        <v>131</v>
+      </c>
+      <c r="D105" s="134" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E105" s="82" t="s">
+        <v>1104</v>
+      </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D106" s="167"/>
+      <c r="A106" s="66"/>
+      <c r="B106" s="66"/>
+      <c r="C106" s="66"/>
+      <c r="D106" s="134"/>
+      <c r="E106" s="99"/>
+      <c r="F106" s="66"/>
+      <c r="G106" s="66"/>
+      <c r="H106" s="66"/>
+      <c r="I106" s="66"/>
+      <c r="J106" s="66"/>
+      <c r="K106" s="69"/>
+      <c r="L106" s="66"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A107" s="66"/>
-      <c r="B107" s="66"/>
-      <c r="C107" s="66"/>
-      <c r="D107" s="169"/>
-      <c r="E107" s="66"/>
-      <c r="F107" s="66"/>
-      <c r="G107" s="66"/>
-      <c r="H107" s="66"/>
-      <c r="I107" s="66"/>
-      <c r="J107" s="66"/>
-      <c r="K107" s="69"/>
-      <c r="L107" s="66"/>
+      <c r="D107" s="134"/>
+      <c r="E107" s="99"/>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D108" s="167"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A109" s="66"/>
-      <c r="B109" s="66"/>
-      <c r="C109" s="66"/>
-      <c r="D109" s="169"/>
-      <c r="E109" s="66"/>
-      <c r="F109" s="66"/>
-      <c r="G109" s="66"/>
-      <c r="H109" s="66"/>
-      <c r="I109" s="66"/>
-      <c r="J109" s="66"/>
-      <c r="K109" s="69"/>
-      <c r="L109" s="66"/>
+      <c r="A108" s="66"/>
+      <c r="B108" s="66"/>
+      <c r="C108" s="66"/>
+      <c r="D108" s="134"/>
+      <c r="E108" s="99"/>
+      <c r="F108" s="66"/>
+      <c r="G108" s="66"/>
+      <c r="H108" s="66"/>
+      <c r="I108" s="66"/>
+      <c r="J108" s="66"/>
+      <c r="K108" s="69"/>
+      <c r="L108" s="66"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F110" s="72" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="111" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F111" s="72" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A112" s="80" t="s">
+      <c r="A111" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="B112" s="80" t="s">
+      <c r="B111" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="C112" s="80" t="s">
+      <c r="C111" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="D112" s="80"/>
-      <c r="E112" s="80"/>
-      <c r="F112" s="80" t="s">
+      <c r="D111" s="80"/>
+      <c r="E111" s="80"/>
+      <c r="F111" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="G112" s="80" t="s">
+      <c r="G111" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="H112" s="80" t="s">
+      <c r="H111" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="I112" s="80" t="s">
+      <c r="I111" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="J112" s="80" t="s">
+      <c r="J111" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="K112" s="75"/>
-      <c r="L112" s="80"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A114" s="66"/>
-      <c r="B114" s="66"/>
-      <c r="C114" s="66"/>
-      <c r="D114" s="66"/>
-      <c r="E114" s="66"/>
-      <c r="F114" s="66"/>
-      <c r="G114" s="66"/>
-      <c r="H114" s="66"/>
-      <c r="I114" s="66"/>
-      <c r="J114" s="66"/>
-      <c r="K114" s="69"/>
-      <c r="L114" s="66"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A116" s="66"/>
-      <c r="B116" s="66"/>
-      <c r="C116" s="66"/>
-      <c r="D116" s="66"/>
-      <c r="E116" s="66"/>
-      <c r="F116" s="66"/>
-      <c r="G116" s="66"/>
-      <c r="H116" s="66"/>
-      <c r="I116" s="66"/>
-      <c r="J116" s="66"/>
-      <c r="K116" s="69"/>
-      <c r="L116" s="66"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A118" s="66"/>
-      <c r="B118" s="66"/>
-      <c r="C118" s="66"/>
-      <c r="D118" s="66"/>
-      <c r="E118" s="66"/>
-      <c r="F118" s="66"/>
-      <c r="G118" s="66"/>
-      <c r="H118" s="66"/>
-      <c r="I118" s="66"/>
-      <c r="J118" s="66"/>
-      <c r="K118" s="69"/>
-      <c r="L118" s="66"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A120" s="66"/>
-      <c r="B120" s="66"/>
-      <c r="C120" s="66"/>
-      <c r="D120" s="66"/>
-      <c r="E120" s="66"/>
-      <c r="F120" s="66"/>
-      <c r="G120" s="66"/>
-      <c r="H120" s="66"/>
-      <c r="I120" s="66"/>
-      <c r="J120" s="66"/>
-      <c r="K120" s="69"/>
-      <c r="L120" s="66"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A122" s="66"/>
-      <c r="B122" s="66"/>
-      <c r="C122" s="66"/>
-      <c r="D122" s="66"/>
-      <c r="E122" s="66"/>
-      <c r="F122" s="66"/>
-      <c r="G122" s="66"/>
-      <c r="H122" s="66"/>
-      <c r="I122" s="66"/>
-      <c r="J122" s="66"/>
-      <c r="K122" s="69"/>
-      <c r="L122" s="66"/>
+      <c r="K111" s="75"/>
+      <c r="L111" s="80"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A113" s="66"/>
+      <c r="B113" s="66"/>
+      <c r="C113" s="66"/>
+      <c r="D113" s="66"/>
+      <c r="E113" s="66"/>
+      <c r="F113" s="66"/>
+      <c r="G113" s="66"/>
+      <c r="H113" s="66"/>
+      <c r="I113" s="66"/>
+      <c r="J113" s="66"/>
+      <c r="K113" s="69"/>
+      <c r="L113" s="66"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A115" s="66"/>
+      <c r="B115" s="66"/>
+      <c r="C115" s="66"/>
+      <c r="D115" s="66"/>
+      <c r="E115" s="66"/>
+      <c r="F115" s="66"/>
+      <c r="G115" s="66"/>
+      <c r="H115" s="66"/>
+      <c r="I115" s="66"/>
+      <c r="J115" s="66"/>
+      <c r="K115" s="69"/>
+      <c r="L115" s="66"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A117" s="66"/>
+      <c r="B117" s="66"/>
+      <c r="C117" s="66"/>
+      <c r="D117" s="66"/>
+      <c r="E117" s="66"/>
+      <c r="F117" s="66"/>
+      <c r="G117" s="66"/>
+      <c r="H117" s="66"/>
+      <c r="I117" s="66"/>
+      <c r="J117" s="66"/>
+      <c r="K117" s="69"/>
+      <c r="L117" s="66"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A119" s="66"/>
+      <c r="B119" s="66"/>
+      <c r="C119" s="66"/>
+      <c r="D119" s="66"/>
+      <c r="E119" s="66"/>
+      <c r="F119" s="66"/>
+      <c r="G119" s="66"/>
+      <c r="H119" s="66"/>
+      <c r="I119" s="66"/>
+      <c r="J119" s="66"/>
+      <c r="K119" s="69"/>
+      <c r="L119" s="66"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A121" s="66"/>
+      <c r="B121" s="66"/>
+      <c r="C121" s="66"/>
+      <c r="D121" s="66"/>
+      <c r="E121" s="66"/>
+      <c r="F121" s="66"/>
+      <c r="G121" s="66"/>
+      <c r="H121" s="66"/>
+      <c r="I121" s="66"/>
+      <c r="J121" s="66"/>
+      <c r="K121" s="69"/>
+      <c r="L121" s="66"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F123" s="72" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F124" s="72" t="s">
-        <v>71</v>
-      </c>
+      <c r="A124" s="230" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B124" s="230"/>
+      <c r="C124" s="231" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D124" s="230" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E124" s="224"/>
+      <c r="F124" s="224"/>
+      <c r="G124" s="224"/>
+      <c r="H124" s="224"/>
+      <c r="I124" s="224"/>
+      <c r="J124" s="224"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B125" s="72"/>
+      <c r="A125" s="230" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B125" s="230"/>
+      <c r="C125" s="231" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D125" s="230" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E125" s="224"/>
+      <c r="F125" s="224"/>
+      <c r="G125" s="224"/>
+      <c r="H125" s="224"/>
+      <c r="I125" s="224"/>
+      <c r="J125" s="224"/>
+      <c r="K125" s="232"/>
+      <c r="L125" s="224"/>
     </row>
     <row r="126" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="66"/>
-      <c r="B126" s="66"/>
-      <c r="C126" s="66"/>
-      <c r="D126" s="66"/>
-      <c r="E126" s="66"/>
-      <c r="F126" s="66"/>
-      <c r="G126" s="66"/>
-      <c r="H126" s="66"/>
-      <c r="I126" s="66"/>
-      <c r="J126" s="66"/>
-      <c r="K126" s="69"/>
-      <c r="L126" s="66"/>
+      <c r="A126" s="230" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B126" s="230"/>
+      <c r="C126" s="231" t="s">
+        <v>101</v>
+      </c>
+      <c r="D126" s="230" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E126" s="224"/>
+      <c r="F126" s="224"/>
+      <c r="G126" s="224"/>
+      <c r="H126" s="224"/>
+      <c r="I126" s="224"/>
+      <c r="J126" s="224"/>
+      <c r="K126" s="232"/>
+      <c r="L126" s="224"/>
     </row>
     <row r="127" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="66"/>
-      <c r="B127" s="66"/>
-      <c r="C127" s="66"/>
-      <c r="D127" s="66"/>
-      <c r="E127" s="66"/>
-      <c r="F127" s="66"/>
-      <c r="G127" s="66"/>
-      <c r="H127" s="66"/>
-      <c r="I127" s="66"/>
-      <c r="J127" s="66"/>
-      <c r="K127" s="69"/>
-      <c r="L127" s="66"/>
+      <c r="A127" s="230" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B127" s="230"/>
+      <c r="C127" s="231" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D127" s="230" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E127" s="224"/>
+      <c r="F127" s="224"/>
+      <c r="G127" s="224"/>
+      <c r="H127" s="224"/>
+      <c r="I127" s="224"/>
+      <c r="J127" s="224"/>
+      <c r="K127" s="232"/>
+      <c r="L127" s="224"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A128" s="61"/>
+      <c r="B128" s="61"/>
+      <c r="C128" s="61"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="61"/>
+      <c r="F128" s="61"/>
+      <c r="G128" s="61"/>
+      <c r="H128" s="61"/>
+      <c r="I128" s="61"/>
+      <c r="J128" s="61"/>
+      <c r="K128" s="78"/>
+      <c r="L128" s="61"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A129" s="66"/>
-      <c r="B129" s="66"/>
-      <c r="C129" s="66"/>
-      <c r="D129" s="66"/>
-      <c r="E129" s="66"/>
-      <c r="F129" s="66"/>
-      <c r="G129" s="66"/>
-      <c r="H129" s="66"/>
-      <c r="I129" s="66"/>
-      <c r="J129" s="66"/>
-      <c r="K129" s="69"/>
-      <c r="L129" s="66"/>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A131" s="66"/>
-      <c r="B131" s="66"/>
-      <c r="C131" s="66"/>
-      <c r="D131" s="66"/>
-      <c r="E131" s="66"/>
-      <c r="F131" s="66"/>
-      <c r="G131" s="66"/>
-      <c r="H131" s="66"/>
-      <c r="I131" s="66"/>
-      <c r="J131" s="66"/>
-      <c r="K131" s="69"/>
-      <c r="L131" s="66"/>
+      <c r="A129" s="63"/>
+      <c r="B129" s="63"/>
+      <c r="C129" s="63"/>
+      <c r="D129" s="63"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A130" s="99"/>
+      <c r="B130" s="99"/>
+      <c r="C130" s="99"/>
+      <c r="D130" s="99"/>
+      <c r="E130" s="66"/>
+      <c r="F130" s="66"/>
+      <c r="G130" s="66"/>
+      <c r="H130" s="66"/>
+      <c r="I130" s="66"/>
+      <c r="J130" s="66"/>
+      <c r="K130" s="69"/>
+      <c r="L130" s="66"/>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A132" s="66"/>
+      <c r="B132" s="66"/>
+      <c r="C132" s="66"/>
+      <c r="D132" s="66"/>
+      <c r="E132" s="66"/>
+      <c r="F132" s="66"/>
+      <c r="G132" s="66"/>
+      <c r="H132" s="66"/>
+      <c r="I132" s="66"/>
+      <c r="J132" s="66"/>
+      <c r="K132" s="69"/>
+      <c r="L132" s="66"/>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B134" s="72" t="s">
@@ -27897,6 +28115,19 @@
       <c r="J149" s="66"/>
       <c r="K149" s="69"/>
       <c r="L149" s="66"/>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A150" s="66"/>
+      <c r="B150" s="66"/>
+      <c r="C150" s="66"/>
+      <c r="D150" s="66"/>
+      <c r="E150" s="66"/>
+      <c r="F150" s="66"/>
+      <c r="G150" s="66"/>
+      <c r="H150" s="66"/>
+      <c r="J150" s="66"/>
+      <c r="K150" s="69"/>
+      <c r="L150" s="66"/>
     </row>
     <row r="175" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="179" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -31367,43 +31598,43 @@
       <c r="C3" s="47"/>
       <c r="D3" s="44">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3" s="44">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" s="44"/>
     </row>
@@ -31466,7 +31697,7 @@
       </c>
       <c r="M5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -31476,27 +31707,27 @@
       <c r="C6" s="47"/>
       <c r="D6" s="46">
         <f t="shared" ref="D6:D13" ca="1" si="2">IF(D$3&gt;=$B6,1,0)+IF(D$3=1,-1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="46">
         <f t="shared" ref="E6:M13" ca="1" si="3">IF(E$3&gt;=$B6,1,0)+D6+IF(E$3=1,-1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J6" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31508,7 +31739,7 @@
       </c>
       <c r="L6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M6" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31522,27 +31753,27 @@
       <c r="C7" s="47"/>
       <c r="D7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J7" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31554,7 +31785,7 @@
       </c>
       <c r="L7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31568,27 +31799,27 @@
       <c r="C8" s="47"/>
       <c r="D8" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J8" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31600,7 +31831,7 @@
       </c>
       <c r="L8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M8" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31626,7 +31857,7 @@
       </c>
       <c r="G9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31638,7 +31869,7 @@
       </c>
       <c r="J9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31646,7 +31877,7 @@
       </c>
       <c r="L9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31676,11 +31907,11 @@
       </c>
       <c r="H10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31688,7 +31919,7 @@
       </c>
       <c r="K10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31696,7 +31927,7 @@
       </c>
       <c r="M10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -31710,23 +31941,23 @@
       </c>
       <c r="E11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31742,7 +31973,7 @@
       </c>
       <c r="M11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -31756,39 +31987,39 @@
       </c>
       <c r="E12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -31822,15 +32053,15 @@
       </c>
       <c r="J13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31857,7 +32088,7 @@
       </c>
       <c r="G16" s="49" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -31873,7 +32104,7 @@
       <c r="F18" s="46"/>
       <c r="G18" s="50" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT(ADDRESS(E18+3,D18+3,1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -31912,7 +32143,7 @@
       <c r="F21" s="46"/>
       <c r="G21" s="50" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(ADDRESS(E21+3,D21+3,1))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -31938,7 +32169,7 @@
       <c r="F23" s="46"/>
       <c r="G23" s="50" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-11-24 17:28:16
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F26A1A-223C-47FF-929E-894A9C742AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC04EFA-456D-4A78-9D4D-123D47459B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25344" yWindow="0" windowWidth="29148" windowHeight="16656" activeTab="1" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
+    <workbookView xWindow="12444" yWindow="0" windowWidth="29148" windowHeight="16656" activeTab="1" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheda V3" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="1107">
   <si>
     <t>Nome</t>
   </si>
@@ -4372,9 +4372,6 @@
   </si>
   <si>
     <t>secondo piano di una casa color pastello, con travi a vista e finestre che danno sui murales.</t>
-  </si>
-  <si>
-    <t>Contatti / Amici</t>
   </si>
   <si>
     <t>Contatto</t>
@@ -26094,8 +26091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB020AF3-E2AF-4B08-9CF1-A8BB16CCBDFC}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G85" sqref="G85"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -26603,7 +26600,7 @@
       <c r="L29" s="54"/>
     </row>
     <row r="30" spans="1:12" s="73" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="57" t="s">
         <v>546</v>
       </c>
       <c r="B30" s="54">
@@ -26629,7 +26626,7 @@
       <c r="L30" s="54"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="57" t="s">
         <v>328</v>
       </c>
       <c r="B31" s="54">
@@ -26650,7 +26647,7 @@
       <c r="L31" s="54"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="57" t="s">
         <v>320</v>
       </c>
       <c r="B32" s="54">
@@ -26668,7 +26665,7 @@
       <c r="L32" s="54"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="57" t="s">
         <v>320</v>
       </c>
       <c r="B33" s="54">
@@ -26979,7 +26976,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="155" t="s">
+      <c r="A52" s="165" t="s">
         <v>780</v>
       </c>
       <c r="C52" s="54">
@@ -26990,7 +26987,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="165" t="s">
         <v>97</v>
       </c>
       <c r="C53" s="54">
@@ -27001,7 +26998,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="155" t="s">
+      <c r="A54" s="165" t="s">
         <v>99</v>
       </c>
       <c r="C54" s="54">
@@ -27013,7 +27010,7 @@
       <c r="E54" s="155"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="155" t="s">
+      <c r="A55" s="165" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="54">
@@ -27025,7 +27022,7 @@
       <c r="E55" s="155"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="155" t="s">
+      <c r="A56" s="165" t="s">
         <v>101</v>
       </c>
       <c r="C56" s="54">
@@ -27037,7 +27034,7 @@
       <c r="E56" s="155"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="155" t="s">
+      <c r="A57" s="165" t="s">
         <v>98</v>
       </c>
       <c r="C57" s="54">
@@ -27097,7 +27094,7 @@
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="155" t="s">
+      <c r="A63" s="165" t="s">
         <v>1056</v>
       </c>
       <c r="C63" s="54">
@@ -27108,12 +27105,13 @@
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="63"/>
       <c r="D64" s="80" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="155" t="s">
+      <c r="A65" s="165" t="s">
         <v>1054</v>
       </c>
       <c r="C65" s="54">
@@ -27124,7 +27122,7 @@
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="155" t="s">
+      <c r="A66" s="165" t="s">
         <v>1057</v>
       </c>
       <c r="C66" s="54">
@@ -27135,7 +27133,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="155" t="s">
+      <c r="A67" s="165" t="s">
         <v>1055</v>
       </c>
       <c r="C67" s="54">
@@ -27146,7 +27144,7 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="155" t="s">
+      <c r="A68" s="165" t="s">
         <v>1058</v>
       </c>
       <c r="C68" s="54">
@@ -27339,7 +27337,7 @@
         <v>118</v>
       </c>
       <c r="G84" s="228" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="I84" s="57" t="s">
         <v>0</v>
@@ -27446,7 +27444,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="90" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
@@ -27558,7 +27556,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -27584,7 +27582,7 @@
         <v>1</v>
       </c>
       <c r="D104" s="134" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E104" s="82" t="s">
         <v>483</v>
@@ -27599,16 +27597,16 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="80" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C105" s="169" t="s">
         <v>131</v>
       </c>
       <c r="D105" s="134" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E105" s="82" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
@@ -27750,19 +27748,19 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F123" s="72" t="s">
-        <v>1090</v>
+        <v>97</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="230" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B124" s="230"/>
       <c r="C124" s="231" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D124" s="230" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E124" s="224"/>
       <c r="F124" s="224"/>
@@ -27773,14 +27771,14 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="230" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B125" s="230"/>
       <c r="C125" s="231" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D125" s="230" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E125" s="224"/>
       <c r="F125" s="224"/>
@@ -27793,14 +27791,14 @@
     </row>
     <row r="126" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="230" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B126" s="230"/>
       <c r="C126" s="231" t="s">
         <v>101</v>
       </c>
       <c r="D126" s="230" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="E126" s="224"/>
       <c r="F126" s="224"/>
@@ -27813,14 +27811,14 @@
     </row>
     <row r="127" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="230" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B127" s="230"/>
       <c r="C127" s="231" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D127" s="230" t="s">
         <v>1097</v>
-      </c>
-      <c r="D127" s="230" t="s">
-        <v>1098</v>
       </c>
       <c r="E127" s="224"/>
       <c r="F127" s="224"/>
@@ -31598,35 +31596,35 @@
       <c r="C3" s="47"/>
       <c r="D3" s="44">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="44">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L3" s="44">
         <f t="shared" ca="1" si="0"/>
@@ -31634,7 +31632,7 @@
       </c>
       <c r="M3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N3" s="44"/>
     </row>
@@ -31707,39 +31705,39 @@
       <c r="C6" s="47"/>
       <c r="D6" s="46">
         <f t="shared" ref="D6:D13" ca="1" si="2">IF(D$3&gt;=$B6,1,0)+IF(D$3=1,-1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="46">
         <f t="shared" ref="E6:M13" ca="1" si="3">IF(E$3&gt;=$B6,1,0)+D6+IF(E$3=1,-1,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M6" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31753,39 +31751,39 @@
       <c r="C7" s="47"/>
       <c r="D7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31799,43 +31797,43 @@
       <c r="C8" s="47"/>
       <c r="D8" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -31849,11 +31847,11 @@
       </c>
       <c r="E9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31861,11 +31859,11 @@
       </c>
       <c r="H9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31881,7 +31879,7 @@
       </c>
       <c r="M9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -31895,11 +31893,11 @@
       </c>
       <c r="E10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31907,11 +31905,11 @@
       </c>
       <c r="H10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31919,11 +31917,11 @@
       </c>
       <c r="K10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31941,11 +31939,11 @@
       </c>
       <c r="E11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31953,7 +31951,7 @@
       </c>
       <c r="H11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31961,19 +31959,19 @@
       </c>
       <c r="J11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -31987,11 +31985,11 @@
       </c>
       <c r="E12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -31999,7 +31997,7 @@
       </c>
       <c r="H12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -32007,19 +32005,19 @@
       </c>
       <c r="J12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -32049,23 +32047,23 @@
       </c>
       <c r="I13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -32088,7 +32086,7 @@
       </c>
       <c r="G16" s="49" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -32117,7 +32115,7 @@
       <c r="F19" s="46"/>
       <c r="G19" s="50" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(E19+3,D19+3,1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -32130,7 +32128,7 @@
       <c r="F20" s="46"/>
       <c r="G20" s="50" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
vault backup: 2025-11-26 01:29:02
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99107EC-4983-470A-BF7D-DDA3E3B16E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C93BE43-A0A6-43B8-BC42-3868EC167D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25452" yWindow="0" windowWidth="29148" windowHeight="16656" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2820" uniqueCount="1217">
   <si>
     <t>Nome</t>
   </si>
@@ -3607,9 +3607,6 @@
     <t>Non mi interessa cosa è di moda. Io rispetto l’ordine. Pretendo lo stesso.</t>
   </si>
   <si>
-    <t>Attivista civica diventata predatrice.</t>
-  </si>
-  <si>
     <t>Sociologia</t>
   </si>
   <si>
@@ -3741,6 +3738,42 @@
   </si>
   <si>
     <t>Caccia “sociale e discreta”: conosce percorsi, dislivelli, movimenti delle persone; tra il Ponte di Tiberio e il Comune.</t>
+  </si>
+  <si>
+    <t>Non gioca al potere: lo esercita davvero.</t>
+  </si>
+  <si>
+    <t>Colei che ospita e accoglie… ma controvoglia</t>
+  </si>
+  <si>
+    <t>Marta Fioravanti</t>
+  </si>
+  <si>
+    <t>Masochista</t>
+  </si>
+  <si>
+    <t>Trova soddisfazione nel dolore o nella punizione.</t>
+  </si>
+  <si>
+    <t>Eloquente</t>
+  </si>
+  <si>
+    <t>+PV Quando si procura o accetta dolore con intenzione per un obiettivo</t>
+  </si>
+  <si>
+    <t>Letteratura</t>
+  </si>
+  <si>
+    <t>Le tradizioni</t>
+  </si>
+  <si>
+    <t>Poesia</t>
+  </si>
+  <si>
+    <t>Notare suoni, odori, dettagli che gli altri perdono.</t>
+  </si>
+  <si>
+    <t>Percezione + Allerta 4 o +1/+2 dadi ai tiri basati sui sensi.</t>
   </si>
 </sst>
 </file>
@@ -3750,7 +3783,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="59" x14ac:knownFonts="1">
+  <fonts count="60" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4129,6 +4162,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Bahnschrift Condensed"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -4526,7 +4566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5204,6 +5244,12 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -6165,6 +6211,111 @@
           </xdr:spPr>
         </xdr:pic>
       </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>309282</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>26895</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>522650</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>151104</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="Gruppo 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68ADF180-209F-BB95-51EF-5643DD70C1BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5230906" y="6660777"/>
+          <a:ext cx="213368" cy="124209"/>
+          <a:chOff x="5239870" y="6665259"/>
+          <a:chExt cx="213368" cy="124209"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="28" name="Elemento grafico 27" descr="Acqua contorno">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72B9873C-3499-4A03-BA57-566961DD1B09}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5239870" y="6665259"/>
+            <a:ext cx="115035" cy="124203"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="29" name="Elemento grafico 28" descr="Acqua contorno">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9E69684-E5A2-4891-9E16-8FE2BADA026E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5337518" y="6665265"/>
+            <a:ext cx="115720" cy="124203"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -21184,8 +21335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5334263-4143-413C-81B1-B37F8CC6DF82}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -21218,8 +21369,8 @@
       </c>
       <c r="J1" s="100"/>
       <c r="K1" s="61"/>
-      <c r="L1" s="209" t="s">
-        <v>1017</v>
+      <c r="L1" s="243" t="s">
+        <v>1206</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -21227,16 +21378,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>1012</v>
+        <v>1207</v>
       </c>
       <c r="E3" s="156" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="152" t="s">
-        <v>503</v>
+        <v>1208</v>
       </c>
       <c r="H3" s="55" t="s">
-        <v>1013</v>
+        <v>1209</v>
       </c>
       <c r="K3" s="57"/>
     </row>
@@ -21247,8 +21398,8 @@
       <c r="B4" s="57" t="s">
         <v>1040</v>
       </c>
-      <c r="H4" s="55" t="s">
-        <v>1014</v>
+      <c r="H4" s="244" t="s">
+        <v>1211</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -21256,7 +21407,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="152" t="s">
-        <v>502</v>
+        <v>387</v>
       </c>
       <c r="E5" s="210" t="s">
         <v>3</v>
@@ -21265,9 +21416,7 @@
         <v>504</v>
       </c>
       <c r="G5" s="85"/>
-      <c r="H5" s="140" t="s">
-        <v>1015</v>
-      </c>
+      <c r="H5" s="140"/>
       <c r="I5" s="85"/>
       <c r="J5" s="85"/>
       <c r="K5" s="131"/>
@@ -21280,9 +21429,7 @@
       <c r="B6" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="H6" s="55" t="s">
-        <v>1016</v>
-      </c>
+      <c r="H6" s="55"/>
     </row>
     <row r="8" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F8" s="72" t="s">
@@ -21312,21 +21459,25 @@
       </c>
       <c r="B10" s="80"/>
       <c r="D10" s="163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="165" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="80"/>
+      <c r="F10" s="80" t="s">
+        <v>1210</v>
+      </c>
       <c r="H10" s="163">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="80"/>
+      <c r="J10" s="80" t="s">
+        <v>1163</v>
+      </c>
       <c r="L10" s="163">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -21335,14 +21486,14 @@
       </c>
       <c r="B11" s="80"/>
       <c r="D11" s="163">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="165" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="80"/>
       <c r="H11" s="163">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11" s="165" t="s">
         <v>18</v>
@@ -21358,23 +21509,21 @@
       </c>
       <c r="B12" s="80"/>
       <c r="D12" s="163">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="80" t="s">
-        <v>509</v>
-      </c>
+      <c r="F12" s="80"/>
       <c r="H12" s="163">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I12" s="165" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="80"/>
       <c r="L12" s="163">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -21424,10 +21573,10 @@
         <v>31</v>
       </c>
       <c r="J16" s="111" t="s">
-        <v>1018</v>
+        <v>1212</v>
       </c>
       <c r="L16" s="163">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -21436,7 +21585,7 @@
       </c>
       <c r="B17" s="80"/>
       <c r="D17" s="163">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="154" t="s">
         <v>33</v>
@@ -21444,14 +21593,14 @@
       <c r="F17" s="80"/>
       <c r="G17" s="54"/>
       <c r="H17" s="163">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I17" s="154" t="s">
         <v>34</v>
       </c>
       <c r="J17" s="80"/>
       <c r="L17" s="163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -21460,7 +21609,7 @@
       </c>
       <c r="B18" s="80"/>
       <c r="D18" s="163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="154" t="s">
         <v>437</v>
@@ -21468,7 +21617,7 @@
       <c r="F18" s="80"/>
       <c r="G18" s="54"/>
       <c r="H18" s="163">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18" s="154" t="s">
         <v>36</v>
@@ -21484,7 +21633,7 @@
       </c>
       <c r="B19" s="80"/>
       <c r="D19" s="163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="154" t="s">
         <v>38</v>
@@ -21492,7 +21641,7 @@
       <c r="F19" s="80"/>
       <c r="G19" s="54"/>
       <c r="H19" s="163">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19" s="154" t="s">
         <v>45</v>
@@ -21506,9 +21655,11 @@
       <c r="A20" s="154" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="80"/>
+      <c r="B20" s="80" t="s">
+        <v>1214</v>
+      </c>
       <c r="D20" s="163">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20" s="154" t="s">
         <v>39</v>
@@ -21521,7 +21672,9 @@
       <c r="I20" s="154" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="80"/>
+      <c r="J20" s="111" t="s">
+        <v>1213</v>
+      </c>
       <c r="L20" s="163">
         <v>1</v>
       </c>
@@ -21532,7 +21685,7 @@
       </c>
       <c r="B21" s="80"/>
       <c r="D21" s="163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="154" t="s">
         <v>40</v>
@@ -21556,7 +21709,7 @@
       </c>
       <c r="B22" s="80"/>
       <c r="D22" s="163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="154" t="s">
         <v>41</v>
@@ -21580,7 +21733,7 @@
       </c>
       <c r="B23" s="80"/>
       <c r="D23" s="163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="154" t="s">
         <v>42</v>
@@ -21588,7 +21741,7 @@
       <c r="F23" s="80"/>
       <c r="G23" s="54"/>
       <c r="H23" s="163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="154" t="s">
         <v>49</v>
@@ -21604,7 +21757,7 @@
       </c>
       <c r="B24" s="80"/>
       <c r="D24" s="163">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" s="154" t="s">
         <v>43</v>
@@ -21619,7 +21772,7 @@
       </c>
       <c r="J24" s="80"/>
       <c r="L24" s="163">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -21628,7 +21781,7 @@
       </c>
       <c r="B25" s="80"/>
       <c r="D25" s="163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="154" t="s">
         <v>44</v>
@@ -21636,7 +21789,7 @@
       <c r="F25" s="80"/>
       <c r="G25" s="54"/>
       <c r="H25" s="163">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I25" s="154" t="s">
         <v>51</v>
@@ -21694,13 +21847,13 @@
     </row>
     <row r="30" spans="1:12" s="73" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="57" t="s">
-        <v>512</v>
+        <v>317</v>
       </c>
       <c r="B30" s="54">
         <v>1</v>
       </c>
       <c r="C30" s="80" t="s">
-        <v>1041</v>
+        <v>1215</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -21719,14 +21872,8 @@
       <c r="L30" s="54"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="57" t="s">
-        <v>328</v>
-      </c>
-      <c r="B31" s="54">
-        <v>1</v>
-      </c>
       <c r="C31" s="80" t="s">
-        <v>440</v>
+        <v>1216</v>
       </c>
       <c r="H31" s="166" t="s">
         <v>59</v>
@@ -21741,13 +21888,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="57" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="B32" s="54">
         <v>1</v>
       </c>
       <c r="C32" s="80" t="s">
-        <v>1042</v>
+        <v>440</v>
       </c>
       <c r="H32" s="63" t="s">
         <v>70</v>
@@ -21758,15 +21905,18 @@
       <c r="L32" s="54"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="233" t="s">
         <v>320</v>
       </c>
-      <c r="B33" s="54">
-        <v>2</v>
-      </c>
-      <c r="C33" s="80" t="s">
-        <v>1044</v>
-      </c>
+      <c r="B33" s="234">
+        <v>1</v>
+      </c>
+      <c r="C33" s="241" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D33" s="233"/>
+      <c r="E33" s="233"/>
+      <c r="F33" s="233"/>
       <c r="H33" s="63" t="s">
         <v>66</v>
       </c>
@@ -21780,9 +21930,12 @@
       <c r="L33" s="54"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="80" t="s">
-        <v>1043</v>
-      </c>
+      <c r="A34" s="61"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
       <c r="L34" s="215" t="s">
         <v>471</v>
       </c>
@@ -21792,7 +21945,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="167">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K35" s="162" t="s">
         <v>478</v>
@@ -21810,7 +21963,7 @@
         <v>1019</v>
       </c>
       <c r="J36" s="167">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K36" s="162" t="s">
         <v>494</v>
@@ -25800,8 +25953,8 @@
   <sheetPr codeName="Foglio7"/>
   <dimension ref="A2:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -30847,8 +31000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AF1615-1EA2-4AD7-A86C-59952E5A099E}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A29" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -30871,10 +31024,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="54" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H1" s="151" t="s">
         <v>1202</v>
-      </c>
-      <c r="H1" s="151" t="s">
-        <v>1203</v>
       </c>
       <c r="I1" s="81" t="s">
         <v>348</v>
@@ -30882,7 +31035,7 @@
       <c r="J1" s="100"/>
       <c r="K1" s="61"/>
       <c r="L1" s="209" t="s">
-        <v>1161</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -30988,7 +31141,7 @@
         <v>13</v>
       </c>
       <c r="J10" s="80" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="L10" s="163">
         <v>4</v>
@@ -30999,7 +31152,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="80" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="D11" s="163">
         <v>4</v>
@@ -31089,7 +31242,7 @@
         <v>31</v>
       </c>
       <c r="J16" s="111" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="L16" s="163">
         <v>1</v>
@@ -31100,7 +31253,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="80" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="D17" s="163">
         <v>4</v>
@@ -31157,7 +31310,7 @@
         <v>38</v>
       </c>
       <c r="F19" s="80" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="G19" s="54"/>
       <c r="H19" s="163">
@@ -31362,13 +31515,13 @@
     </row>
     <row r="30" spans="1:12" s="73" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="57" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B30" s="54">
         <v>1</v>
       </c>
       <c r="C30" s="175" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -31388,13 +31541,13 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="239" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B31" s="54">
         <v>1</v>
       </c>
       <c r="C31" s="80" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="H31" s="166" t="s">
         <v>59</v>
@@ -31409,13 +31562,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="239" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B32" s="54">
         <v>2</v>
       </c>
       <c r="C32" s="80" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H32" s="63" t="s">
         <v>70</v>
@@ -31429,7 +31582,7 @@
       <c r="A33" s="233"/>
       <c r="B33" s="234"/>
       <c r="C33" s="241" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="D33" s="233"/>
       <c r="E33" s="233"/>
@@ -31479,7 +31632,7 @@
         <v>1019</v>
       </c>
       <c r="J36" s="167">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K36" s="162" t="s">
         <v>494</v>
@@ -31751,7 +31904,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="80" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -31762,7 +31915,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="80" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -31773,7 +31926,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="80" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="E54" s="155"/>
     </row>
@@ -31797,7 +31950,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="80" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="E56" s="155"/>
     </row>
@@ -31863,30 +32016,30 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="165" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C63" s="54">
         <v>-3</v>
       </c>
       <c r="D63" s="80" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="63"/>
       <c r="D64" s="239" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="165" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C65" s="54">
         <v>-3</v>
       </c>
       <c r="D65" s="239" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -31955,7 +32108,7 @@
         <v>105</v>
       </c>
       <c r="C73" s="63" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -31963,7 +32116,7 @@
         <v>106</v>
       </c>
       <c r="C74" s="63" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -31971,7 +32124,7 @@
         <v>98</v>
       </c>
       <c r="C75" s="63" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -32006,10 +32159,10 @@
       </c>
       <c r="B79" s="80"/>
       <c r="C79" s="80" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E79" s="57" t="s">
         <v>1192</v>
-      </c>
-      <c r="E79" s="57" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -32061,7 +32214,7 @@
         <v>118</v>
       </c>
       <c r="G84" s="212" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="I84" s="57" t="s">
         <v>0</v>
@@ -32101,7 +32254,7 @@
         <v>120</v>
       </c>
       <c r="G86" s="212" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="I86" s="85"/>
       <c r="J86" s="85"/>
@@ -32121,7 +32274,7 @@
       </c>
       <c r="F87" s="66"/>
       <c r="G87" s="211" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="I87" s="66"/>
       <c r="J87" s="66"/>
@@ -32133,13 +32286,13 @@
         <v>116</v>
       </c>
       <c r="C88" s="212" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E88" s="80" t="s">
         <v>122</v>
       </c>
       <c r="G88" s="212" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="K88" s="57"/>
       <c r="L88" s="54"/>
@@ -32150,7 +32303,7 @@
       </c>
       <c r="B89" s="66"/>
       <c r="C89" s="211" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="E89" s="80"/>
       <c r="F89" s="66"/>
@@ -32173,7 +32326,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="237" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B93" s="237"/>
       <c r="C93" s="237"/>
@@ -32236,7 +32389,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="216" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B98" s="216"/>
       <c r="C98" s="216"/>
@@ -32321,7 +32474,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="80" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C104" s="169" t="s">
         <v>131</v>
@@ -32330,7 +32483,7 @@
         <v>1071</v>
       </c>
       <c r="E104" s="238" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
@@ -32491,26 +32644,26 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="63" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B124" s="63"/>
       <c r="C124" s="155" t="s">
         <v>96</v>
       </c>
       <c r="D124" s="63" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="232" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B125" s="232"/>
       <c r="C125" s="240" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D125" s="241" t="s">
         <v>1181</v>
-      </c>
-      <c r="D125" s="241" t="s">
-        <v>1182</v>
       </c>
       <c r="E125" s="233"/>
       <c r="F125" s="233"/>
@@ -32523,14 +32676,14 @@
     </row>
     <row r="126" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="232" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B126" s="232"/>
       <c r="C126" s="240" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D126" s="232" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="E126" s="233"/>
       <c r="F126" s="233"/>
@@ -33082,7 +33235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB020AF3-E2AF-4B08-9CF1-A8BB16CCBDFC}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -35293,7 +35446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618731C0-8D69-42F5-B683-631FA94DA355}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
@@ -42761,19 +42914,19 @@
       <c r="C3" s="47"/>
       <c r="D3" s="44">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E3" s="44">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H3" s="44">
         <f t="shared" ca="1" si="0"/>
@@ -42781,23 +42934,23 @@
       </c>
       <c r="I3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N3" s="44"/>
     </row>
@@ -42898,15 +43051,15 @@
       </c>
       <c r="K6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -42944,11 +43097,11 @@
       </c>
       <c r="K7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -42962,43 +43115,43 @@
       <c r="C8" s="47"/>
       <c r="D8" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -43008,43 +43161,43 @@
       <c r="C9" s="47"/>
       <c r="D9" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -43054,43 +43207,43 @@
       <c r="C10" s="47"/>
       <c r="D10" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -43100,43 +43253,43 @@
       <c r="C11" s="47"/>
       <c r="D11" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -43146,43 +43299,43 @@
       <c r="C12" s="47"/>
       <c r="D12" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -43192,43 +43345,43 @@
       <c r="C13" s="47"/>
       <c r="D13" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -43251,7 +43404,7 @@
       </c>
       <c r="G16" s="49" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -43267,7 +43420,7 @@
       <c r="F18" s="46"/>
       <c r="G18" s="50" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT(ADDRESS(E18+3,D18+3,1))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -43280,7 +43433,7 @@
       <c r="F19" s="46"/>
       <c r="G19" s="50" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(E19+3,D19+3,1))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -43293,7 +43446,7 @@
       <c r="F20" s="46"/>
       <c r="G20" s="50" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -43306,7 +43459,7 @@
       <c r="F21" s="46"/>
       <c r="G21" s="50" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(ADDRESS(E21+3,D21+3,1))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -43319,7 +43472,7 @@
       <c r="F22" s="46"/>
       <c r="G22" s="50" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT(ADDRESS(E22+3,D22+3,1))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -43332,7 +43485,7 @@
       <c r="F23" s="46"/>
       <c r="G23" s="50" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-11-26 15:13:24
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BC718F-41FF-48E2-AED7-59F2A00D0C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468A6866-40DC-45C3-BFAD-C57D37869489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25452" yWindow="0" windowWidth="29148" windowHeight="16656" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
+    <workbookView xWindow="24120" yWindow="1116" windowWidth="29148" windowHeight="15228" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
   <sheets>
     <sheet name="_Ventrue" sheetId="18" r:id="rId1"/>
@@ -4733,7 +4733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5330,11 +5330,53 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="57" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="57" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="57" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5357,73 +5399,10 @@
     <xf numFmtId="164" fontId="57" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="57" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="57" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -22441,7 +22420,7 @@
       <c r="B4" s="57" t="s">
         <v>1040</v>
       </c>
-      <c r="H4" s="243" t="s">
+      <c r="H4" s="224" t="s">
         <v>1253</v>
       </c>
     </row>
@@ -23406,7 +23385,7 @@
       <c r="D66" s="80"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="241"/>
+      <c r="A67" s="222"/>
       <c r="B67" s="66"/>
       <c r="C67" s="69"/>
       <c r="D67" s="82"/>
@@ -23420,7 +23399,7 @@
       <c r="L67" s="66"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="241"/>
+      <c r="A68" s="222"/>
       <c r="B68" s="66"/>
       <c r="C68" s="69"/>
       <c r="D68" s="82"/>
@@ -23584,7 +23563,7 @@
       <c r="A86" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="C86" s="235"/>
+      <c r="C86" s="219"/>
       <c r="E86" s="80" t="s">
         <v>120</v>
       </c>
@@ -23648,60 +23627,60 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="216"/>
-      <c r="B93" s="216"/>
-      <c r="C93" s="216"/>
-      <c r="D93" s="216"/>
-      <c r="E93" s="216"/>
-      <c r="F93" s="216"/>
-      <c r="G93" s="216"/>
-      <c r="H93" s="216"/>
-      <c r="I93" s="216"/>
-      <c r="J93" s="216"/>
-      <c r="K93" s="216"/>
-      <c r="L93" s="216"/>
+      <c r="A93" s="227"/>
+      <c r="B93" s="227"/>
+      <c r="C93" s="227"/>
+      <c r="D93" s="227"/>
+      <c r="E93" s="227"/>
+      <c r="F93" s="227"/>
+      <c r="G93" s="227"/>
+      <c r="H93" s="227"/>
+      <c r="I93" s="227"/>
+      <c r="J93" s="227"/>
+      <c r="K93" s="227"/>
+      <c r="L93" s="227"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="216"/>
-      <c r="B94" s="216"/>
-      <c r="C94" s="216"/>
-      <c r="D94" s="216"/>
-      <c r="E94" s="216"/>
-      <c r="F94" s="216"/>
-      <c r="G94" s="216"/>
-      <c r="H94" s="216"/>
-      <c r="I94" s="216"/>
-      <c r="J94" s="216"/>
-      <c r="K94" s="216"/>
-      <c r="L94" s="216"/>
+      <c r="A94" s="227"/>
+      <c r="B94" s="227"/>
+      <c r="C94" s="227"/>
+      <c r="D94" s="227"/>
+      <c r="E94" s="227"/>
+      <c r="F94" s="227"/>
+      <c r="G94" s="227"/>
+      <c r="H94" s="227"/>
+      <c r="I94" s="227"/>
+      <c r="J94" s="227"/>
+      <c r="K94" s="227"/>
+      <c r="L94" s="227"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="216"/>
-      <c r="B95" s="216"/>
-      <c r="C95" s="216"/>
-      <c r="D95" s="216"/>
-      <c r="E95" s="216"/>
-      <c r="F95" s="216"/>
-      <c r="G95" s="216"/>
-      <c r="H95" s="216"/>
-      <c r="I95" s="216"/>
-      <c r="J95" s="216"/>
-      <c r="K95" s="216"/>
-      <c r="L95" s="216"/>
+      <c r="A95" s="227"/>
+      <c r="B95" s="227"/>
+      <c r="C95" s="227"/>
+      <c r="D95" s="227"/>
+      <c r="E95" s="227"/>
+      <c r="F95" s="227"/>
+      <c r="G95" s="227"/>
+      <c r="H95" s="227"/>
+      <c r="I95" s="227"/>
+      <c r="J95" s="227"/>
+      <c r="K95" s="227"/>
+      <c r="L95" s="227"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="216"/>
-      <c r="B96" s="216"/>
-      <c r="C96" s="216"/>
-      <c r="D96" s="216"/>
-      <c r="E96" s="216"/>
-      <c r="F96" s="216"/>
-      <c r="G96" s="216"/>
-      <c r="H96" s="216"/>
-      <c r="I96" s="216"/>
-      <c r="J96" s="216"/>
-      <c r="K96" s="216"/>
-      <c r="L96" s="216"/>
+      <c r="A96" s="227"/>
+      <c r="B96" s="227"/>
+      <c r="C96" s="227"/>
+      <c r="D96" s="227"/>
+      <c r="E96" s="227"/>
+      <c r="F96" s="227"/>
+      <c r="G96" s="227"/>
+      <c r="H96" s="227"/>
+      <c r="I96" s="227"/>
+      <c r="J96" s="227"/>
+      <c r="K96" s="227"/>
+      <c r="L96" s="227"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="90" t="s">
@@ -23709,46 +23688,46 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="216"/>
-      <c r="B98" s="216"/>
-      <c r="C98" s="216"/>
-      <c r="D98" s="216"/>
-      <c r="E98" s="216"/>
-      <c r="F98" s="216"/>
-      <c r="G98" s="216"/>
-      <c r="H98" s="216"/>
-      <c r="I98" s="216"/>
-      <c r="J98" s="216"/>
-      <c r="K98" s="216"/>
-      <c r="L98" s="216"/>
+      <c r="A98" s="227"/>
+      <c r="B98" s="227"/>
+      <c r="C98" s="227"/>
+      <c r="D98" s="227"/>
+      <c r="E98" s="227"/>
+      <c r="F98" s="227"/>
+      <c r="G98" s="227"/>
+      <c r="H98" s="227"/>
+      <c r="I98" s="227"/>
+      <c r="J98" s="227"/>
+      <c r="K98" s="227"/>
+      <c r="L98" s="227"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="216"/>
-      <c r="B99" s="216"/>
-      <c r="C99" s="216"/>
-      <c r="D99" s="216"/>
-      <c r="E99" s="216"/>
-      <c r="F99" s="216"/>
-      <c r="G99" s="216"/>
-      <c r="H99" s="216"/>
-      <c r="I99" s="216"/>
-      <c r="J99" s="216"/>
-      <c r="K99" s="216"/>
-      <c r="L99" s="216"/>
+      <c r="A99" s="227"/>
+      <c r="B99" s="227"/>
+      <c r="C99" s="227"/>
+      <c r="D99" s="227"/>
+      <c r="E99" s="227"/>
+      <c r="F99" s="227"/>
+      <c r="G99" s="227"/>
+      <c r="H99" s="227"/>
+      <c r="I99" s="227"/>
+      <c r="J99" s="227"/>
+      <c r="K99" s="227"/>
+      <c r="L99" s="227"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="216"/>
-      <c r="B100" s="216"/>
-      <c r="C100" s="216"/>
-      <c r="D100" s="216"/>
-      <c r="E100" s="216"/>
-      <c r="F100" s="216"/>
-      <c r="G100" s="216"/>
-      <c r="H100" s="216"/>
-      <c r="I100" s="216"/>
-      <c r="J100" s="216"/>
-      <c r="K100" s="216"/>
-      <c r="L100" s="216"/>
+      <c r="A100" s="227"/>
+      <c r="B100" s="227"/>
+      <c r="C100" s="227"/>
+      <c r="D100" s="227"/>
+      <c r="E100" s="227"/>
+      <c r="F100" s="227"/>
+      <c r="G100" s="227"/>
+      <c r="H100" s="227"/>
+      <c r="I100" s="227"/>
+      <c r="J100" s="227"/>
+      <c r="K100" s="227"/>
+      <c r="L100" s="227"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
@@ -23770,40 +23749,24 @@
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="240" t="s">
+      <c r="A103" s="80" t="s">
         <v>407</v>
       </c>
-      <c r="B103" s="233"/>
-      <c r="C103" s="245">
+      <c r="C103" s="167">
         <v>1</v>
       </c>
-      <c r="D103" s="247" t="s">
+      <c r="D103" s="226" t="s">
         <v>1068</v>
       </c>
-      <c r="E103" s="240" t="s">
+      <c r="E103" s="80" t="s">
         <v>483</v>
       </c>
-      <c r="F103" s="233"/>
-      <c r="G103" s="233"/>
-      <c r="H103" s="233"/>
-      <c r="I103" s="233"/>
-      <c r="J103" s="233"/>
-      <c r="K103" s="234"/>
-      <c r="L103" s="233"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="240"/>
-      <c r="B104" s="233"/>
-      <c r="C104" s="245"/>
-      <c r="D104" s="247"/>
-      <c r="E104" s="240"/>
-      <c r="F104" s="233"/>
-      <c r="G104" s="233"/>
-      <c r="H104" s="233"/>
-      <c r="I104" s="233"/>
-      <c r="J104" s="233"/>
-      <c r="K104" s="234"/>
-      <c r="L104" s="233"/>
+      <c r="A104" s="80"/>
+      <c r="C104" s="167"/>
+      <c r="D104" s="226"/>
+      <c r="E104" s="80"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="61"/>
@@ -27939,172 +27902,172 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" s="229" t="s">
+      <c r="B9" s="216" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" s="229" t="s">
+      <c r="B10" s="216" t="s">
         <v>1076</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="229" t="s">
+      <c r="B11" s="216" t="s">
         <v>1077</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="229" t="s">
+      <c r="B12" s="216" t="s">
         <v>1078</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="229" t="s">
+      <c r="B13" s="216" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="229" t="s">
+      <c r="B14" s="216" t="s">
         <v>1080</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" s="229" t="s">
+      <c r="B15" s="216" t="s">
         <v>1081</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B16" s="229" t="s">
+      <c r="B16" s="216" t="s">
         <v>1082</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="229" t="s">
+      <c r="B17" s="216" t="s">
         <v>1083</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="229" t="s">
+      <c r="B18" s="216" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="229" t="s">
+      <c r="B19" s="216" t="s">
         <v>1085</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="229" t="s">
+      <c r="B20" s="216" t="s">
         <v>1086</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="229" t="s">
+      <c r="B21" s="216" t="s">
         <v>1087</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="229" t="s">
+      <c r="B22" s="216" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="229" t="s">
+      <c r="B23" s="216" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="229" t="s">
+      <c r="B24" s="216" t="s">
         <v>1090</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="229" t="s">
+      <c r="B25" s="216" t="s">
         <v>1091</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="229" t="s">
+      <c r="B26" s="216" t="s">
         <v>1092</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="229" t="s">
+      <c r="B27" s="216" t="s">
         <v>1093</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" s="229" t="s">
+      <c r="B28" s="216" t="s">
         <v>1094</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="229" t="s">
+      <c r="B29" s="216" t="s">
         <v>1095</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B30" s="229" t="s">
+      <c r="B30" s="216" t="s">
         <v>1096</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B31" s="229" t="s">
+      <c r="B31" s="216" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="229" t="s">
+      <c r="B32" s="216" t="s">
         <v>1098</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="229" t="s">
+      <c r="B33" s="216" t="s">
         <v>1099</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="229" t="s">
+      <c r="B34" s="216" t="s">
         <v>1100</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="229" t="s">
+      <c r="B35" s="216" t="s">
         <v>1101</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="229" t="s">
+      <c r="B36" s="216" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" s="229" t="s">
+      <c r="B37" s="216" t="s">
         <v>1103</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" s="229" t="s">
+      <c r="B38" s="216" t="s">
         <v>1104</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="229" t="s">
+      <c r="B39" s="216" t="s">
         <v>1105</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" s="229" t="s">
+      <c r="B40" s="216" t="s">
         <v>1106</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" s="229" t="s">
+      <c r="B41" s="216" t="s">
         <v>1107</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B42" s="229" t="s">
+      <c r="B42" s="216" t="s">
         <v>1108</v>
       </c>
     </row>
@@ -30101,45 +30064,45 @@
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="217" t="s">
+      <c r="A142" s="229" t="s">
         <v>426</v>
       </c>
-      <c r="B142" s="217"/>
-      <c r="C142" s="217"/>
-      <c r="D142" s="217"/>
-      <c r="E142" s="217"/>
-      <c r="F142" s="217"/>
-      <c r="G142" s="217"/>
-      <c r="H142" s="217"/>
-      <c r="I142" s="217"/>
-      <c r="J142" s="217"/>
-      <c r="K142" s="217"/>
+      <c r="B142" s="229"/>
+      <c r="C142" s="229"/>
+      <c r="D142" s="229"/>
+      <c r="E142" s="229"/>
+      <c r="F142" s="229"/>
+      <c r="G142" s="229"/>
+      <c r="H142" s="229"/>
+      <c r="I142" s="229"/>
+      <c r="J142" s="229"/>
+      <c r="K142" s="229"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A143" s="217"/>
-      <c r="B143" s="217"/>
-      <c r="C143" s="217"/>
-      <c r="D143" s="217"/>
-      <c r="E143" s="217"/>
-      <c r="F143" s="217"/>
-      <c r="G143" s="217"/>
-      <c r="H143" s="217"/>
-      <c r="I143" s="217"/>
-      <c r="J143" s="217"/>
-      <c r="K143" s="217"/>
+      <c r="A143" s="229"/>
+      <c r="B143" s="229"/>
+      <c r="C143" s="229"/>
+      <c r="D143" s="229"/>
+      <c r="E143" s="229"/>
+      <c r="F143" s="229"/>
+      <c r="G143" s="229"/>
+      <c r="H143" s="229"/>
+      <c r="I143" s="229"/>
+      <c r="J143" s="229"/>
+      <c r="K143" s="229"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A144" s="217"/>
-      <c r="B144" s="217"/>
-      <c r="C144" s="217"/>
-      <c r="D144" s="217"/>
-      <c r="E144" s="217"/>
-      <c r="F144" s="217"/>
-      <c r="G144" s="217"/>
-      <c r="H144" s="217"/>
-      <c r="I144" s="217"/>
-      <c r="J144" s="217"/>
-      <c r="K144" s="217"/>
+      <c r="A144" s="229"/>
+      <c r="B144" s="229"/>
+      <c r="C144" s="229"/>
+      <c r="D144" s="229"/>
+      <c r="E144" s="229"/>
+      <c r="F144" s="229"/>
+      <c r="G144" s="229"/>
+      <c r="H144" s="229"/>
+      <c r="I144" s="229"/>
+      <c r="J144" s="229"/>
+      <c r="K144" s="229"/>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="90" t="s">
@@ -30147,45 +30110,45 @@
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A147" s="217" t="s">
+      <c r="A147" s="229" t="s">
         <v>427</v>
       </c>
-      <c r="B147" s="217"/>
-      <c r="C147" s="217"/>
-      <c r="D147" s="217"/>
-      <c r="E147" s="217"/>
-      <c r="F147" s="217"/>
-      <c r="G147" s="217"/>
-      <c r="H147" s="217"/>
-      <c r="I147" s="217"/>
-      <c r="J147" s="217"/>
-      <c r="K147" s="217"/>
+      <c r="B147" s="229"/>
+      <c r="C147" s="229"/>
+      <c r="D147" s="229"/>
+      <c r="E147" s="229"/>
+      <c r="F147" s="229"/>
+      <c r="G147" s="229"/>
+      <c r="H147" s="229"/>
+      <c r="I147" s="229"/>
+      <c r="J147" s="229"/>
+      <c r="K147" s="229"/>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A148" s="217"/>
-      <c r="B148" s="217"/>
-      <c r="C148" s="217"/>
-      <c r="D148" s="217"/>
-      <c r="E148" s="217"/>
-      <c r="F148" s="217"/>
-      <c r="G148" s="217"/>
-      <c r="H148" s="217"/>
-      <c r="I148" s="217"/>
-      <c r="J148" s="217"/>
-      <c r="K148" s="217"/>
+      <c r="A148" s="229"/>
+      <c r="B148" s="229"/>
+      <c r="C148" s="229"/>
+      <c r="D148" s="229"/>
+      <c r="E148" s="229"/>
+      <c r="F148" s="229"/>
+      <c r="G148" s="229"/>
+      <c r="H148" s="229"/>
+      <c r="I148" s="229"/>
+      <c r="J148" s="229"/>
+      <c r="K148" s="229"/>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A149" s="217"/>
-      <c r="B149" s="217"/>
-      <c r="C149" s="217"/>
-      <c r="D149" s="217"/>
-      <c r="E149" s="217"/>
-      <c r="F149" s="217"/>
-      <c r="G149" s="217"/>
-      <c r="H149" s="217"/>
-      <c r="I149" s="217"/>
-      <c r="J149" s="217"/>
-      <c r="K149" s="217"/>
+      <c r="A149" s="229"/>
+      <c r="B149" s="229"/>
+      <c r="C149" s="229"/>
+      <c r="D149" s="229"/>
+      <c r="E149" s="229"/>
+      <c r="F149" s="229"/>
+      <c r="G149" s="229"/>
+      <c r="H149" s="229"/>
+      <c r="I149" s="229"/>
+      <c r="J149" s="229"/>
+      <c r="K149" s="229"/>
     </row>
     <row r="150" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F150" s="71" t="s">
@@ -30616,18 +30579,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="228" t="s">
+      <c r="A1" s="240" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="228"/>
-      <c r="C1" s="228"/>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
-      <c r="I1" s="228"/>
-      <c r="J1" s="228"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
       <c r="K1" s="34"/>
       <c r="L1" s="34"/>
       <c r="M1" s="34"/>
@@ -31044,121 +31007,121 @@
       <c r="A23" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="C23" s="227" t="s">
+      <c r="C23" s="239" t="s">
         <v>230</v>
       </c>
-      <c r="D23" s="227"/>
-      <c r="E23" s="227"/>
-      <c r="F23" s="227"/>
-      <c r="G23" s="227"/>
-      <c r="H23" s="227"/>
-      <c r="I23" s="227"/>
-      <c r="J23" s="227"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="239"/>
+      <c r="F23" s="239"/>
+      <c r="G23" s="239"/>
+      <c r="H23" s="239"/>
+      <c r="I23" s="239"/>
+      <c r="J23" s="239"/>
     </row>
     <row r="24" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="227" t="s">
+      <c r="C24" s="239" t="s">
         <v>223</v>
       </c>
-      <c r="D24" s="227"/>
-      <c r="E24" s="227"/>
-      <c r="F24" s="227"/>
-      <c r="G24" s="227"/>
-      <c r="H24" s="227"/>
-      <c r="I24" s="227"/>
-      <c r="J24" s="227"/>
+      <c r="D24" s="239"/>
+      <c r="E24" s="239"/>
+      <c r="F24" s="239"/>
+      <c r="G24" s="239"/>
+      <c r="H24" s="239"/>
+      <c r="I24" s="239"/>
+      <c r="J24" s="239"/>
     </row>
     <row r="25" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C25" s="227" t="s">
+      <c r="C25" s="239" t="s">
         <v>224</v>
       </c>
-      <c r="D25" s="227"/>
-      <c r="E25" s="227"/>
-      <c r="F25" s="227"/>
-      <c r="G25" s="227"/>
-      <c r="H25" s="227"/>
-      <c r="I25" s="227"/>
-      <c r="J25" s="227"/>
+      <c r="D25" s="239"/>
+      <c r="E25" s="239"/>
+      <c r="F25" s="239"/>
+      <c r="G25" s="239"/>
+      <c r="H25" s="239"/>
+      <c r="I25" s="239"/>
+      <c r="J25" s="239"/>
     </row>
     <row r="26" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C26" s="227" t="s">
+      <c r="C26" s="239" t="s">
         <v>225</v>
       </c>
-      <c r="D26" s="227"/>
-      <c r="E26" s="227"/>
-      <c r="F26" s="227"/>
-      <c r="G26" s="227"/>
-      <c r="H26" s="227"/>
-      <c r="I26" s="227"/>
-      <c r="J26" s="227"/>
+      <c r="D26" s="239"/>
+      <c r="E26" s="239"/>
+      <c r="F26" s="239"/>
+      <c r="G26" s="239"/>
+      <c r="H26" s="239"/>
+      <c r="I26" s="239"/>
+      <c r="J26" s="239"/>
     </row>
     <row r="27" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="C27" s="227" t="s">
+      <c r="C27" s="239" t="s">
         <v>226</v>
       </c>
-      <c r="D27" s="227"/>
-      <c r="E27" s="227"/>
-      <c r="F27" s="227"/>
-      <c r="G27" s="227"/>
-      <c r="H27" s="227"/>
-      <c r="I27" s="227"/>
-      <c r="J27" s="227"/>
+      <c r="D27" s="239"/>
+      <c r="E27" s="239"/>
+      <c r="F27" s="239"/>
+      <c r="G27" s="239"/>
+      <c r="H27" s="239"/>
+      <c r="I27" s="239"/>
+      <c r="J27" s="239"/>
     </row>
     <row r="28" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="C28" s="227" t="s">
+      <c r="C28" s="239" t="s">
         <v>227</v>
       </c>
-      <c r="D28" s="227"/>
-      <c r="E28" s="227"/>
-      <c r="F28" s="227"/>
-      <c r="G28" s="227"/>
-      <c r="H28" s="227"/>
-      <c r="I28" s="227"/>
-      <c r="J28" s="227"/>
+      <c r="D28" s="239"/>
+      <c r="E28" s="239"/>
+      <c r="F28" s="239"/>
+      <c r="G28" s="239"/>
+      <c r="H28" s="239"/>
+      <c r="I28" s="239"/>
+      <c r="J28" s="239"/>
     </row>
     <row r="29" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="C29" s="227" t="s">
+      <c r="C29" s="239" t="s">
         <v>234</v>
       </c>
-      <c r="D29" s="227"/>
-      <c r="E29" s="227"/>
-      <c r="F29" s="227"/>
-      <c r="G29" s="227"/>
-      <c r="H29" s="227"/>
-      <c r="I29" s="227"/>
-      <c r="J29" s="227"/>
+      <c r="D29" s="239"/>
+      <c r="E29" s="239"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="239"/>
+      <c r="H29" s="239"/>
+      <c r="I29" s="239"/>
+      <c r="J29" s="239"/>
     </row>
     <row r="30" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="C30" s="227" t="s">
+      <c r="C30" s="239" t="s">
         <v>233</v>
       </c>
-      <c r="D30" s="227"/>
-      <c r="E30" s="227"/>
-      <c r="F30" s="227"/>
-      <c r="G30" s="227"/>
-      <c r="H30" s="227"/>
-      <c r="I30" s="227"/>
-      <c r="J30" s="227"/>
+      <c r="D30" s="239"/>
+      <c r="E30" s="239"/>
+      <c r="F30" s="239"/>
+      <c r="G30" s="239"/>
+      <c r="H30" s="239"/>
+      <c r="I30" s="239"/>
+      <c r="J30" s="239"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31"/>
@@ -32990,7 +32953,7 @@
       </c>
       <c r="J1" s="100"/>
       <c r="K1" s="61"/>
-      <c r="L1" s="242" t="s">
+      <c r="L1" s="223" t="s">
         <v>1205</v>
       </c>
     </row>
@@ -33019,7 +32982,7 @@
       <c r="B4" s="57" t="s">
         <v>1040</v>
       </c>
-      <c r="H4" s="243" t="s">
+      <c r="H4" s="224" t="s">
         <v>1210</v>
       </c>
     </row>
@@ -33530,18 +33493,15 @@
       <c r="L32" s="54"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="233" t="s">
+      <c r="A33" s="57" t="s">
         <v>320</v>
       </c>
-      <c r="B33" s="234">
+      <c r="B33" s="54">
         <v>1</v>
       </c>
-      <c r="C33" s="240" t="s">
+      <c r="C33" s="80" t="s">
         <v>1042</v>
       </c>
-      <c r="D33" s="233"/>
-      <c r="E33" s="233"/>
-      <c r="F33" s="233"/>
       <c r="H33" s="63" t="s">
         <v>66</v>
       </c>
@@ -33999,7 +33959,7 @@
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="241"/>
+      <c r="A66" s="222"/>
       <c r="B66" s="66"/>
       <c r="C66" s="69"/>
       <c r="D66" s="82"/>
@@ -34018,7 +33978,7 @@
       <c r="D67" s="80"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="241"/>
+      <c r="A68" s="222"/>
       <c r="B68" s="66"/>
       <c r="C68" s="69"/>
       <c r="D68" s="82"/>
@@ -34203,7 +34163,7 @@
       <c r="A86" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="C86" s="235">
+      <c r="C86" s="219">
         <v>26373</v>
       </c>
       <c r="E86" s="80" t="s">
@@ -34281,62 +34241,62 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="216" t="s">
+      <c r="A93" s="227" t="s">
         <v>1246</v>
       </c>
-      <c r="B93" s="216"/>
-      <c r="C93" s="216"/>
-      <c r="D93" s="216"/>
-      <c r="E93" s="216"/>
-      <c r="F93" s="216"/>
-      <c r="G93" s="216"/>
-      <c r="H93" s="216"/>
-      <c r="I93" s="216"/>
-      <c r="J93" s="216"/>
-      <c r="K93" s="216"/>
-      <c r="L93" s="216"/>
+      <c r="B93" s="227"/>
+      <c r="C93" s="227"/>
+      <c r="D93" s="227"/>
+      <c r="E93" s="227"/>
+      <c r="F93" s="227"/>
+      <c r="G93" s="227"/>
+      <c r="H93" s="227"/>
+      <c r="I93" s="227"/>
+      <c r="J93" s="227"/>
+      <c r="K93" s="227"/>
+      <c r="L93" s="227"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="216"/>
-      <c r="B94" s="216"/>
-      <c r="C94" s="216"/>
-      <c r="D94" s="216"/>
-      <c r="E94" s="216"/>
-      <c r="F94" s="216"/>
-      <c r="G94" s="216"/>
-      <c r="H94" s="216"/>
-      <c r="I94" s="216"/>
-      <c r="J94" s="216"/>
-      <c r="K94" s="216"/>
-      <c r="L94" s="216"/>
+      <c r="A94" s="227"/>
+      <c r="B94" s="227"/>
+      <c r="C94" s="227"/>
+      <c r="D94" s="227"/>
+      <c r="E94" s="227"/>
+      <c r="F94" s="227"/>
+      <c r="G94" s="227"/>
+      <c r="H94" s="227"/>
+      <c r="I94" s="227"/>
+      <c r="J94" s="227"/>
+      <c r="K94" s="227"/>
+      <c r="L94" s="227"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="216"/>
-      <c r="B95" s="216"/>
-      <c r="C95" s="216"/>
-      <c r="D95" s="216"/>
-      <c r="E95" s="216"/>
-      <c r="F95" s="216"/>
-      <c r="G95" s="216"/>
-      <c r="H95" s="216"/>
-      <c r="I95" s="216"/>
-      <c r="J95" s="216"/>
-      <c r="K95" s="216"/>
-      <c r="L95" s="216"/>
+      <c r="A95" s="227"/>
+      <c r="B95" s="227"/>
+      <c r="C95" s="227"/>
+      <c r="D95" s="227"/>
+      <c r="E95" s="227"/>
+      <c r="F95" s="227"/>
+      <c r="G95" s="227"/>
+      <c r="H95" s="227"/>
+      <c r="I95" s="227"/>
+      <c r="J95" s="227"/>
+      <c r="K95" s="227"/>
+      <c r="L95" s="227"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="216"/>
-      <c r="B96" s="216"/>
-      <c r="C96" s="216"/>
-      <c r="D96" s="216"/>
-      <c r="E96" s="216"/>
-      <c r="F96" s="216"/>
-      <c r="G96" s="216"/>
-      <c r="H96" s="216"/>
-      <c r="I96" s="216"/>
-      <c r="J96" s="216"/>
-      <c r="K96" s="216"/>
-      <c r="L96" s="216"/>
+      <c r="A96" s="227"/>
+      <c r="B96" s="227"/>
+      <c r="C96" s="227"/>
+      <c r="D96" s="227"/>
+      <c r="E96" s="227"/>
+      <c r="F96" s="227"/>
+      <c r="G96" s="227"/>
+      <c r="H96" s="227"/>
+      <c r="I96" s="227"/>
+      <c r="J96" s="227"/>
+      <c r="K96" s="227"/>
+      <c r="L96" s="227"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="90" t="s">
@@ -34344,48 +34304,48 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="237" t="s">
+      <c r="A98" s="228" t="s">
         <v>1247</v>
       </c>
-      <c r="B98" s="237"/>
-      <c r="C98" s="237"/>
-      <c r="D98" s="237"/>
-      <c r="E98" s="237"/>
-      <c r="F98" s="237"/>
-      <c r="G98" s="237"/>
-      <c r="H98" s="237"/>
-      <c r="I98" s="237"/>
-      <c r="J98" s="237"/>
-      <c r="K98" s="237"/>
-      <c r="L98" s="237"/>
+      <c r="B98" s="228"/>
+      <c r="C98" s="228"/>
+      <c r="D98" s="228"/>
+      <c r="E98" s="228"/>
+      <c r="F98" s="228"/>
+      <c r="G98" s="228"/>
+      <c r="H98" s="228"/>
+      <c r="I98" s="228"/>
+      <c r="J98" s="228"/>
+      <c r="K98" s="228"/>
+      <c r="L98" s="228"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="237"/>
-      <c r="B99" s="237"/>
-      <c r="C99" s="237"/>
-      <c r="D99" s="237"/>
-      <c r="E99" s="237"/>
-      <c r="F99" s="237"/>
-      <c r="G99" s="237"/>
-      <c r="H99" s="237"/>
-      <c r="I99" s="237"/>
-      <c r="J99" s="237"/>
-      <c r="K99" s="237"/>
-      <c r="L99" s="237"/>
+      <c r="A99" s="228"/>
+      <c r="B99" s="228"/>
+      <c r="C99" s="228"/>
+      <c r="D99" s="228"/>
+      <c r="E99" s="228"/>
+      <c r="F99" s="228"/>
+      <c r="G99" s="228"/>
+      <c r="H99" s="228"/>
+      <c r="I99" s="228"/>
+      <c r="J99" s="228"/>
+      <c r="K99" s="228"/>
+      <c r="L99" s="228"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="237"/>
-      <c r="B100" s="237"/>
-      <c r="C100" s="237"/>
-      <c r="D100" s="237"/>
-      <c r="E100" s="237"/>
-      <c r="F100" s="237"/>
-      <c r="G100" s="237"/>
-      <c r="H100" s="237"/>
-      <c r="I100" s="237"/>
-      <c r="J100" s="237"/>
-      <c r="K100" s="237"/>
-      <c r="L100" s="237"/>
+      <c r="A100" s="228"/>
+      <c r="B100" s="228"/>
+      <c r="C100" s="228"/>
+      <c r="D100" s="228"/>
+      <c r="E100" s="228"/>
+      <c r="F100" s="228"/>
+      <c r="G100" s="228"/>
+      <c r="H100" s="228"/>
+      <c r="I100" s="228"/>
+      <c r="J100" s="228"/>
+      <c r="K100" s="228"/>
+      <c r="L100" s="228"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
@@ -34407,70 +34367,46 @@
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="240" t="s">
+      <c r="A103" s="80" t="s">
         <v>407</v>
       </c>
-      <c r="B103" s="233"/>
-      <c r="C103" s="245">
+      <c r="C103" s="167">
         <v>1</v>
       </c>
-      <c r="D103" s="247" t="s">
+      <c r="D103" s="226" t="s">
         <v>1068</v>
       </c>
-      <c r="E103" s="240" t="s">
+      <c r="E103" s="80" t="s">
         <v>483</v>
       </c>
-      <c r="F103" s="233"/>
-      <c r="G103" s="233"/>
-      <c r="H103" s="233"/>
-      <c r="I103" s="233"/>
-      <c r="J103" s="233"/>
-      <c r="K103" s="234"/>
-      <c r="L103" s="233"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="240" t="s">
+      <c r="A104" s="80" t="s">
         <v>1229</v>
       </c>
-      <c r="B104" s="233"/>
-      <c r="C104" s="245" t="s">
+      <c r="C104" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="D104" s="247" t="s">
+      <c r="D104" s="226" t="s">
         <v>1071</v>
       </c>
-      <c r="E104" s="240" t="s">
+      <c r="E104" s="80" t="s">
         <v>1230</v>
       </c>
-      <c r="F104" s="233"/>
-      <c r="G104" s="233"/>
-      <c r="H104" s="233"/>
-      <c r="I104" s="233"/>
-      <c r="J104" s="233"/>
-      <c r="K104" s="234"/>
-      <c r="L104" s="233"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A105" s="240" t="s">
+      <c r="A105" s="80" t="s">
         <v>1231</v>
       </c>
-      <c r="B105" s="233"/>
-      <c r="C105" s="245" t="s">
+      <c r="C105" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="D105" s="247" t="s">
+      <c r="D105" s="226" t="s">
         <v>1128</v>
       </c>
-      <c r="E105" s="240" t="s">
+      <c r="E105" s="80" t="s">
         <v>1232</v>
       </c>
-      <c r="F105" s="233"/>
-      <c r="G105" s="233"/>
-      <c r="H105" s="233"/>
-      <c r="I105" s="233"/>
-      <c r="J105" s="233"/>
-      <c r="K105" s="234"/>
-      <c r="L105" s="233"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D106" s="133"/>
@@ -34646,14 +34582,14 @@
       <c r="C126" s="155" t="s">
         <v>1225</v>
       </c>
-      <c r="D126" s="244" t="s">
+      <c r="D126" s="225" t="s">
         <v>1226</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="100"/>
       <c r="B127" s="100"/>
-      <c r="C127" s="231"/>
+      <c r="C127" s="218"/>
       <c r="D127" s="100"/>
       <c r="E127" s="61"/>
       <c r="F127" s="61"/>
@@ -35254,7 +35190,7 @@
       <c r="B4" s="57" t="s">
         <v>1040</v>
       </c>
-      <c r="H4" s="230" t="s">
+      <c r="H4" s="217" t="s">
         <v>1155</v>
       </c>
     </row>
@@ -35731,7 +35667,7 @@
       <c r="L30" s="54"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="238" t="s">
+      <c r="A31" s="221" t="s">
         <v>1166</v>
       </c>
       <c r="B31" s="54">
@@ -35752,7 +35688,7 @@
       <c r="L31" s="54"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="238" t="s">
+      <c r="A32" s="221" t="s">
         <v>1166</v>
       </c>
       <c r="B32" s="54">
@@ -35770,14 +35706,10 @@
       <c r="L32" s="54"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="233"/>
-      <c r="B33" s="234"/>
-      <c r="C33" s="240" t="s">
+      <c r="B33" s="54"/>
+      <c r="C33" s="80" t="s">
         <v>1169</v>
       </c>
-      <c r="D33" s="233"/>
-      <c r="E33" s="233"/>
-      <c r="F33" s="233"/>
       <c r="H33" s="63" t="s">
         <v>66</v>
       </c>
@@ -36218,7 +36150,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="63"/>
-      <c r="D64" s="238" t="s">
+      <c r="D64" s="221" t="s">
         <v>1186</v>
       </c>
     </row>
@@ -36229,7 +36161,7 @@
       <c r="C65" s="54">
         <v>-3</v>
       </c>
-      <c r="D65" s="238" t="s">
+      <c r="D65" s="221" t="s">
         <v>1185</v>
       </c>
     </row>
@@ -36239,7 +36171,7 @@
       <c r="D66" s="80"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="241"/>
+      <c r="A67" s="222"/>
       <c r="B67" s="66"/>
       <c r="C67" s="69"/>
       <c r="D67" s="82"/>
@@ -36253,7 +36185,7 @@
       <c r="L67" s="66"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="241"/>
+      <c r="A68" s="222"/>
       <c r="B68" s="66"/>
       <c r="C68" s="69"/>
       <c r="D68" s="82"/>
@@ -36426,7 +36358,7 @@
         <v>119</v>
       </c>
       <c r="F85" s="66"/>
-      <c r="G85" s="236" t="s">
+      <c r="G85" s="220" t="s">
         <v>392</v>
       </c>
       <c r="I85" s="66"/>
@@ -36516,62 +36448,62 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="237" t="s">
+      <c r="A93" s="228" t="s">
         <v>1198</v>
       </c>
-      <c r="B93" s="237"/>
-      <c r="C93" s="237"/>
-      <c r="D93" s="237"/>
-      <c r="E93" s="237"/>
-      <c r="F93" s="237"/>
-      <c r="G93" s="237"/>
-      <c r="H93" s="237"/>
-      <c r="I93" s="237"/>
-      <c r="J93" s="237"/>
-      <c r="K93" s="237"/>
-      <c r="L93" s="237"/>
+      <c r="B93" s="228"/>
+      <c r="C93" s="228"/>
+      <c r="D93" s="228"/>
+      <c r="E93" s="228"/>
+      <c r="F93" s="228"/>
+      <c r="G93" s="228"/>
+      <c r="H93" s="228"/>
+      <c r="I93" s="228"/>
+      <c r="J93" s="228"/>
+      <c r="K93" s="228"/>
+      <c r="L93" s="228"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="237"/>
-      <c r="B94" s="237"/>
-      <c r="C94" s="237"/>
-      <c r="D94" s="237"/>
-      <c r="E94" s="237"/>
-      <c r="F94" s="237"/>
-      <c r="G94" s="237"/>
-      <c r="H94" s="237"/>
-      <c r="I94" s="237"/>
-      <c r="J94" s="237"/>
-      <c r="K94" s="237"/>
-      <c r="L94" s="237"/>
+      <c r="A94" s="228"/>
+      <c r="B94" s="228"/>
+      <c r="C94" s="228"/>
+      <c r="D94" s="228"/>
+      <c r="E94" s="228"/>
+      <c r="F94" s="228"/>
+      <c r="G94" s="228"/>
+      <c r="H94" s="228"/>
+      <c r="I94" s="228"/>
+      <c r="J94" s="228"/>
+      <c r="K94" s="228"/>
+      <c r="L94" s="228"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="237"/>
-      <c r="B95" s="237"/>
-      <c r="C95" s="237"/>
-      <c r="D95" s="237"/>
-      <c r="E95" s="237"/>
-      <c r="F95" s="237"/>
-      <c r="G95" s="237"/>
-      <c r="H95" s="237"/>
-      <c r="I95" s="237"/>
-      <c r="J95" s="237"/>
-      <c r="K95" s="237"/>
-      <c r="L95" s="237"/>
+      <c r="A95" s="228"/>
+      <c r="B95" s="228"/>
+      <c r="C95" s="228"/>
+      <c r="D95" s="228"/>
+      <c r="E95" s="228"/>
+      <c r="F95" s="228"/>
+      <c r="G95" s="228"/>
+      <c r="H95" s="228"/>
+      <c r="I95" s="228"/>
+      <c r="J95" s="228"/>
+      <c r="K95" s="228"/>
+      <c r="L95" s="228"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="237"/>
-      <c r="B96" s="237"/>
-      <c r="C96" s="237"/>
-      <c r="D96" s="237"/>
-      <c r="E96" s="237"/>
-      <c r="F96" s="237"/>
-      <c r="G96" s="237"/>
-      <c r="H96" s="237"/>
-      <c r="I96" s="237"/>
-      <c r="J96" s="237"/>
-      <c r="K96" s="237"/>
-      <c r="L96" s="237"/>
+      <c r="A96" s="228"/>
+      <c r="B96" s="228"/>
+      <c r="C96" s="228"/>
+      <c r="D96" s="228"/>
+      <c r="E96" s="228"/>
+      <c r="F96" s="228"/>
+      <c r="G96" s="228"/>
+      <c r="H96" s="228"/>
+      <c r="I96" s="228"/>
+      <c r="J96" s="228"/>
+      <c r="K96" s="228"/>
+      <c r="L96" s="228"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="90" t="s">
@@ -36579,48 +36511,48 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="216" t="s">
+      <c r="A98" s="227" t="s">
         <v>1202</v>
       </c>
-      <c r="B98" s="216"/>
-      <c r="C98" s="216"/>
-      <c r="D98" s="216"/>
-      <c r="E98" s="216"/>
-      <c r="F98" s="216"/>
-      <c r="G98" s="216"/>
-      <c r="H98" s="216"/>
-      <c r="I98" s="216"/>
-      <c r="J98" s="216"/>
-      <c r="K98" s="216"/>
-      <c r="L98" s="216"/>
+      <c r="B98" s="227"/>
+      <c r="C98" s="227"/>
+      <c r="D98" s="227"/>
+      <c r="E98" s="227"/>
+      <c r="F98" s="227"/>
+      <c r="G98" s="227"/>
+      <c r="H98" s="227"/>
+      <c r="I98" s="227"/>
+      <c r="J98" s="227"/>
+      <c r="K98" s="227"/>
+      <c r="L98" s="227"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="216"/>
-      <c r="B99" s="216"/>
-      <c r="C99" s="216"/>
-      <c r="D99" s="216"/>
-      <c r="E99" s="216"/>
-      <c r="F99" s="216"/>
-      <c r="G99" s="216"/>
-      <c r="H99" s="216"/>
-      <c r="I99" s="216"/>
-      <c r="J99" s="216"/>
-      <c r="K99" s="216"/>
-      <c r="L99" s="216"/>
+      <c r="A99" s="227"/>
+      <c r="B99" s="227"/>
+      <c r="C99" s="227"/>
+      <c r="D99" s="227"/>
+      <c r="E99" s="227"/>
+      <c r="F99" s="227"/>
+      <c r="G99" s="227"/>
+      <c r="H99" s="227"/>
+      <c r="I99" s="227"/>
+      <c r="J99" s="227"/>
+      <c r="K99" s="227"/>
+      <c r="L99" s="227"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="216"/>
-      <c r="B100" s="216"/>
-      <c r="C100" s="216"/>
-      <c r="D100" s="216"/>
-      <c r="E100" s="216"/>
-      <c r="F100" s="216"/>
-      <c r="G100" s="216"/>
-      <c r="H100" s="216"/>
-      <c r="I100" s="216"/>
-      <c r="J100" s="216"/>
-      <c r="K100" s="216"/>
-      <c r="L100" s="216"/>
+      <c r="A100" s="227"/>
+      <c r="B100" s="227"/>
+      <c r="C100" s="227"/>
+      <c r="D100" s="227"/>
+      <c r="E100" s="227"/>
+      <c r="F100" s="227"/>
+      <c r="G100" s="227"/>
+      <c r="H100" s="227"/>
+      <c r="I100" s="227"/>
+      <c r="J100" s="227"/>
+      <c r="K100" s="227"/>
+      <c r="L100" s="227"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
@@ -36642,48 +36574,32 @@
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="240" t="s">
+      <c r="A103" s="80" t="s">
         <v>407</v>
       </c>
-      <c r="B103" s="233"/>
-      <c r="C103" s="245">
+      <c r="C103" s="167">
         <v>1</v>
       </c>
-      <c r="D103" s="247" t="s">
+      <c r="D103" s="226" t="s">
         <v>1068</v>
       </c>
-      <c r="E103" s="240" t="s">
+      <c r="E103" s="80" t="s">
         <v>483</v>
       </c>
-      <c r="F103" s="233"/>
-      <c r="G103" s="233"/>
-      <c r="H103" s="233"/>
-      <c r="I103" s="233"/>
-      <c r="J103" s="233"/>
-      <c r="K103" s="234"/>
-      <c r="L103" s="233"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="240" t="s">
+      <c r="A104" s="80" t="s">
         <v>1183</v>
       </c>
-      <c r="B104" s="233"/>
-      <c r="C104" s="245" t="s">
+      <c r="C104" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="D104" s="247" t="s">
+      <c r="D104" s="226" t="s">
         <v>1071</v>
       </c>
-      <c r="E104" s="246" t="s">
+      <c r="E104" s="221" t="s">
         <v>1184</v>
       </c>
-      <c r="F104" s="233"/>
-      <c r="G104" s="233"/>
-      <c r="H104" s="233"/>
-      <c r="I104" s="233"/>
-      <c r="J104" s="233"/>
-      <c r="K104" s="234"/>
-      <c r="L104" s="233"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="61"/>
@@ -36854,44 +36770,28 @@
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A125" s="232" t="s">
+      <c r="A125" s="63" t="s">
         <v>1178</v>
       </c>
-      <c r="B125" s="232"/>
-      <c r="C125" s="239" t="s">
+      <c r="B125" s="63"/>
+      <c r="C125" s="155" t="s">
         <v>1179</v>
       </c>
-      <c r="D125" s="240" t="s">
+      <c r="D125" s="80" t="s">
         <v>1180</v>
       </c>
-      <c r="E125" s="233"/>
-      <c r="F125" s="233"/>
-      <c r="G125" s="233"/>
-      <c r="H125" s="233"/>
-      <c r="I125" s="233"/>
-      <c r="J125" s="233"/>
-      <c r="K125" s="234"/>
-      <c r="L125" s="233"/>
     </row>
     <row r="126" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="232" t="s">
+      <c r="A126" s="63" t="s">
         <v>1181</v>
       </c>
-      <c r="B126" s="232"/>
-      <c r="C126" s="239" t="s">
+      <c r="B126" s="63"/>
+      <c r="C126" s="155" t="s">
         <v>1179</v>
       </c>
-      <c r="D126" s="232" t="s">
+      <c r="D126" s="63" t="s">
         <v>1182</v>
       </c>
-      <c r="E126" s="233"/>
-      <c r="F126" s="233"/>
-      <c r="G126" s="233"/>
-      <c r="H126" s="233"/>
-      <c r="I126" s="233"/>
-      <c r="J126" s="233"/>
-      <c r="K126" s="234"/>
-      <c r="L126" s="233"/>
     </row>
     <row r="127" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="100"/>
@@ -38675,7 +38575,7 @@
       <c r="A86" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="C86" s="235">
+      <c r="C86" s="219">
         <v>36047</v>
       </c>
       <c r="E86" s="80" t="s">
@@ -38753,62 +38653,62 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="216" t="s">
+      <c r="A93" s="227" t="s">
         <v>1045</v>
       </c>
-      <c r="B93" s="216"/>
-      <c r="C93" s="216"/>
-      <c r="D93" s="216"/>
-      <c r="E93" s="216"/>
-      <c r="F93" s="216"/>
-      <c r="G93" s="216"/>
-      <c r="H93" s="216"/>
-      <c r="I93" s="216"/>
-      <c r="J93" s="216"/>
-      <c r="K93" s="216"/>
-      <c r="L93" s="216"/>
+      <c r="B93" s="227"/>
+      <c r="C93" s="227"/>
+      <c r="D93" s="227"/>
+      <c r="E93" s="227"/>
+      <c r="F93" s="227"/>
+      <c r="G93" s="227"/>
+      <c r="H93" s="227"/>
+      <c r="I93" s="227"/>
+      <c r="J93" s="227"/>
+      <c r="K93" s="227"/>
+      <c r="L93" s="227"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="216"/>
-      <c r="B94" s="216"/>
-      <c r="C94" s="216"/>
-      <c r="D94" s="216"/>
-      <c r="E94" s="216"/>
-      <c r="F94" s="216"/>
-      <c r="G94" s="216"/>
-      <c r="H94" s="216"/>
-      <c r="I94" s="216"/>
-      <c r="J94" s="216"/>
-      <c r="K94" s="216"/>
-      <c r="L94" s="216"/>
+      <c r="A94" s="227"/>
+      <c r="B94" s="227"/>
+      <c r="C94" s="227"/>
+      <c r="D94" s="227"/>
+      <c r="E94" s="227"/>
+      <c r="F94" s="227"/>
+      <c r="G94" s="227"/>
+      <c r="H94" s="227"/>
+      <c r="I94" s="227"/>
+      <c r="J94" s="227"/>
+      <c r="K94" s="227"/>
+      <c r="L94" s="227"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="216"/>
-      <c r="B95" s="216"/>
-      <c r="C95" s="216"/>
-      <c r="D95" s="216"/>
-      <c r="E95" s="216"/>
-      <c r="F95" s="216"/>
-      <c r="G95" s="216"/>
-      <c r="H95" s="216"/>
-      <c r="I95" s="216"/>
-      <c r="J95" s="216"/>
-      <c r="K95" s="216"/>
-      <c r="L95" s="216"/>
+      <c r="A95" s="227"/>
+      <c r="B95" s="227"/>
+      <c r="C95" s="227"/>
+      <c r="D95" s="227"/>
+      <c r="E95" s="227"/>
+      <c r="F95" s="227"/>
+      <c r="G95" s="227"/>
+      <c r="H95" s="227"/>
+      <c r="I95" s="227"/>
+      <c r="J95" s="227"/>
+      <c r="K95" s="227"/>
+      <c r="L95" s="227"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="216"/>
-      <c r="B96" s="216"/>
-      <c r="C96" s="216"/>
-      <c r="D96" s="216"/>
-      <c r="E96" s="216"/>
-      <c r="F96" s="216"/>
-      <c r="G96" s="216"/>
-      <c r="H96" s="216"/>
-      <c r="I96" s="216"/>
-      <c r="J96" s="216"/>
-      <c r="K96" s="216"/>
-      <c r="L96" s="216"/>
+      <c r="A96" s="227"/>
+      <c r="B96" s="227"/>
+      <c r="C96" s="227"/>
+      <c r="D96" s="227"/>
+      <c r="E96" s="227"/>
+      <c r="F96" s="227"/>
+      <c r="G96" s="227"/>
+      <c r="H96" s="227"/>
+      <c r="I96" s="227"/>
+      <c r="J96" s="227"/>
+      <c r="K96" s="227"/>
+      <c r="L96" s="227"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="90" t="s">
@@ -38816,48 +38716,48 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="216" t="s">
+      <c r="A98" s="227" t="s">
         <v>1051</v>
       </c>
-      <c r="B98" s="216"/>
-      <c r="C98" s="216"/>
-      <c r="D98" s="216"/>
-      <c r="E98" s="216"/>
-      <c r="F98" s="216"/>
-      <c r="G98" s="216"/>
-      <c r="H98" s="216"/>
-      <c r="I98" s="216"/>
-      <c r="J98" s="216"/>
-      <c r="K98" s="216"/>
-      <c r="L98" s="216"/>
+      <c r="B98" s="227"/>
+      <c r="C98" s="227"/>
+      <c r="D98" s="227"/>
+      <c r="E98" s="227"/>
+      <c r="F98" s="227"/>
+      <c r="G98" s="227"/>
+      <c r="H98" s="227"/>
+      <c r="I98" s="227"/>
+      <c r="J98" s="227"/>
+      <c r="K98" s="227"/>
+      <c r="L98" s="227"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="216"/>
-      <c r="B99" s="216"/>
-      <c r="C99" s="216"/>
-      <c r="D99" s="216"/>
-      <c r="E99" s="216"/>
-      <c r="F99" s="216"/>
-      <c r="G99" s="216"/>
-      <c r="H99" s="216"/>
-      <c r="I99" s="216"/>
-      <c r="J99" s="216"/>
-      <c r="K99" s="216"/>
-      <c r="L99" s="216"/>
+      <c r="A99" s="227"/>
+      <c r="B99" s="227"/>
+      <c r="C99" s="227"/>
+      <c r="D99" s="227"/>
+      <c r="E99" s="227"/>
+      <c r="F99" s="227"/>
+      <c r="G99" s="227"/>
+      <c r="H99" s="227"/>
+      <c r="I99" s="227"/>
+      <c r="J99" s="227"/>
+      <c r="K99" s="227"/>
+      <c r="L99" s="227"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="216"/>
-      <c r="B100" s="216"/>
-      <c r="C100" s="216"/>
-      <c r="D100" s="216"/>
-      <c r="E100" s="216"/>
-      <c r="F100" s="216"/>
-      <c r="G100" s="216"/>
-      <c r="H100" s="216"/>
-      <c r="I100" s="216"/>
-      <c r="J100" s="216"/>
-      <c r="K100" s="216"/>
-      <c r="L100" s="216"/>
+      <c r="A100" s="227"/>
+      <c r="B100" s="227"/>
+      <c r="C100" s="227"/>
+      <c r="D100" s="227"/>
+      <c r="E100" s="227"/>
+      <c r="F100" s="227"/>
+      <c r="G100" s="227"/>
+      <c r="H100" s="227"/>
+      <c r="I100" s="227"/>
+      <c r="J100" s="227"/>
+      <c r="K100" s="227"/>
+      <c r="L100" s="227"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
@@ -38879,48 +38779,32 @@
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="240" t="s">
+      <c r="A103" s="80" t="s">
         <v>407</v>
       </c>
-      <c r="B103" s="233"/>
-      <c r="C103" s="245">
+      <c r="C103" s="167">
         <v>1</v>
       </c>
-      <c r="D103" s="247" t="s">
+      <c r="D103" s="226" t="s">
         <v>1068</v>
       </c>
-      <c r="E103" s="240" t="s">
+      <c r="E103" s="80" t="s">
         <v>483</v>
       </c>
-      <c r="F103" s="233"/>
-      <c r="G103" s="233"/>
-      <c r="H103" s="233"/>
-      <c r="I103" s="233"/>
-      <c r="J103" s="233"/>
-      <c r="K103" s="234"/>
-      <c r="L103" s="233"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="240" t="s">
+      <c r="A104" s="80" t="s">
         <v>1067</v>
       </c>
-      <c r="B104" s="233"/>
-      <c r="C104" s="245" t="s">
+      <c r="C104" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="D104" s="247" t="s">
+      <c r="D104" s="226" t="s">
         <v>1071</v>
       </c>
-      <c r="E104" s="240" t="s">
+      <c r="E104" s="80" t="s">
         <v>1069</v>
       </c>
-      <c r="F104" s="233"/>
-      <c r="G104" s="233"/>
-      <c r="H104" s="233"/>
-      <c r="I104" s="233"/>
-      <c r="J104" s="233"/>
-      <c r="K104" s="234"/>
-      <c r="L104" s="233"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="61"/>
@@ -39716,7 +39600,7 @@
       <c r="B4" s="57" t="s">
         <v>1040</v>
       </c>
-      <c r="H4" s="230" t="s">
+      <c r="H4" s="217" t="s">
         <v>1111</v>
       </c>
     </row>
@@ -40867,7 +40751,7 @@
         <v>119</v>
       </c>
       <c r="F85" s="66"/>
-      <c r="G85" s="236" t="s">
+      <c r="G85" s="220" t="s">
         <v>1146</v>
       </c>
       <c r="I85" s="66"/>
@@ -40957,62 +40841,62 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="237" t="s">
+      <c r="A93" s="228" t="s">
         <v>1149</v>
       </c>
-      <c r="B93" s="237"/>
-      <c r="C93" s="237"/>
-      <c r="D93" s="237"/>
-      <c r="E93" s="237"/>
-      <c r="F93" s="237"/>
-      <c r="G93" s="237"/>
-      <c r="H93" s="237"/>
-      <c r="I93" s="237"/>
-      <c r="J93" s="237"/>
-      <c r="K93" s="237"/>
-      <c r="L93" s="237"/>
+      <c r="B93" s="228"/>
+      <c r="C93" s="228"/>
+      <c r="D93" s="228"/>
+      <c r="E93" s="228"/>
+      <c r="F93" s="228"/>
+      <c r="G93" s="228"/>
+      <c r="H93" s="228"/>
+      <c r="I93" s="228"/>
+      <c r="J93" s="228"/>
+      <c r="K93" s="228"/>
+      <c r="L93" s="228"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="237"/>
-      <c r="B94" s="237"/>
-      <c r="C94" s="237"/>
-      <c r="D94" s="237"/>
-      <c r="E94" s="237"/>
-      <c r="F94" s="237"/>
-      <c r="G94" s="237"/>
-      <c r="H94" s="237"/>
-      <c r="I94" s="237"/>
-      <c r="J94" s="237"/>
-      <c r="K94" s="237"/>
-      <c r="L94" s="237"/>
+      <c r="A94" s="228"/>
+      <c r="B94" s="228"/>
+      <c r="C94" s="228"/>
+      <c r="D94" s="228"/>
+      <c r="E94" s="228"/>
+      <c r="F94" s="228"/>
+      <c r="G94" s="228"/>
+      <c r="H94" s="228"/>
+      <c r="I94" s="228"/>
+      <c r="J94" s="228"/>
+      <c r="K94" s="228"/>
+      <c r="L94" s="228"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="237"/>
-      <c r="B95" s="237"/>
-      <c r="C95" s="237"/>
-      <c r="D95" s="237"/>
-      <c r="E95" s="237"/>
-      <c r="F95" s="237"/>
-      <c r="G95" s="237"/>
-      <c r="H95" s="237"/>
-      <c r="I95" s="237"/>
-      <c r="J95" s="237"/>
-      <c r="K95" s="237"/>
-      <c r="L95" s="237"/>
+      <c r="A95" s="228"/>
+      <c r="B95" s="228"/>
+      <c r="C95" s="228"/>
+      <c r="D95" s="228"/>
+      <c r="E95" s="228"/>
+      <c r="F95" s="228"/>
+      <c r="G95" s="228"/>
+      <c r="H95" s="228"/>
+      <c r="I95" s="228"/>
+      <c r="J95" s="228"/>
+      <c r="K95" s="228"/>
+      <c r="L95" s="228"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="237"/>
-      <c r="B96" s="237"/>
-      <c r="C96" s="237"/>
-      <c r="D96" s="237"/>
-      <c r="E96" s="237"/>
-      <c r="F96" s="237"/>
-      <c r="G96" s="237"/>
-      <c r="H96" s="237"/>
-      <c r="I96" s="237"/>
-      <c r="J96" s="237"/>
-      <c r="K96" s="237"/>
-      <c r="L96" s="237"/>
+      <c r="A96" s="228"/>
+      <c r="B96" s="228"/>
+      <c r="C96" s="228"/>
+      <c r="D96" s="228"/>
+      <c r="E96" s="228"/>
+      <c r="F96" s="228"/>
+      <c r="G96" s="228"/>
+      <c r="H96" s="228"/>
+      <c r="I96" s="228"/>
+      <c r="J96" s="228"/>
+      <c r="K96" s="228"/>
+      <c r="L96" s="228"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="90" t="s">
@@ -41020,48 +40904,48 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="216" t="s">
+      <c r="A98" s="227" t="s">
         <v>1150</v>
       </c>
-      <c r="B98" s="216"/>
-      <c r="C98" s="216"/>
-      <c r="D98" s="216"/>
-      <c r="E98" s="216"/>
-      <c r="F98" s="216"/>
-      <c r="G98" s="216"/>
-      <c r="H98" s="216"/>
-      <c r="I98" s="216"/>
-      <c r="J98" s="216"/>
-      <c r="K98" s="216"/>
-      <c r="L98" s="216"/>
+      <c r="B98" s="227"/>
+      <c r="C98" s="227"/>
+      <c r="D98" s="227"/>
+      <c r="E98" s="227"/>
+      <c r="F98" s="227"/>
+      <c r="G98" s="227"/>
+      <c r="H98" s="227"/>
+      <c r="I98" s="227"/>
+      <c r="J98" s="227"/>
+      <c r="K98" s="227"/>
+      <c r="L98" s="227"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="216"/>
-      <c r="B99" s="216"/>
-      <c r="C99" s="216"/>
-      <c r="D99" s="216"/>
-      <c r="E99" s="216"/>
-      <c r="F99" s="216"/>
-      <c r="G99" s="216"/>
-      <c r="H99" s="216"/>
-      <c r="I99" s="216"/>
-      <c r="J99" s="216"/>
-      <c r="K99" s="216"/>
-      <c r="L99" s="216"/>
+      <c r="A99" s="227"/>
+      <c r="B99" s="227"/>
+      <c r="C99" s="227"/>
+      <c r="D99" s="227"/>
+      <c r="E99" s="227"/>
+      <c r="F99" s="227"/>
+      <c r="G99" s="227"/>
+      <c r="H99" s="227"/>
+      <c r="I99" s="227"/>
+      <c r="J99" s="227"/>
+      <c r="K99" s="227"/>
+      <c r="L99" s="227"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="216"/>
-      <c r="B100" s="216"/>
-      <c r="C100" s="216"/>
-      <c r="D100" s="216"/>
-      <c r="E100" s="216"/>
-      <c r="F100" s="216"/>
-      <c r="G100" s="216"/>
-      <c r="H100" s="216"/>
-      <c r="I100" s="216"/>
-      <c r="J100" s="216"/>
-      <c r="K100" s="216"/>
-      <c r="L100" s="216"/>
+      <c r="A100" s="227"/>
+      <c r="B100" s="227"/>
+      <c r="C100" s="227"/>
+      <c r="D100" s="227"/>
+      <c r="E100" s="227"/>
+      <c r="F100" s="227"/>
+      <c r="G100" s="227"/>
+      <c r="H100" s="227"/>
+      <c r="I100" s="227"/>
+      <c r="J100" s="227"/>
+      <c r="K100" s="227"/>
+      <c r="L100" s="227"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F101" s="72" t="s">
@@ -41083,48 +40967,32 @@
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="240" t="s">
+      <c r="A103" s="80" t="s">
         <v>407</v>
       </c>
-      <c r="B103" s="233"/>
-      <c r="C103" s="245">
+      <c r="C103" s="167">
         <v>1</v>
       </c>
-      <c r="D103" s="247" t="s">
+      <c r="D103" s="226" t="s">
         <v>1068</v>
       </c>
-      <c r="E103" s="240" t="s">
+      <c r="E103" s="80" t="s">
         <v>483</v>
       </c>
-      <c r="F103" s="233"/>
-      <c r="G103" s="233"/>
-      <c r="H103" s="233"/>
-      <c r="I103" s="233"/>
-      <c r="J103" s="233"/>
-      <c r="K103" s="234"/>
-      <c r="L103" s="233"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="240" t="s">
+      <c r="A104" s="80" t="s">
         <v>1151</v>
       </c>
-      <c r="B104" s="233"/>
-      <c r="C104" s="245" t="s">
+      <c r="C104" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="D104" s="247" t="s">
+      <c r="D104" s="226" t="s">
         <v>1128</v>
       </c>
-      <c r="E104" s="246" t="s">
+      <c r="E104" s="221" t="s">
         <v>1152</v>
       </c>
-      <c r="F104" s="233"/>
-      <c r="G104" s="233"/>
-      <c r="H104" s="233"/>
-      <c r="I104" s="233"/>
-      <c r="J104" s="233"/>
-      <c r="K104" s="234"/>
-      <c r="L104" s="233"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="61"/>
@@ -41295,29 +41163,21 @@
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A125" s="232" t="s">
+      <c r="A125" s="63" t="s">
         <v>1129</v>
       </c>
-      <c r="B125" s="232"/>
+      <c r="B125" s="63"/>
       <c r="C125" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="D125" s="232" t="s">
+      <c r="D125" s="63" t="s">
         <v>1130</v>
       </c>
-      <c r="E125" s="233"/>
-      <c r="F125" s="233"/>
-      <c r="G125" s="233"/>
-      <c r="H125" s="233"/>
-      <c r="I125" s="233"/>
-      <c r="J125" s="233"/>
-      <c r="K125" s="234"/>
-      <c r="L125" s="233"/>
     </row>
     <row r="126" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="100"/>
       <c r="B126" s="100"/>
-      <c r="C126" s="231"/>
+      <c r="C126" s="218"/>
       <c r="D126" s="100"/>
       <c r="E126" s="61"/>
       <c r="F126" s="61"/>
@@ -43578,45 +43438,45 @@
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A141" s="217" t="s">
+      <c r="A141" s="229" t="s">
         <v>127</v>
       </c>
-      <c r="B141" s="217"/>
-      <c r="C141" s="217"/>
-      <c r="D141" s="217"/>
-      <c r="E141" s="217"/>
-      <c r="F141" s="217"/>
-      <c r="G141" s="217"/>
-      <c r="H141" s="217"/>
-      <c r="I141" s="217"/>
-      <c r="J141" s="217"/>
-      <c r="K141" s="217"/>
+      <c r="B141" s="229"/>
+      <c r="C141" s="229"/>
+      <c r="D141" s="229"/>
+      <c r="E141" s="229"/>
+      <c r="F141" s="229"/>
+      <c r="G141" s="229"/>
+      <c r="H141" s="229"/>
+      <c r="I141" s="229"/>
+      <c r="J141" s="229"/>
+      <c r="K141" s="229"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="217"/>
-      <c r="B142" s="217"/>
-      <c r="C142" s="217"/>
-      <c r="D142" s="217"/>
-      <c r="E142" s="217"/>
-      <c r="F142" s="217"/>
-      <c r="G142" s="217"/>
-      <c r="H142" s="217"/>
-      <c r="I142" s="217"/>
-      <c r="J142" s="217"/>
-      <c r="K142" s="217"/>
+      <c r="A142" s="229"/>
+      <c r="B142" s="229"/>
+      <c r="C142" s="229"/>
+      <c r="D142" s="229"/>
+      <c r="E142" s="229"/>
+      <c r="F142" s="229"/>
+      <c r="G142" s="229"/>
+      <c r="H142" s="229"/>
+      <c r="I142" s="229"/>
+      <c r="J142" s="229"/>
+      <c r="K142" s="229"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A143" s="217"/>
-      <c r="B143" s="217"/>
-      <c r="C143" s="217"/>
-      <c r="D143" s="217"/>
-      <c r="E143" s="217"/>
-      <c r="F143" s="217"/>
-      <c r="G143" s="217"/>
-      <c r="H143" s="217"/>
-      <c r="I143" s="217"/>
-      <c r="J143" s="217"/>
-      <c r="K143" s="217"/>
+      <c r="A143" s="229"/>
+      <c r="B143" s="229"/>
+      <c r="C143" s="229"/>
+      <c r="D143" s="229"/>
+      <c r="E143" s="229"/>
+      <c r="F143" s="229"/>
+      <c r="G143" s="229"/>
+      <c r="H143" s="229"/>
+      <c r="I143" s="229"/>
+      <c r="J143" s="229"/>
+      <c r="K143" s="229"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="90" t="s">
@@ -43624,45 +43484,45 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A146" s="217" t="s">
+      <c r="A146" s="229" t="s">
         <v>124</v>
       </c>
-      <c r="B146" s="217"/>
-      <c r="C146" s="217"/>
-      <c r="D146" s="217"/>
-      <c r="E146" s="217"/>
-      <c r="F146" s="217"/>
-      <c r="G146" s="217"/>
-      <c r="H146" s="217"/>
-      <c r="I146" s="217"/>
-      <c r="J146" s="217"/>
-      <c r="K146" s="217"/>
+      <c r="B146" s="229"/>
+      <c r="C146" s="229"/>
+      <c r="D146" s="229"/>
+      <c r="E146" s="229"/>
+      <c r="F146" s="229"/>
+      <c r="G146" s="229"/>
+      <c r="H146" s="229"/>
+      <c r="I146" s="229"/>
+      <c r="J146" s="229"/>
+      <c r="K146" s="229"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" s="217"/>
-      <c r="B147" s="217"/>
-      <c r="C147" s="217"/>
-      <c r="D147" s="217"/>
-      <c r="E147" s="217"/>
-      <c r="F147" s="217"/>
-      <c r="G147" s="217"/>
-      <c r="H147" s="217"/>
-      <c r="I147" s="217"/>
-      <c r="J147" s="217"/>
-      <c r="K147" s="217"/>
+      <c r="A147" s="229"/>
+      <c r="B147" s="229"/>
+      <c r="C147" s="229"/>
+      <c r="D147" s="229"/>
+      <c r="E147" s="229"/>
+      <c r="F147" s="229"/>
+      <c r="G147" s="229"/>
+      <c r="H147" s="229"/>
+      <c r="I147" s="229"/>
+      <c r="J147" s="229"/>
+      <c r="K147" s="229"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A148" s="217"/>
-      <c r="B148" s="217"/>
-      <c r="C148" s="217"/>
-      <c r="D148" s="217"/>
-      <c r="E148" s="217"/>
-      <c r="F148" s="217"/>
-      <c r="G148" s="217"/>
-      <c r="H148" s="217"/>
-      <c r="I148" s="217"/>
-      <c r="J148" s="217"/>
-      <c r="K148" s="217"/>
+      <c r="A148" s="229"/>
+      <c r="B148" s="229"/>
+      <c r="C148" s="229"/>
+      <c r="D148" s="229"/>
+      <c r="E148" s="229"/>
+      <c r="F148" s="229"/>
+      <c r="G148" s="229"/>
+      <c r="H148" s="229"/>
+      <c r="I148" s="229"/>
+      <c r="J148" s="229"/>
+      <c r="K148" s="229"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F149" s="72" t="s">
@@ -45775,45 +45635,45 @@
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A141" s="217" t="s">
+      <c r="A141" s="229" t="s">
         <v>127</v>
       </c>
-      <c r="B141" s="217"/>
-      <c r="C141" s="217"/>
-      <c r="D141" s="217"/>
-      <c r="E141" s="217"/>
-      <c r="F141" s="217"/>
-      <c r="G141" s="217"/>
-      <c r="H141" s="217"/>
-      <c r="I141" s="217"/>
-      <c r="J141" s="217"/>
-      <c r="K141" s="217"/>
+      <c r="B141" s="229"/>
+      <c r="C141" s="229"/>
+      <c r="D141" s="229"/>
+      <c r="E141" s="229"/>
+      <c r="F141" s="229"/>
+      <c r="G141" s="229"/>
+      <c r="H141" s="229"/>
+      <c r="I141" s="229"/>
+      <c r="J141" s="229"/>
+      <c r="K141" s="229"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="217"/>
-      <c r="B142" s="217"/>
-      <c r="C142" s="217"/>
-      <c r="D142" s="217"/>
-      <c r="E142" s="217"/>
-      <c r="F142" s="217"/>
-      <c r="G142" s="217"/>
-      <c r="H142" s="217"/>
-      <c r="I142" s="217"/>
-      <c r="J142" s="217"/>
-      <c r="K142" s="217"/>
+      <c r="A142" s="229"/>
+      <c r="B142" s="229"/>
+      <c r="C142" s="229"/>
+      <c r="D142" s="229"/>
+      <c r="E142" s="229"/>
+      <c r="F142" s="229"/>
+      <c r="G142" s="229"/>
+      <c r="H142" s="229"/>
+      <c r="I142" s="229"/>
+      <c r="J142" s="229"/>
+      <c r="K142" s="229"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A143" s="217"/>
-      <c r="B143" s="217"/>
-      <c r="C143" s="217"/>
-      <c r="D143" s="217"/>
-      <c r="E143" s="217"/>
-      <c r="F143" s="217"/>
-      <c r="G143" s="217"/>
-      <c r="H143" s="217"/>
-      <c r="I143" s="217"/>
-      <c r="J143" s="217"/>
-      <c r="K143" s="217"/>
+      <c r="A143" s="229"/>
+      <c r="B143" s="229"/>
+      <c r="C143" s="229"/>
+      <c r="D143" s="229"/>
+      <c r="E143" s="229"/>
+      <c r="F143" s="229"/>
+      <c r="G143" s="229"/>
+      <c r="H143" s="229"/>
+      <c r="I143" s="229"/>
+      <c r="J143" s="229"/>
+      <c r="K143" s="229"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="90" t="s">
@@ -45821,45 +45681,45 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A146" s="217" t="s">
+      <c r="A146" s="229" t="s">
         <v>124</v>
       </c>
-      <c r="B146" s="217"/>
-      <c r="C146" s="217"/>
-      <c r="D146" s="217"/>
-      <c r="E146" s="217"/>
-      <c r="F146" s="217"/>
-      <c r="G146" s="217"/>
-      <c r="H146" s="217"/>
-      <c r="I146" s="217"/>
-      <c r="J146" s="217"/>
-      <c r="K146" s="217"/>
+      <c r="B146" s="229"/>
+      <c r="C146" s="229"/>
+      <c r="D146" s="229"/>
+      <c r="E146" s="229"/>
+      <c r="F146" s="229"/>
+      <c r="G146" s="229"/>
+      <c r="H146" s="229"/>
+      <c r="I146" s="229"/>
+      <c r="J146" s="229"/>
+      <c r="K146" s="229"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" s="217"/>
-      <c r="B147" s="217"/>
-      <c r="C147" s="217"/>
-      <c r="D147" s="217"/>
-      <c r="E147" s="217"/>
-      <c r="F147" s="217"/>
-      <c r="G147" s="217"/>
-      <c r="H147" s="217"/>
-      <c r="I147" s="217"/>
-      <c r="J147" s="217"/>
-      <c r="K147" s="217"/>
+      <c r="A147" s="229"/>
+      <c r="B147" s="229"/>
+      <c r="C147" s="229"/>
+      <c r="D147" s="229"/>
+      <c r="E147" s="229"/>
+      <c r="F147" s="229"/>
+      <c r="G147" s="229"/>
+      <c r="H147" s="229"/>
+      <c r="I147" s="229"/>
+      <c r="J147" s="229"/>
+      <c r="K147" s="229"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A148" s="217"/>
-      <c r="B148" s="217"/>
-      <c r="C148" s="217"/>
-      <c r="D148" s="217"/>
-      <c r="E148" s="217"/>
-      <c r="F148" s="217"/>
-      <c r="G148" s="217"/>
-      <c r="H148" s="217"/>
-      <c r="I148" s="217"/>
-      <c r="J148" s="217"/>
-      <c r="K148" s="217"/>
+      <c r="A148" s="229"/>
+      <c r="B148" s="229"/>
+      <c r="C148" s="229"/>
+      <c r="D148" s="229"/>
+      <c r="E148" s="229"/>
+      <c r="F148" s="229"/>
+      <c r="G148" s="229"/>
+      <c r="H148" s="229"/>
+      <c r="I148" s="229"/>
+      <c r="J148" s="229"/>
+      <c r="K148" s="229"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F149" s="72" t="s">
@@ -46182,42 +46042,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="236" t="s">
         <v>994</v>
       </c>
-      <c r="B1" s="222"/>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="222"/>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="223">
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="237">
         <f>C7</f>
         <v>0.8125</v>
       </c>
-      <c r="K1" s="224"/>
-      <c r="L1" s="225">
+      <c r="K1" s="238"/>
+      <c r="L1" s="230">
         <f>C8</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M1" s="224"/>
-      <c r="N1" s="225">
+      <c r="M1" s="238"/>
+      <c r="N1" s="230">
         <f>C9</f>
         <v>0.85416666666666674</v>
       </c>
-      <c r="O1" s="224"/>
-      <c r="P1" s="225">
+      <c r="O1" s="238"/>
+      <c r="P1" s="230">
         <f>C10</f>
         <v>0.87500000000000011</v>
       </c>
-      <c r="Q1" s="224"/>
-      <c r="R1" s="225">
+      <c r="Q1" s="238"/>
+      <c r="R1" s="230">
         <f>C11</f>
         <v>0.89583333333333348</v>
       </c>
-      <c r="S1" s="226"/>
+      <c r="S1" s="231"/>
     </row>
     <row r="2" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="J2" s="196"/>
@@ -46297,31 +46157,31 @@
       <c r="F6" s="7" t="s">
         <v>993</v>
       </c>
-      <c r="J6" s="218">
+      <c r="J6" s="232">
         <f>C12</f>
         <v>0.91666666666666685</v>
       </c>
-      <c r="K6" s="219"/>
-      <c r="L6" s="220">
+      <c r="K6" s="233"/>
+      <c r="L6" s="234">
         <f>C13</f>
         <v>0.93750000000000022</v>
       </c>
-      <c r="M6" s="219"/>
-      <c r="N6" s="220">
+      <c r="M6" s="233"/>
+      <c r="N6" s="234">
         <f>C14</f>
         <v>0.95833333333333359</v>
       </c>
-      <c r="O6" s="219"/>
-      <c r="P6" s="220">
+      <c r="O6" s="233"/>
+      <c r="P6" s="234">
         <f>C15</f>
         <v>0.97916666666666696</v>
       </c>
-      <c r="Q6" s="219"/>
-      <c r="R6" s="220">
+      <c r="Q6" s="233"/>
+      <c r="R6" s="234">
         <f>C16</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S6" s="221"/>
+      <c r="S6" s="235"/>
     </row>
     <row r="7" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
@@ -46459,31 +46319,31 @@
       <c r="F11" s="7" t="s">
         <v>988</v>
       </c>
-      <c r="J11" s="218">
+      <c r="J11" s="232">
         <f>C17</f>
         <v>1.0208333333333335</v>
       </c>
-      <c r="K11" s="219"/>
-      <c r="L11" s="220">
+      <c r="K11" s="233"/>
+      <c r="L11" s="234">
         <f>C18</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="M11" s="219"/>
-      <c r="N11" s="220">
+      <c r="M11" s="233"/>
+      <c r="N11" s="234">
         <f>C19</f>
         <v>1.0625</v>
       </c>
-      <c r="O11" s="219"/>
-      <c r="P11" s="220">
+      <c r="O11" s="233"/>
+      <c r="P11" s="234">
         <f>C20</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="Q11" s="219"/>
-      <c r="R11" s="220">
+      <c r="Q11" s="233"/>
+      <c r="R11" s="234">
         <f>C21</f>
         <v>1.1041666666666665</v>
       </c>
-      <c r="S11" s="221"/>
+      <c r="S11" s="235"/>
     </row>
     <row r="12" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B12" s="193">
@@ -46613,31 +46473,31 @@
       <c r="E16" s="6" t="s">
         <v>978</v>
       </c>
-      <c r="J16" s="218">
+      <c r="J16" s="232">
         <f>C22</f>
         <v>1.1249999999999998</v>
       </c>
-      <c r="K16" s="219"/>
-      <c r="L16" s="220">
+      <c r="K16" s="233"/>
+      <c r="L16" s="234">
         <f>C23</f>
         <v>1.145833333333333</v>
       </c>
-      <c r="M16" s="219"/>
-      <c r="N16" s="220">
+      <c r="M16" s="233"/>
+      <c r="N16" s="234">
         <f>C24</f>
         <v>1.1666666666666663</v>
       </c>
-      <c r="O16" s="219"/>
-      <c r="P16" s="220">
+      <c r="O16" s="233"/>
+      <c r="P16" s="234">
         <f>C25</f>
         <v>1.1874999999999996</v>
       </c>
-      <c r="Q16" s="219"/>
-      <c r="R16" s="220">
+      <c r="Q16" s="233"/>
+      <c r="R16" s="234">
         <f>C26</f>
         <v>1.2083333333333328</v>
       </c>
-      <c r="S16" s="221"/>
+      <c r="S16" s="235"/>
     </row>
     <row r="17" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B17" s="193">
@@ -46773,31 +46633,31 @@
       <c r="F21" s="7" t="s">
         <v>990</v>
       </c>
-      <c r="J21" s="218">
+      <c r="J21" s="232">
         <f>C27</f>
         <v>1.2291666666666661</v>
       </c>
-      <c r="K21" s="219"/>
-      <c r="L21" s="220">
+      <c r="K21" s="233"/>
+      <c r="L21" s="234">
         <f>C28</f>
         <v>1.2499999999999993</v>
       </c>
-      <c r="M21" s="219"/>
-      <c r="N21" s="220">
+      <c r="M21" s="233"/>
+      <c r="N21" s="234">
         <f>C29</f>
         <v>1.2708333333333326</v>
       </c>
-      <c r="O21" s="219"/>
-      <c r="P21" s="220">
+      <c r="O21" s="233"/>
+      <c r="P21" s="234">
         <f>C30</f>
         <v>1.2916666666666659</v>
       </c>
-      <c r="Q21" s="219"/>
-      <c r="R21" s="220">
+      <c r="Q21" s="233"/>
+      <c r="R21" s="234">
         <f>C31</f>
         <v>1.3124999999999991</v>
       </c>
-      <c r="S21" s="221"/>
+      <c r="S21" s="235"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B22" s="193">
@@ -47032,18 +46892,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
@@ -47053,11 +46906,18 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -47129,31 +46989,31 @@
       <c r="C3" s="47"/>
       <c r="D3" s="44">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3" s="44">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K3" s="44">
         <f t="shared" ca="1" si="0"/>
@@ -47161,11 +47021,11 @@
       </c>
       <c r="L3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N3" s="44"/>
     </row>
@@ -47196,39 +47056,39 @@
       </c>
       <c r="E5" s="46">
         <f ca="1">IF(E$3&gt;=$B5,1,0)+D5+IF(E$3=1,-1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="46">
         <f t="shared" ref="F5:M5" ca="1" si="1">IF(F$3&gt;=$B5,1,0)+E5+IF(F$3=1,-1,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -47242,39 +47102,39 @@
       </c>
       <c r="E6" s="46">
         <f t="shared" ref="E6:M13" ca="1" si="3">IF(E$3&gt;=$B6,1,0)+D6+IF(E$3=1,-1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -47284,43 +47144,43 @@
       <c r="C7" s="47"/>
       <c r="D7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -47330,7 +47190,7 @@
       <c r="C8" s="47"/>
       <c r="D8" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47338,35 +47198,35 @@
       </c>
       <c r="F8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -47376,7 +47236,7 @@
       <c r="C9" s="47"/>
       <c r="D9" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47384,35 +47244,35 @@
       </c>
       <c r="F9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -47422,7 +47282,7 @@
       <c r="C10" s="47"/>
       <c r="D10" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47430,7 +47290,7 @@
       </c>
       <c r="F10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47438,27 +47298,27 @@
       </c>
       <c r="H10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -47468,7 +47328,7 @@
       <c r="C11" s="47"/>
       <c r="D11" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47476,7 +47336,7 @@
       </c>
       <c r="F11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47484,27 +47344,27 @@
       </c>
       <c r="H11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -47514,7 +47374,7 @@
       <c r="C12" s="47"/>
       <c r="D12" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47526,7 +47386,7 @@
       </c>
       <c r="G12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47550,7 +47410,7 @@
       </c>
       <c r="M12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -47560,7 +47420,7 @@
       <c r="C13" s="47"/>
       <c r="D13" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -47576,27 +47436,27 @@
       </c>
       <c r="H13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -47619,7 +47479,7 @@
       </c>
       <c r="G16" s="49" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -47635,7 +47495,7 @@
       <c r="F18" s="46"/>
       <c r="G18" s="50" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT(ADDRESS(E18+3,D18+3,1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -47648,7 +47508,7 @@
       <c r="F19" s="46"/>
       <c r="G19" s="50" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(E19+3,D19+3,1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -47661,7 +47521,7 @@
       <c r="F20" s="46"/>
       <c r="G20" s="50" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -47674,7 +47534,7 @@
       <c r="F21" s="46"/>
       <c r="G21" s="50" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(ADDRESS(E21+3,D21+3,1))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -47687,7 +47547,7 @@
       <c r="F22" s="46"/>
       <c r="G22" s="50" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT(ADDRESS(E22+3,D22+3,1))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -47700,7 +47560,7 @@
       <c r="F23" s="46"/>
       <c r="G23" s="50" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-11-26 23:53:51
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90850649-8AE9-4B55-A195-D60439221189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59888373-7DC4-47FB-BE52-0F33D6F78ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26904" yWindow="0" windowWidth="31584" windowHeight="16656" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3292" uniqueCount="1315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="1337">
   <si>
     <t>Nome</t>
   </si>
@@ -4075,6 +4075,74 @@
   </si>
   <si>
     <t>Decine di migliaia di euro disponibili.</t>
+  </si>
+  <si>
+    <t>Spiaggia libera, chioschi notturni, cerchi di respiro, fiere del benessere</t>
+  </si>
+  <si>
+    <t>Bicicletta vecchia, niente auto</t>
+  </si>
+  <si>
+    <t>offerte libere, serate al chiosco, vita essenziale</t>
+  </si>
+  <si>
+    <t>Monolocale spartano zona mare, Rimini — tappeto, pochi mobili, telefono nel cassetto</t>
+  </si>
+  <si>
+    <t>zona mare, Rimini</t>
+  </si>
+  <si>
+    <t>Neri corti</t>
+  </si>
+  <si>
+    <t>Marroni Caldi</t>
+  </si>
+  <si>
+    <t>Afroamericano/Latino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statunitense </t>
+  </si>
+  <si>
+    <t>1,88 Mt</t>
+  </si>
+  <si>
+    <t>92 Kg</t>
+  </si>
+  <si>
+    <t>I Malkavian sono irrimediabilmente folli. Il personaggio può acquisirne altri durante il gioco, ma quello iniziale è permanente.
+Disturbo d'ansia generalizzato o Attacchi di panico</t>
+  </si>
+  <si>
+    <t>Movimenti lenti, voce bassa, spalle aperte. Non occupa spazio — lo tiene libero per gli altri.
+Ascolta fino alla fine. Risponde dopo un respiro. Non alza mai la voce, neanche quando dice no.</t>
+  </si>
+  <si>
+    <t>Valerio Bernardi</t>
+  </si>
+  <si>
+    <t>Proprietario del Chiosco 72, 56 anni, vedovo. Ex pescatore. Valerio gli ha dato un panino e le chiavi del retro.</t>
+  </si>
+  <si>
+    <t>Amara Diallo</t>
+  </si>
+  <si>
+    <t>Mediatrice culturale, 42 anni, senegalese, vive a Rimini da 20 anni. Lavora con migranti, gente che arriva dal mare con niente.</t>
+  </si>
+  <si>
+    <t>Minore</t>
+  </si>
+  <si>
+    <t>Credito</t>
+  </si>
+  <si>
+    <t>Calmato durante una Frenesia imminente sul lungomare</t>
+  </si>
+  <si>
+    <t>Estete</t>
+  </si>
+  <si>
+    <t>Non Saldato</t>
   </si>
 </sst>
 </file>
@@ -4867,7 +4935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5561,6 +5629,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -23382,8 +23459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7F1D12-FD81-4CF0-ABD2-4533A3B56036}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -24508,19 +24585,25 @@
       <c r="A73" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="C73" s="63"/>
+      <c r="C73" s="63" t="s">
+        <v>1315</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="63"/>
+      <c r="C74" s="63" t="s">
+        <v>1316</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="63"/>
+      <c r="C75" s="63" t="s">
+        <v>1317</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="57" t="s">
@@ -24554,10 +24637,10 @@
       </c>
       <c r="B79" s="80"/>
       <c r="C79" s="80" t="s">
-        <v>1279</v>
+        <v>1319</v>
       </c>
       <c r="E79" s="57" t="s">
-        <v>1280</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -24603,13 +24686,13 @@
         <v>113</v>
       </c>
       <c r="C84" s="212">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E84" s="80" t="s">
         <v>118</v>
       </c>
       <c r="G84" s="212" t="s">
-        <v>1281</v>
+        <v>1322</v>
       </c>
       <c r="I84" s="57" t="s">
         <v>0</v>
@@ -24631,7 +24714,7 @@
       </c>
       <c r="F85" s="66"/>
       <c r="G85" s="211" t="s">
-        <v>392</v>
+        <v>1323</v>
       </c>
       <c r="I85" s="66"/>
       <c r="J85" s="66"/>
@@ -24643,13 +24726,13 @@
         <v>114</v>
       </c>
       <c r="C86" s="219">
-        <v>31120</v>
+        <v>30139</v>
       </c>
       <c r="E86" s="80" t="s">
         <v>120</v>
       </c>
       <c r="G86" s="212" t="s">
-        <v>1282</v>
+        <v>1324</v>
       </c>
       <c r="I86" s="85"/>
       <c r="J86" s="85"/>
@@ -24669,7 +24752,7 @@
       </c>
       <c r="F87" s="66"/>
       <c r="G87" s="211" t="s">
-        <v>1196</v>
+        <v>1325</v>
       </c>
       <c r="I87" s="66"/>
       <c r="J87" s="66"/>
@@ -24681,13 +24764,13 @@
         <v>116</v>
       </c>
       <c r="C88" s="212" t="s">
-        <v>390</v>
+        <v>1320</v>
       </c>
       <c r="E88" s="80" t="s">
         <v>122</v>
       </c>
       <c r="G88" s="212" t="s">
-        <v>1197</v>
+        <v>394</v>
       </c>
       <c r="K88" s="57"/>
       <c r="L88" s="54"/>
@@ -24698,7 +24781,7 @@
       </c>
       <c r="B89" s="66"/>
       <c r="C89" s="211" t="s">
-        <v>1283</v>
+        <v>1321</v>
       </c>
       <c r="E89" s="80"/>
       <c r="F89" s="66"/>
@@ -24721,7 +24804,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="227" t="s">
-        <v>1273</v>
+        <v>1326</v>
       </c>
       <c r="B93" s="227"/>
       <c r="C93" s="227"/>
@@ -24784,7 +24867,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="227" t="s">
-        <v>1274</v>
+        <v>1327</v>
       </c>
       <c r="B98" s="227"/>
       <c r="C98" s="227"/>
@@ -24860,11 +24943,19 @@
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="81"/>
+      <c r="A104" s="81" t="s">
+        <v>1328</v>
+      </c>
       <c r="B104" s="61"/>
-      <c r="C104" s="241"/>
-      <c r="D104" s="242"/>
-      <c r="E104" s="81"/>
+      <c r="C104" s="241" t="s">
+        <v>131</v>
+      </c>
+      <c r="D104" s="242" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E104" s="81" t="s">
+        <v>1329</v>
+      </c>
       <c r="F104" s="61"/>
       <c r="G104" s="61"/>
       <c r="H104" s="61"/>
@@ -24874,11 +24965,19 @@
       <c r="L104" s="61"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A105" s="61"/>
+      <c r="A105" s="81" t="s">
+        <v>1330</v>
+      </c>
       <c r="B105" s="61"/>
-      <c r="C105" s="61"/>
-      <c r="D105" s="133"/>
-      <c r="E105" s="100"/>
+      <c r="C105" s="241" t="s">
+        <v>131</v>
+      </c>
+      <c r="D105" s="242" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E105" s="249" t="s">
+        <v>1331</v>
+      </c>
       <c r="F105" s="61"/>
       <c r="G105" s="61"/>
       <c r="H105" s="61"/>
@@ -24936,93 +25035,170 @@
       </c>
       <c r="D111" s="80"/>
       <c r="E111" s="80"/>
-      <c r="F111" s="80" t="s">
+      <c r="H111" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="G111" s="80" t="s">
+      <c r="J111" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="H111" s="80" t="s">
+      <c r="K111" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="I111" s="80" t="s">
+      <c r="L111" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="J111" s="80" t="s">
-        <v>87</v>
-      </c>
-      <c r="K111" s="75"/>
-      <c r="L111" s="80"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A112" s="245" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B112" s="245" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C112" s="245" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D112" s="245"/>
+      <c r="E112" s="245"/>
+      <c r="F112" s="244"/>
+      <c r="G112" s="244"/>
+      <c r="H112" s="250"/>
+      <c r="I112" s="81"/>
+      <c r="J112" s="251" t="s">
+        <v>421</v>
+      </c>
+      <c r="K112" s="251" t="s">
+        <v>1335</v>
+      </c>
+      <c r="L112" s="251" t="s">
+        <v>1336</v>
+      </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A113" s="66"/>
-      <c r="B113" s="66"/>
-      <c r="C113" s="66"/>
-      <c r="D113" s="66"/>
-      <c r="E113" s="66"/>
-      <c r="F113" s="66"/>
-      <c r="G113" s="66"/>
-      <c r="H113" s="66"/>
-      <c r="I113" s="66"/>
-      <c r="J113" s="66"/>
-      <c r="K113" s="69"/>
-      <c r="L113" s="66"/>
+      <c r="A113" s="81"/>
+      <c r="B113" s="81"/>
+      <c r="C113" s="81"/>
+      <c r="D113" s="81"/>
+      <c r="E113" s="81"/>
+      <c r="F113" s="81"/>
+      <c r="G113" s="81"/>
+      <c r="H113" s="81"/>
+      <c r="I113" s="81"/>
+      <c r="J113" s="81"/>
+      <c r="K113" s="145"/>
+      <c r="L113" s="81"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A114" s="80"/>
+      <c r="B114" s="80"/>
+      <c r="C114" s="80"/>
+      <c r="D114" s="80"/>
+      <c r="E114" s="80"/>
+      <c r="F114" s="80"/>
+      <c r="G114" s="80"/>
+      <c r="H114" s="80"/>
+      <c r="I114" s="80"/>
+      <c r="J114" s="80"/>
+      <c r="K114" s="75"/>
+      <c r="L114" s="80"/>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A115" s="66"/>
-      <c r="B115" s="66"/>
-      <c r="C115" s="66"/>
-      <c r="D115" s="66"/>
-      <c r="E115" s="66"/>
-      <c r="F115" s="66"/>
-      <c r="G115" s="66"/>
-      <c r="H115" s="66"/>
-      <c r="I115" s="66"/>
-      <c r="J115" s="66"/>
-      <c r="K115" s="69"/>
-      <c r="L115" s="66"/>
+      <c r="A115" s="82"/>
+      <c r="B115" s="82"/>
+      <c r="C115" s="82"/>
+      <c r="D115" s="82"/>
+      <c r="E115" s="82"/>
+      <c r="F115" s="82"/>
+      <c r="G115" s="82"/>
+      <c r="H115" s="82"/>
+      <c r="I115" s="82"/>
+      <c r="J115" s="82"/>
+      <c r="K115" s="147"/>
+      <c r="L115" s="82"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A116" s="80"/>
+      <c r="B116" s="80"/>
+      <c r="C116" s="80"/>
+      <c r="D116" s="80"/>
+      <c r="E116" s="80"/>
+      <c r="F116" s="80"/>
+      <c r="G116" s="80"/>
+      <c r="H116" s="80"/>
+      <c r="I116" s="80"/>
+      <c r="J116" s="80"/>
+      <c r="K116" s="75"/>
+      <c r="L116" s="80"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A117" s="66"/>
-      <c r="B117" s="66"/>
-      <c r="C117" s="66"/>
-      <c r="D117" s="66"/>
-      <c r="E117" s="66"/>
-      <c r="F117" s="66"/>
-      <c r="G117" s="66"/>
-      <c r="H117" s="66"/>
-      <c r="I117" s="66"/>
-      <c r="J117" s="66"/>
-      <c r="K117" s="69"/>
-      <c r="L117" s="66"/>
+      <c r="A117" s="82"/>
+      <c r="B117" s="82"/>
+      <c r="C117" s="82"/>
+      <c r="D117" s="82"/>
+      <c r="E117" s="82"/>
+      <c r="F117" s="82"/>
+      <c r="G117" s="82"/>
+      <c r="H117" s="82"/>
+      <c r="I117" s="82"/>
+      <c r="J117" s="82"/>
+      <c r="K117" s="147"/>
+      <c r="L117" s="82"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A118" s="80"/>
+      <c r="B118" s="80"/>
+      <c r="C118" s="80"/>
+      <c r="D118" s="80"/>
+      <c r="E118" s="80"/>
+      <c r="F118" s="80"/>
+      <c r="G118" s="80"/>
+      <c r="H118" s="80"/>
+      <c r="I118" s="80"/>
+      <c r="J118" s="80"/>
+      <c r="K118" s="75"/>
+      <c r="L118" s="80"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A119" s="66"/>
-      <c r="B119" s="66"/>
-      <c r="C119" s="66"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="66"/>
-      <c r="G119" s="66"/>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="66"/>
-      <c r="K119" s="69"/>
-      <c r="L119" s="66"/>
+      <c r="A119" s="82"/>
+      <c r="B119" s="82"/>
+      <c r="C119" s="82"/>
+      <c r="D119" s="82"/>
+      <c r="E119" s="82"/>
+      <c r="F119" s="82"/>
+      <c r="G119" s="82"/>
+      <c r="H119" s="82"/>
+      <c r="I119" s="82"/>
+      <c r="J119" s="82"/>
+      <c r="K119" s="147"/>
+      <c r="L119" s="82"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A120" s="80"/>
+      <c r="B120" s="80"/>
+      <c r="C120" s="80"/>
+      <c r="D120" s="80"/>
+      <c r="E120" s="80"/>
+      <c r="F120" s="80"/>
+      <c r="G120" s="80"/>
+      <c r="H120" s="80"/>
+      <c r="I120" s="80"/>
+      <c r="J120" s="80"/>
+      <c r="K120" s="75"/>
+      <c r="L120" s="80"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A121" s="66"/>
-      <c r="B121" s="66"/>
-      <c r="C121" s="66"/>
-      <c r="D121" s="66"/>
-      <c r="E121" s="66"/>
-      <c r="F121" s="66"/>
-      <c r="G121" s="66"/>
-      <c r="H121" s="66"/>
-      <c r="I121" s="66"/>
-      <c r="J121" s="66"/>
-      <c r="K121" s="69"/>
-      <c r="L121" s="66"/>
+      <c r="A121" s="82"/>
+      <c r="B121" s="82"/>
+      <c r="C121" s="82"/>
+      <c r="D121" s="82"/>
+      <c r="E121" s="82"/>
+      <c r="F121" s="82"/>
+      <c r="G121" s="82"/>
+      <c r="H121" s="82"/>
+      <c r="I121" s="82"/>
+      <c r="J121" s="82"/>
+      <c r="K121" s="147"/>
+      <c r="L121" s="82"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F123" s="72" t="s">
@@ -25667,35 +25843,35 @@
       <c r="C3" s="47"/>
       <c r="D3" s="44">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E3" s="44">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L3" s="44">
         <f t="shared" ca="1" si="0"/>
@@ -25703,7 +25879,7 @@
       </c>
       <c r="M3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N3" s="44"/>
     </row>
@@ -25792,27 +25968,27 @@
       </c>
       <c r="H6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -25846,19 +26022,19 @@
       </c>
       <c r="J7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -25868,43 +26044,43 @@
       <c r="C8" s="47"/>
       <c r="D8" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -25914,43 +26090,43 @@
       <c r="C9" s="47"/>
       <c r="D9" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -25960,43 +26136,43 @@
       <c r="C10" s="47"/>
       <c r="D10" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -26006,43 +26182,43 @@
       <c r="C11" s="47"/>
       <c r="D11" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -26052,43 +26228,43 @@
       <c r="C12" s="47"/>
       <c r="D12" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -26098,43 +26274,43 @@
       <c r="C13" s="47"/>
       <c r="D13" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -26157,7 +26333,7 @@
       </c>
       <c r="G16" s="49" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -26173,7 +26349,7 @@
       <c r="F18" s="46"/>
       <c r="G18" s="50" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT(ADDRESS(E18+3,D18+3,1))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -26186,7 +26362,7 @@
       <c r="F19" s="46"/>
       <c r="G19" s="50" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(E19+3,D19+3,1))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -26199,7 +26375,7 @@
       <c r="F20" s="46"/>
       <c r="G20" s="50" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -26212,7 +26388,7 @@
       <c r="F21" s="46"/>
       <c r="G21" s="50" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(ADDRESS(E21+3,D21+3,1))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -26225,7 +26401,7 @@
       <c r="F22" s="46"/>
       <c r="G22" s="50" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT(ADDRESS(E22+3,D22+3,1))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -26238,7 +26414,7 @@
       <c r="F23" s="46"/>
       <c r="G23" s="50" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-11-27 01:45:24
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59888373-7DC4-47FB-BE52-0F33D6F78ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502F059F-0AC0-485A-A3BC-DA4369173383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26904" yWindow="0" windowWidth="31584" windowHeight="16656" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
+    <workbookView xWindow="28056" yWindow="0" windowWidth="31584" windowHeight="16656" activeTab="1" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
   <sheets>
     <sheet name="_Malkavian" sheetId="19" r:id="rId1"/>
@@ -23459,8 +23459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7F1D12-FD81-4CF0-ABD2-4533A3B56036}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I117" sqref="I117"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -25843,7 +25843,7 @@
       <c r="C3" s="47"/>
       <c r="D3" s="44">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3" s="44">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
@@ -25851,35 +25851,35 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N3" s="44"/>
     </row>
@@ -25938,11 +25938,11 @@
       </c>
       <c r="L5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M5" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -25984,11 +25984,11 @@
       </c>
       <c r="L6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M6" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -25998,19 +25998,19 @@
       <c r="C7" s="47"/>
       <c r="D7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26030,11 +26030,11 @@
       </c>
       <c r="L7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -26044,15 +26044,15 @@
       <c r="C8" s="47"/>
       <c r="D8" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26060,7 +26060,7 @@
       </c>
       <c r="H8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I8" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26068,11 +26068,11 @@
       </c>
       <c r="J8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K8" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L8" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26090,15 +26090,15 @@
       <c r="C9" s="47"/>
       <c r="D9" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26106,11 +26106,11 @@
       </c>
       <c r="H9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26122,7 +26122,7 @@
       </c>
       <c r="L9" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M9" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26136,15 +26136,15 @@
       <c r="C10" s="47"/>
       <c r="D10" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26152,11 +26152,11 @@
       </c>
       <c r="H10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26164,7 +26164,7 @@
       </c>
       <c r="K10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L10" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26172,7 +26172,7 @@
       </c>
       <c r="M10" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -26182,15 +26182,15 @@
       <c r="C11" s="47"/>
       <c r="D11" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26198,15 +26198,15 @@
       </c>
       <c r="H11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26214,11 +26214,11 @@
       </c>
       <c r="L11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -26228,15 +26228,15 @@
       <c r="C12" s="47"/>
       <c r="D12" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26256,7 +26256,7 @@
       </c>
       <c r="K12" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26274,11 +26274,11 @@
       <c r="C13" s="47"/>
       <c r="D13" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26302,7 +26302,7 @@
       </c>
       <c r="K13" s="46">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" s="46">
         <f t="shared" ca="1" si="3"/>
@@ -26333,7 +26333,7 @@
       </c>
       <c r="G16" s="49" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -26362,7 +26362,7 @@
       <c r="F19" s="46"/>
       <c r="G19" s="50" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(E19+3,D19+3,1))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -26375,7 +26375,7 @@
       <c r="F20" s="46"/>
       <c r="G20" s="50" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -26414,7 +26414,7 @@
       <c r="F23" s="46"/>
       <c r="G23" s="50" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -34881,8 +34881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F8F40E-FA57-4F3C-B9C3-6981E5263578}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -37075,8 +37075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5334263-4143-413C-81B1-B37F8CC6DF82}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -39283,8 +39283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AF1615-1EA2-4AD7-A86C-59952E5A099E}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A78" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -41490,8 +41490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB020AF3-E2AF-4B08-9CF1-A8BB16CCBDFC}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103:D104"/>
+    <sheetView topLeftCell="A78" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -43693,8 +43693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618731C0-8D69-42F5-B683-631FA94DA355}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103:D104"/>
+    <sheetView topLeftCell="A78" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>